<commit_message>
Start mammals risk score script - calc F and D
</commit_message>
<xml_diff>
--- a/Mammal matrix.xlsx
+++ b/Mammal matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713DFA67-7652-4340-9D40-8EF1AB59D8F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA49EDBE-D048-834F-B084-CDA20F58E389}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -543,10 +543,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -555,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -590,6 +599,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -930,8 +946,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AE11" sqref="AE11"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD13" sqref="AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -943,22 +960,27 @@
     <col min="5" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="19" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" style="19" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5" style="19" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="29" width="7.6640625" customWidth="1"/>
-    <col min="30" max="31" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="37" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="7.6640625" customWidth="1"/>
+    <col min="29" max="29" width="7.6640625" style="19" customWidth="1"/>
+    <col min="30" max="30" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
@@ -1041,7 +1063,7 @@
       <c r="AB2" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AC2" s="23" t="s">
         <v>129</v>
       </c>
       <c r="AD2" s="14" t="s">
@@ -1086,7 +1108,7 @@
       <c r="H3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="18" t="s">
         <v>95</v>
       </c>
       <c r="J3" s="9" t="s">
@@ -1101,7 +1123,7 @@
       <c r="M3" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="20" t="s">
         <v>101</v>
       </c>
       <c r="O3" s="7" t="s">
@@ -1116,7 +1138,7 @@
       <c r="R3" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="18" t="s">
         <v>107</v>
       </c>
       <c r="T3" s="9" t="s">
@@ -1134,7 +1156,7 @@
       <c r="X3" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="Y3" s="20" t="s">
         <v>110</v>
       </c>
       <c r="Z3" s="11" t="s">
@@ -1146,25 +1168,25 @@
       <c r="AB3" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="AC3" s="12" t="s">
+      <c r="AC3" s="23" t="s">
         <v>125</v>
       </c>
       <c r="AD3" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="AE3" s="15" t="s">
+      <c r="AE3" s="21" t="s">
         <v>115</v>
       </c>
       <c r="AF3" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="AG3" s="17" t="s">
+      <c r="AG3" s="22" t="s">
         <v>117</v>
       </c>
       <c r="AH3" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="AI3" s="15" t="s">
+      <c r="AI3" s="21" t="s">
         <v>119</v>
       </c>
       <c r="AJ3" s="17" t="s">
@@ -1200,7 +1222,7 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="19">
         <v>1</v>
       </c>
       <c r="J4">
@@ -1215,7 +1237,7 @@
       <c r="M4">
         <v>1</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="19">
         <v>1</v>
       </c>
       <c r="O4">
@@ -1230,7 +1252,7 @@
       <c r="R4">
         <v>1</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="19">
         <v>1</v>
       </c>
       <c r="T4">
@@ -1248,7 +1270,7 @@
       <c r="X4">
         <v>0</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="19">
         <v>0</v>
       </c>
       <c r="Z4" s="1">
@@ -1260,25 +1282,25 @@
       <c r="AB4" s="1">
         <v>1</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AC4" s="24">
         <v>0</v>
       </c>
       <c r="AD4">
         <v>0</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="19">
         <v>1</v>
       </c>
       <c r="AF4">
         <v>0</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="19">
         <v>1</v>
       </c>
       <c r="AH4">
         <v>0</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="19">
         <v>1</v>
       </c>
       <c r="AJ4">
@@ -1314,7 +1336,7 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="19">
         <v>0</v>
       </c>
       <c r="J5">
@@ -1329,7 +1351,7 @@
       <c r="M5">
         <v>1</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="19">
         <v>0</v>
       </c>
       <c r="O5">
@@ -1344,7 +1366,7 @@
       <c r="R5">
         <v>1</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="19">
         <v>0</v>
       </c>
       <c r="T5">
@@ -1362,7 +1384,7 @@
       <c r="X5">
         <v>0</v>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="19">
         <v>0</v>
       </c>
       <c r="Z5" s="1">
@@ -1374,25 +1396,25 @@
       <c r="AB5" s="1">
         <v>1</v>
       </c>
-      <c r="AC5" s="1">
+      <c r="AC5" s="24">
         <v>0</v>
       </c>
       <c r="AD5">
         <v>0</v>
       </c>
-      <c r="AE5">
+      <c r="AE5" s="19">
         <v>0</v>
       </c>
       <c r="AF5">
         <v>0</v>
       </c>
-      <c r="AG5">
+      <c r="AG5" s="19">
         <v>1</v>
       </c>
       <c r="AH5">
         <v>0</v>
       </c>
-      <c r="AI5">
+      <c r="AI5" s="19">
         <v>1</v>
       </c>
       <c r="AJ5">
@@ -1428,7 +1450,7 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="19">
         <v>0</v>
       </c>
       <c r="J6">
@@ -1443,7 +1465,7 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="19">
         <v>0</v>
       </c>
       <c r="O6">
@@ -1458,7 +1480,7 @@
       <c r="R6">
         <v>0</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="19">
         <v>0</v>
       </c>
       <c r="T6">
@@ -1476,7 +1498,7 @@
       <c r="X6">
         <v>0</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="19">
         <v>0</v>
       </c>
       <c r="Z6" s="1">
@@ -1488,25 +1510,25 @@
       <c r="AB6" s="1">
         <v>1</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AC6" s="24">
         <v>1</v>
       </c>
       <c r="AD6">
         <v>0</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="19">
         <v>0</v>
       </c>
       <c r="AF6">
         <v>0</v>
       </c>
-      <c r="AG6">
+      <c r="AG6" s="19">
         <v>0</v>
       </c>
       <c r="AH6">
         <v>1</v>
       </c>
-      <c r="AI6">
+      <c r="AI6" s="19">
         <v>0</v>
       </c>
       <c r="AJ6">
@@ -1542,7 +1564,7 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="19">
         <v>0</v>
       </c>
       <c r="J7">
@@ -1557,7 +1579,7 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="19">
         <v>0</v>
       </c>
       <c r="O7">
@@ -1572,7 +1594,7 @@
       <c r="R7">
         <v>0</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="19">
         <v>0</v>
       </c>
       <c r="T7">
@@ -1590,7 +1612,7 @@
       <c r="X7">
         <v>0</v>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="19">
         <v>0</v>
       </c>
       <c r="Z7" s="1">
@@ -1602,25 +1624,25 @@
       <c r="AB7" s="1">
         <v>1</v>
       </c>
-      <c r="AC7" s="1">
+      <c r="AC7" s="24">
         <v>1</v>
       </c>
       <c r="AD7">
         <v>0</v>
       </c>
-      <c r="AE7">
+      <c r="AE7" s="19">
         <v>0</v>
       </c>
       <c r="AF7">
         <v>0</v>
       </c>
-      <c r="AG7">
+      <c r="AG7" s="19">
         <v>0</v>
       </c>
       <c r="AH7">
         <v>1</v>
       </c>
-      <c r="AI7">
+      <c r="AI7" s="19">
         <v>0</v>
       </c>
       <c r="AJ7">
@@ -1656,7 +1678,7 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="19">
         <v>0</v>
       </c>
       <c r="J8">
@@ -1671,7 +1693,7 @@
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="19">
         <v>0</v>
       </c>
       <c r="O8">
@@ -1686,7 +1708,7 @@
       <c r="R8">
         <v>0</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="19">
         <v>0</v>
       </c>
       <c r="T8">
@@ -1704,7 +1726,7 @@
       <c r="X8">
         <v>0</v>
       </c>
-      <c r="Y8">
+      <c r="Y8" s="19">
         <v>0</v>
       </c>
       <c r="Z8" s="1">
@@ -1716,25 +1738,25 @@
       <c r="AB8" s="1">
         <v>1</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AC8" s="24">
         <v>1</v>
       </c>
       <c r="AD8">
         <v>0</v>
       </c>
-      <c r="AE8">
+      <c r="AE8" s="19">
         <v>0</v>
       </c>
       <c r="AF8">
         <v>0</v>
       </c>
-      <c r="AG8">
+      <c r="AG8" s="19">
         <v>0</v>
       </c>
       <c r="AH8">
         <v>1</v>
       </c>
-      <c r="AI8">
+      <c r="AI8" s="19">
         <v>0</v>
       </c>
       <c r="AJ8">
@@ -1770,7 +1792,7 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="19">
         <v>0</v>
       </c>
       <c r="J9">
@@ -1785,7 +1807,7 @@
       <c r="M9">
         <v>1</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="19">
         <v>0</v>
       </c>
       <c r="O9">
@@ -1800,7 +1822,7 @@
       <c r="R9">
         <v>1</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="19">
         <v>0</v>
       </c>
       <c r="T9">
@@ -1818,7 +1840,7 @@
       <c r="X9">
         <v>0</v>
       </c>
-      <c r="Y9">
+      <c r="Y9" s="19">
         <v>0</v>
       </c>
       <c r="Z9" s="1">
@@ -1830,25 +1852,25 @@
       <c r="AB9" s="1">
         <v>1</v>
       </c>
-      <c r="AC9" s="1">
+      <c r="AC9" s="24">
         <v>0</v>
       </c>
       <c r="AD9">
         <v>1</v>
       </c>
-      <c r="AE9">
+      <c r="AE9" s="19">
         <v>0</v>
       </c>
       <c r="AF9">
         <v>1</v>
       </c>
-      <c r="AG9">
+      <c r="AG9" s="19">
         <v>0</v>
       </c>
       <c r="AH9">
         <v>1</v>
       </c>
-      <c r="AI9">
+      <c r="AI9" s="19">
         <v>0</v>
       </c>
       <c r="AJ9">
@@ -1884,7 +1906,7 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="19">
         <v>0</v>
       </c>
       <c r="J10">
@@ -1899,7 +1921,7 @@
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="19">
         <v>0</v>
       </c>
       <c r="O10">
@@ -1914,7 +1936,7 @@
       <c r="R10">
         <v>0</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="19">
         <v>0</v>
       </c>
       <c r="T10">
@@ -1932,7 +1954,7 @@
       <c r="X10">
         <v>0</v>
       </c>
-      <c r="Y10">
+      <c r="Y10" s="19">
         <v>0</v>
       </c>
       <c r="Z10" s="1">
@@ -1944,25 +1966,25 @@
       <c r="AB10" s="1">
         <v>1</v>
       </c>
-      <c r="AC10" s="1">
+      <c r="AC10" s="24">
         <v>1</v>
       </c>
       <c r="AD10">
         <v>0</v>
       </c>
-      <c r="AE10">
+      <c r="AE10" s="19">
         <v>0</v>
       </c>
       <c r="AF10">
         <v>0</v>
       </c>
-      <c r="AG10">
+      <c r="AG10" s="19">
         <v>0</v>
       </c>
       <c r="AH10">
         <v>1</v>
       </c>
-      <c r="AI10">
+      <c r="AI10" s="19">
         <v>0</v>
       </c>
       <c r="AJ10">
@@ -1998,7 +2020,7 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="19">
         <v>1</v>
       </c>
       <c r="J11">
@@ -2013,7 +2035,7 @@
       <c r="M11">
         <v>1</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="19">
         <v>1</v>
       </c>
       <c r="O11">
@@ -2028,7 +2050,7 @@
       <c r="R11">
         <v>1</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="19">
         <v>1</v>
       </c>
       <c r="T11">
@@ -2046,7 +2068,7 @@
       <c r="X11">
         <v>1</v>
       </c>
-      <c r="Y11">
+      <c r="Y11" s="19">
         <v>0</v>
       </c>
       <c r="Z11" s="1">
@@ -2058,25 +2080,25 @@
       <c r="AB11" s="1">
         <v>1</v>
       </c>
-      <c r="AC11" s="1">
+      <c r="AC11" s="24">
         <v>1</v>
       </c>
       <c r="AD11">
         <v>1</v>
       </c>
-      <c r="AE11">
+      <c r="AE11" s="19">
         <v>1</v>
       </c>
       <c r="AF11">
         <v>1</v>
       </c>
-      <c r="AG11">
+      <c r="AG11" s="19">
         <v>1</v>
       </c>
       <c r="AH11">
         <v>1</v>
       </c>
-      <c r="AI11">
+      <c r="AI11" s="19">
         <v>1</v>
       </c>
       <c r="AJ11">
@@ -2112,7 +2134,7 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="19">
         <v>0</v>
       </c>
       <c r="J12">
@@ -2127,7 +2149,7 @@
       <c r="M12">
         <v>1</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="19">
         <v>0</v>
       </c>
       <c r="O12">
@@ -2142,7 +2164,7 @@
       <c r="R12">
         <v>1</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="19">
         <v>0</v>
       </c>
       <c r="T12">
@@ -2160,7 +2182,7 @@
       <c r="X12">
         <v>0</v>
       </c>
-      <c r="Y12">
+      <c r="Y12" s="19">
         <v>0</v>
       </c>
       <c r="Z12" s="1">
@@ -2172,25 +2194,25 @@
       <c r="AB12" s="1">
         <v>1</v>
       </c>
-      <c r="AC12" s="1">
+      <c r="AC12" s="24">
         <v>1</v>
       </c>
       <c r="AD12">
         <v>0</v>
       </c>
-      <c r="AE12">
+      <c r="AE12" s="19">
         <v>0</v>
       </c>
       <c r="AF12">
         <v>0</v>
       </c>
-      <c r="AG12">
+      <c r="AG12" s="19">
         <v>0</v>
       </c>
       <c r="AH12">
         <v>1</v>
       </c>
-      <c r="AI12">
+      <c r="AI12" s="19">
         <v>0</v>
       </c>
       <c r="AJ12">
@@ -2226,7 +2248,7 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="19">
         <v>0</v>
       </c>
       <c r="J13">
@@ -2241,7 +2263,7 @@
       <c r="M13">
         <v>0</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="19">
         <v>0</v>
       </c>
       <c r="O13">
@@ -2256,7 +2278,7 @@
       <c r="R13">
         <v>1</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="19">
         <v>0</v>
       </c>
       <c r="T13">
@@ -2274,7 +2296,7 @@
       <c r="X13">
         <v>0</v>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="19">
         <v>0</v>
       </c>
       <c r="Z13" s="1">
@@ -2286,25 +2308,25 @@
       <c r="AB13" s="1">
         <v>1</v>
       </c>
-      <c r="AC13" s="1">
+      <c r="AC13" s="24">
         <v>0</v>
       </c>
       <c r="AD13">
         <v>0</v>
       </c>
-      <c r="AE13">
+      <c r="AE13" s="19">
         <v>0</v>
       </c>
       <c r="AF13">
         <v>0</v>
       </c>
-      <c r="AG13">
+      <c r="AG13" s="19">
         <v>0</v>
       </c>
       <c r="AH13">
         <v>1</v>
       </c>
-      <c r="AI13">
+      <c r="AI13" s="19">
         <v>1</v>
       </c>
       <c r="AJ13">
@@ -2340,7 +2362,7 @@
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="19">
         <v>0</v>
       </c>
       <c r="J14">
@@ -2355,7 +2377,7 @@
       <c r="M14">
         <v>0</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="19">
         <v>0</v>
       </c>
       <c r="O14">
@@ -2370,7 +2392,7 @@
       <c r="R14">
         <v>0</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="19">
         <v>0</v>
       </c>
       <c r="T14">
@@ -2388,7 +2410,7 @@
       <c r="X14">
         <v>0</v>
       </c>
-      <c r="Y14">
+      <c r="Y14" s="19">
         <v>0</v>
       </c>
       <c r="Z14" s="1">
@@ -2400,25 +2422,25 @@
       <c r="AB14" s="1">
         <v>1</v>
       </c>
-      <c r="AC14" s="1">
+      <c r="AC14" s="24">
         <v>0</v>
       </c>
       <c r="AD14">
         <v>0</v>
       </c>
-      <c r="AE14">
+      <c r="AE14" s="19">
         <v>1</v>
       </c>
       <c r="AF14">
         <v>0</v>
       </c>
-      <c r="AG14">
+      <c r="AG14" s="19">
         <v>1</v>
       </c>
       <c r="AH14">
         <v>0</v>
       </c>
-      <c r="AI14">
+      <c r="AI14" s="19">
         <v>1</v>
       </c>
       <c r="AJ14">
@@ -2454,7 +2476,7 @@
       <c r="H15">
         <v>0</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="19">
         <v>0</v>
       </c>
       <c r="J15">
@@ -2469,7 +2491,7 @@
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="19">
         <v>0</v>
       </c>
       <c r="O15">
@@ -2484,7 +2506,7 @@
       <c r="R15">
         <v>0</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="19">
         <v>0</v>
       </c>
       <c r="T15">
@@ -2502,7 +2524,7 @@
       <c r="X15">
         <v>0</v>
       </c>
-      <c r="Y15">
+      <c r="Y15" s="19">
         <v>0</v>
       </c>
       <c r="Z15" s="1">
@@ -2514,25 +2536,25 @@
       <c r="AB15" s="1">
         <v>1</v>
       </c>
-      <c r="AC15" s="1">
+      <c r="AC15" s="24">
         <v>0</v>
       </c>
       <c r="AD15">
         <v>1</v>
       </c>
-      <c r="AE15">
+      <c r="AE15" s="19">
         <v>1</v>
       </c>
       <c r="AF15">
         <v>1</v>
       </c>
-      <c r="AG15">
+      <c r="AG15" s="19">
         <v>1</v>
       </c>
       <c r="AH15">
         <v>1</v>
       </c>
-      <c r="AI15">
+      <c r="AI15" s="19">
         <v>1</v>
       </c>
       <c r="AJ15">
@@ -2568,7 +2590,7 @@
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="19">
         <v>0</v>
       </c>
       <c r="J16">
@@ -2583,7 +2605,7 @@
       <c r="M16">
         <v>0</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="19">
         <v>0</v>
       </c>
       <c r="O16">
@@ -2598,7 +2620,7 @@
       <c r="R16">
         <v>0</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="19">
         <v>0</v>
       </c>
       <c r="T16">
@@ -2616,7 +2638,7 @@
       <c r="X16">
         <v>0</v>
       </c>
-      <c r="Y16">
+      <c r="Y16" s="19">
         <v>0</v>
       </c>
       <c r="Z16" s="1">
@@ -2628,25 +2650,25 @@
       <c r="AB16" s="1">
         <v>1</v>
       </c>
-      <c r="AC16" s="1">
+      <c r="AC16" s="24">
         <v>1</v>
       </c>
       <c r="AD16">
         <v>0</v>
       </c>
-      <c r="AE16">
+      <c r="AE16" s="19">
         <v>0</v>
       </c>
       <c r="AF16">
         <v>0</v>
       </c>
-      <c r="AG16">
+      <c r="AG16" s="19">
         <v>0</v>
       </c>
       <c r="AH16">
         <v>1</v>
       </c>
-      <c r="AI16">
+      <c r="AI16" s="19">
         <v>0</v>
       </c>
       <c r="AJ16">
@@ -2682,7 +2704,7 @@
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="19">
         <v>0</v>
       </c>
       <c r="J17">
@@ -2697,7 +2719,7 @@
       <c r="M17">
         <v>1</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="19">
         <v>0</v>
       </c>
       <c r="O17">
@@ -2712,7 +2734,7 @@
       <c r="R17">
         <v>1</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="19">
         <v>0</v>
       </c>
       <c r="T17">
@@ -2730,7 +2752,7 @@
       <c r="X17">
         <v>0</v>
       </c>
-      <c r="Y17">
+      <c r="Y17" s="19">
         <v>0</v>
       </c>
       <c r="Z17" s="1">
@@ -2742,25 +2764,25 @@
       <c r="AB17" s="1">
         <v>1</v>
       </c>
-      <c r="AC17" s="1">
+      <c r="AC17" s="24">
         <v>0</v>
       </c>
       <c r="AD17">
         <v>0</v>
       </c>
-      <c r="AE17">
+      <c r="AE17" s="19">
         <v>0</v>
       </c>
       <c r="AF17">
         <v>0</v>
       </c>
-      <c r="AG17">
+      <c r="AG17" s="19">
         <v>0</v>
       </c>
       <c r="AH17">
         <v>0</v>
       </c>
-      <c r="AI17">
+      <c r="AI17" s="19">
         <v>0</v>
       </c>
       <c r="AJ17">
@@ -2796,7 +2818,7 @@
       <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="19">
         <v>0</v>
       </c>
       <c r="J18">
@@ -2811,7 +2833,7 @@
       <c r="M18">
         <v>1</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="19">
         <v>0</v>
       </c>
       <c r="O18">
@@ -2826,7 +2848,7 @@
       <c r="R18">
         <v>1</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="19">
         <v>0</v>
       </c>
       <c r="T18">
@@ -2844,7 +2866,7 @@
       <c r="X18">
         <v>0</v>
       </c>
-      <c r="Y18">
+      <c r="Y18" s="19">
         <v>0</v>
       </c>
       <c r="Z18" s="1">
@@ -2856,25 +2878,25 @@
       <c r="AB18" s="1">
         <v>1</v>
       </c>
-      <c r="AC18" s="1">
+      <c r="AC18" s="24">
         <v>0</v>
       </c>
       <c r="AD18">
         <v>1</v>
       </c>
-      <c r="AE18">
+      <c r="AE18" s="19">
         <v>1</v>
       </c>
       <c r="AF18">
         <v>1</v>
       </c>
-      <c r="AG18">
+      <c r="AG18" s="19">
         <v>1</v>
       </c>
       <c r="AH18">
         <v>1</v>
       </c>
-      <c r="AI18">
+      <c r="AI18" s="19">
         <v>1</v>
       </c>
       <c r="AJ18">
@@ -2910,7 +2932,7 @@
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="19">
         <v>0</v>
       </c>
       <c r="J19">
@@ -2925,7 +2947,7 @@
       <c r="M19">
         <v>0</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="19">
         <v>0</v>
       </c>
       <c r="O19">
@@ -2940,7 +2962,7 @@
       <c r="R19">
         <v>0</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="19">
         <v>0</v>
       </c>
       <c r="T19">
@@ -2958,7 +2980,7 @@
       <c r="X19">
         <v>0</v>
       </c>
-      <c r="Y19">
+      <c r="Y19" s="19">
         <v>0</v>
       </c>
       <c r="Z19" s="1">
@@ -2970,25 +2992,25 @@
       <c r="AB19" s="1">
         <v>1</v>
       </c>
-      <c r="AC19" s="1">
+      <c r="AC19" s="24">
         <v>1</v>
       </c>
       <c r="AD19">
         <v>0</v>
       </c>
-      <c r="AE19">
+      <c r="AE19" s="19">
         <v>0</v>
       </c>
       <c r="AF19">
         <v>0</v>
       </c>
-      <c r="AG19">
+      <c r="AG19" s="19">
         <v>0</v>
       </c>
       <c r="AH19">
         <v>0</v>
       </c>
-      <c r="AI19">
+      <c r="AI19" s="19">
         <v>0</v>
       </c>
       <c r="AJ19">
@@ -3024,7 +3046,7 @@
       <c r="H20">
         <v>0</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="19">
         <v>0</v>
       </c>
       <c r="J20">
@@ -3039,7 +3061,7 @@
       <c r="M20">
         <v>0</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="19">
         <v>0</v>
       </c>
       <c r="O20">
@@ -3054,7 +3076,7 @@
       <c r="R20">
         <v>0</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="19">
         <v>0</v>
       </c>
       <c r="T20">
@@ -3072,7 +3094,7 @@
       <c r="X20">
         <v>0</v>
       </c>
-      <c r="Y20">
+      <c r="Y20" s="19">
         <v>0</v>
       </c>
       <c r="Z20" s="1">
@@ -3084,25 +3106,25 @@
       <c r="AB20" s="1">
         <v>1</v>
       </c>
-      <c r="AC20" s="1">
+      <c r="AC20" s="24">
         <v>1</v>
       </c>
       <c r="AD20">
         <v>0</v>
       </c>
-      <c r="AE20">
+      <c r="AE20" s="19">
         <v>0</v>
       </c>
       <c r="AF20">
         <v>0</v>
       </c>
-      <c r="AG20">
+      <c r="AG20" s="19">
         <v>0</v>
       </c>
       <c r="AH20">
         <v>1</v>
       </c>
-      <c r="AI20">
+      <c r="AI20" s="19">
         <v>0</v>
       </c>
       <c r="AJ20">
@@ -3138,7 +3160,7 @@
       <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="19">
         <v>0</v>
       </c>
       <c r="J21">
@@ -3153,7 +3175,7 @@
       <c r="M21">
         <v>1</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="19">
         <v>0</v>
       </c>
       <c r="O21">
@@ -3168,7 +3190,7 @@
       <c r="R21">
         <v>1</v>
       </c>
-      <c r="S21">
+      <c r="S21" s="19">
         <v>0</v>
       </c>
       <c r="T21">
@@ -3186,7 +3208,7 @@
       <c r="X21">
         <v>0</v>
       </c>
-      <c r="Y21">
+      <c r="Y21" s="19">
         <v>0</v>
       </c>
       <c r="Z21" s="1">
@@ -3198,25 +3220,25 @@
       <c r="AB21" s="1">
         <v>1</v>
       </c>
-      <c r="AC21" s="1">
+      <c r="AC21" s="24">
         <v>1</v>
       </c>
       <c r="AD21">
         <v>1</v>
       </c>
-      <c r="AE21">
+      <c r="AE21" s="19">
         <v>1</v>
       </c>
       <c r="AF21">
         <v>1</v>
       </c>
-      <c r="AG21">
+      <c r="AG21" s="19">
         <v>1</v>
       </c>
       <c r="AH21">
         <v>1</v>
       </c>
-      <c r="AI21">
+      <c r="AI21" s="19">
         <v>1</v>
       </c>
       <c r="AJ21">
@@ -3252,7 +3274,7 @@
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="19">
         <v>1</v>
       </c>
       <c r="J22">
@@ -3267,7 +3289,7 @@
       <c r="M22">
         <v>1</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="19">
         <v>1</v>
       </c>
       <c r="O22">
@@ -3282,7 +3304,7 @@
       <c r="R22">
         <v>1</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="19">
         <v>1</v>
       </c>
       <c r="T22">
@@ -3300,7 +3322,7 @@
       <c r="X22">
         <v>0</v>
       </c>
-      <c r="Y22">
+      <c r="Y22" s="19">
         <v>0</v>
       </c>
       <c r="Z22" s="1">
@@ -3312,25 +3334,25 @@
       <c r="AB22" s="1">
         <v>1</v>
       </c>
-      <c r="AC22" s="1">
+      <c r="AC22" s="24">
         <v>0</v>
       </c>
       <c r="AD22">
         <v>0</v>
       </c>
-      <c r="AE22">
+      <c r="AE22" s="19">
         <v>0</v>
       </c>
       <c r="AF22">
         <v>1</v>
       </c>
-      <c r="AG22">
+      <c r="AG22" s="19">
         <v>0</v>
       </c>
       <c r="AH22">
         <v>1</v>
       </c>
-      <c r="AI22">
+      <c r="AI22" s="19">
         <v>0</v>
       </c>
       <c r="AJ22">
@@ -3366,7 +3388,7 @@
       <c r="H23">
         <v>1</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="19">
         <v>0</v>
       </c>
       <c r="J23">
@@ -3381,7 +3403,7 @@
       <c r="M23">
         <v>1</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="19">
         <v>0</v>
       </c>
       <c r="O23">
@@ -3396,7 +3418,7 @@
       <c r="R23">
         <v>1</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="19">
         <v>0</v>
       </c>
       <c r="T23">
@@ -3414,7 +3436,7 @@
       <c r="X23">
         <v>0</v>
       </c>
-      <c r="Y23">
+      <c r="Y23" s="19">
         <v>0</v>
       </c>
       <c r="Z23" s="1">
@@ -3426,25 +3448,25 @@
       <c r="AB23" s="1">
         <v>1</v>
       </c>
-      <c r="AC23" s="1">
+      <c r="AC23" s="24">
         <v>0</v>
       </c>
       <c r="AD23">
         <v>1</v>
       </c>
-      <c r="AE23">
+      <c r="AE23" s="19">
         <v>0</v>
       </c>
       <c r="AF23">
         <v>1</v>
       </c>
-      <c r="AG23">
+      <c r="AG23" s="19">
         <v>0</v>
       </c>
       <c r="AH23">
         <v>1</v>
       </c>
-      <c r="AI23">
+      <c r="AI23" s="19">
         <v>0</v>
       </c>
       <c r="AJ23">
@@ -3480,7 +3502,7 @@
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="19">
         <v>0</v>
       </c>
       <c r="J24">
@@ -3495,7 +3517,7 @@
       <c r="M24">
         <v>0</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="19">
         <v>0</v>
       </c>
       <c r="O24">
@@ -3510,7 +3532,7 @@
       <c r="R24">
         <v>0</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="19">
         <v>0</v>
       </c>
       <c r="T24">
@@ -3528,7 +3550,7 @@
       <c r="X24">
         <v>0</v>
       </c>
-      <c r="Y24">
+      <c r="Y24" s="19">
         <v>0</v>
       </c>
       <c r="Z24" s="1">
@@ -3540,25 +3562,25 @@
       <c r="AB24" s="1">
         <v>1</v>
       </c>
-      <c r="AC24" s="1">
+      <c r="AC24" s="24">
         <v>1</v>
       </c>
       <c r="AD24">
         <v>0</v>
       </c>
-      <c r="AE24">
+      <c r="AE24" s="19">
         <v>0</v>
       </c>
       <c r="AF24">
         <v>0</v>
       </c>
-      <c r="AG24">
+      <c r="AG24" s="19">
         <v>0</v>
       </c>
       <c r="AH24">
         <v>1</v>
       </c>
-      <c r="AI24">
+      <c r="AI24" s="19">
         <v>0</v>
       </c>
       <c r="AJ24">
@@ -3594,7 +3616,7 @@
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="19">
         <v>0</v>
       </c>
       <c r="J25">
@@ -3609,7 +3631,7 @@
       <c r="M25">
         <v>0</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="19">
         <v>0</v>
       </c>
       <c r="O25">
@@ -3624,7 +3646,7 @@
       <c r="R25">
         <v>0</v>
       </c>
-      <c r="S25">
+      <c r="S25" s="19">
         <v>0</v>
       </c>
       <c r="T25">
@@ -3642,7 +3664,7 @@
       <c r="X25">
         <v>0</v>
       </c>
-      <c r="Y25">
+      <c r="Y25" s="19">
         <v>0</v>
       </c>
       <c r="Z25" s="1">
@@ -3654,25 +3676,25 @@
       <c r="AB25" s="1">
         <v>1</v>
       </c>
-      <c r="AC25" s="1">
+      <c r="AC25" s="24">
         <v>1</v>
       </c>
       <c r="AD25">
         <v>0</v>
       </c>
-      <c r="AE25">
+      <c r="AE25" s="19">
         <v>0</v>
       </c>
       <c r="AF25">
         <v>0</v>
       </c>
-      <c r="AG25">
+      <c r="AG25" s="19">
         <v>0</v>
       </c>
       <c r="AH25">
         <v>0</v>
       </c>
-      <c r="AI25">
+      <c r="AI25" s="19">
         <v>0</v>
       </c>
       <c r="AJ25">
@@ -3708,7 +3730,7 @@
       <c r="H26">
         <v>1</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="19">
         <v>0</v>
       </c>
       <c r="J26">
@@ -3723,7 +3745,7 @@
       <c r="M26">
         <v>1</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="19">
         <v>0</v>
       </c>
       <c r="O26">
@@ -3738,7 +3760,7 @@
       <c r="R26">
         <v>1</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="19">
         <v>0</v>
       </c>
       <c r="T26">
@@ -3756,7 +3778,7 @@
       <c r="X26">
         <v>0</v>
       </c>
-      <c r="Y26">
+      <c r="Y26" s="19">
         <v>0</v>
       </c>
       <c r="Z26" s="1">
@@ -3768,25 +3790,25 @@
       <c r="AB26" s="1">
         <v>1</v>
       </c>
-      <c r="AC26" s="1">
+      <c r="AC26" s="24">
         <v>0</v>
       </c>
       <c r="AD26">
         <v>0</v>
       </c>
-      <c r="AE26">
+      <c r="AE26" s="19">
         <v>0</v>
       </c>
       <c r="AF26">
         <v>0</v>
       </c>
-      <c r="AG26">
+      <c r="AG26" s="19">
         <v>0</v>
       </c>
       <c r="AH26">
         <v>1</v>
       </c>
-      <c r="AI26">
+      <c r="AI26" s="19">
         <v>0</v>
       </c>
       <c r="AJ26">
@@ -3822,7 +3844,7 @@
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="19">
         <v>0</v>
       </c>
       <c r="J27">
@@ -3837,7 +3859,7 @@
       <c r="M27">
         <v>0</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="19">
         <v>0</v>
       </c>
       <c r="O27">
@@ -3852,7 +3874,7 @@
       <c r="R27">
         <v>0</v>
       </c>
-      <c r="S27">
+      <c r="S27" s="19">
         <v>0</v>
       </c>
       <c r="T27">
@@ -3870,7 +3892,7 @@
       <c r="X27">
         <v>0</v>
       </c>
-      <c r="Y27">
+      <c r="Y27" s="19">
         <v>0</v>
       </c>
       <c r="Z27" s="1">
@@ -3882,25 +3904,25 @@
       <c r="AB27" s="1">
         <v>1</v>
       </c>
-      <c r="AC27" s="1">
+      <c r="AC27" s="24">
         <v>1</v>
       </c>
       <c r="AD27">
         <v>0</v>
       </c>
-      <c r="AE27">
+      <c r="AE27" s="19">
         <v>0</v>
       </c>
       <c r="AF27">
         <v>0</v>
       </c>
-      <c r="AG27">
+      <c r="AG27" s="19">
         <v>0</v>
       </c>
       <c r="AH27">
         <v>1</v>
       </c>
-      <c r="AI27">
+      <c r="AI27" s="19">
         <v>0</v>
       </c>
       <c r="AJ27">
@@ -3936,7 +3958,7 @@
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="19">
         <v>0</v>
       </c>
       <c r="J28">
@@ -3951,7 +3973,7 @@
       <c r="M28">
         <v>0</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="19">
         <v>0</v>
       </c>
       <c r="O28">
@@ -3966,7 +3988,7 @@
       <c r="R28">
         <v>0</v>
       </c>
-      <c r="S28">
+      <c r="S28" s="19">
         <v>0</v>
       </c>
       <c r="T28">
@@ -3984,7 +4006,7 @@
       <c r="X28">
         <v>0</v>
       </c>
-      <c r="Y28">
+      <c r="Y28" s="19">
         <v>0</v>
       </c>
       <c r="Z28" s="1">
@@ -3996,25 +4018,25 @@
       <c r="AB28" s="1">
         <v>1</v>
       </c>
-      <c r="AC28" s="1">
+      <c r="AC28" s="24">
         <v>1</v>
       </c>
       <c r="AD28">
         <v>0</v>
       </c>
-      <c r="AE28">
+      <c r="AE28" s="19">
         <v>0</v>
       </c>
       <c r="AF28">
         <v>0</v>
       </c>
-      <c r="AG28">
+      <c r="AG28" s="19">
         <v>0</v>
       </c>
       <c r="AH28">
         <v>1</v>
       </c>
-      <c r="AI28">
+      <c r="AI28" s="19">
         <v>0</v>
       </c>
       <c r="AJ28">
@@ -4050,7 +4072,7 @@
       <c r="H29">
         <v>0</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="19">
         <v>0</v>
       </c>
       <c r="J29">
@@ -4065,7 +4087,7 @@
       <c r="M29">
         <v>0</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="19">
         <v>0</v>
       </c>
       <c r="O29">
@@ -4080,7 +4102,7 @@
       <c r="R29">
         <v>0</v>
       </c>
-      <c r="S29">
+      <c r="S29" s="19">
         <v>0</v>
       </c>
       <c r="T29">
@@ -4098,7 +4120,7 @@
       <c r="X29">
         <v>0</v>
       </c>
-      <c r="Y29">
+      <c r="Y29" s="19">
         <v>0</v>
       </c>
       <c r="Z29" s="1">
@@ -4110,25 +4132,25 @@
       <c r="AB29" s="1">
         <v>1</v>
       </c>
-      <c r="AC29" s="1">
+      <c r="AC29" s="24">
         <v>1</v>
       </c>
       <c r="AD29">
         <v>0</v>
       </c>
-      <c r="AE29">
+      <c r="AE29" s="19">
         <v>0</v>
       </c>
       <c r="AF29">
         <v>0</v>
       </c>
-      <c r="AG29">
+      <c r="AG29" s="19">
         <v>0</v>
       </c>
       <c r="AH29">
         <v>1</v>
       </c>
-      <c r="AI29">
+      <c r="AI29" s="19">
         <v>0</v>
       </c>
       <c r="AJ29">
@@ -4164,7 +4186,7 @@
       <c r="H30">
         <v>0</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="19">
         <v>0</v>
       </c>
       <c r="J30">
@@ -4179,7 +4201,7 @@
       <c r="M30">
         <v>0</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="19">
         <v>0</v>
       </c>
       <c r="O30">
@@ -4194,7 +4216,7 @@
       <c r="R30">
         <v>0</v>
       </c>
-      <c r="S30">
+      <c r="S30" s="19">
         <v>0</v>
       </c>
       <c r="T30">
@@ -4212,7 +4234,7 @@
       <c r="X30">
         <v>1</v>
       </c>
-      <c r="Y30">
+      <c r="Y30" s="19">
         <v>1</v>
       </c>
       <c r="Z30" s="1">
@@ -4224,25 +4246,25 @@
       <c r="AB30" s="1">
         <v>0</v>
       </c>
-      <c r="AC30" s="1">
+      <c r="AC30" s="24">
         <v>1</v>
       </c>
       <c r="AD30">
         <v>0</v>
       </c>
-      <c r="AE30">
+      <c r="AE30" s="19">
         <v>0</v>
       </c>
       <c r="AF30">
         <v>0</v>
       </c>
-      <c r="AG30">
+      <c r="AG30" s="19">
         <v>0</v>
       </c>
       <c r="AH30">
         <v>0</v>
       </c>
-      <c r="AI30">
+      <c r="AI30" s="19">
         <v>0</v>
       </c>
       <c r="AJ30">
@@ -4278,7 +4300,7 @@
       <c r="H31">
         <v>0</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="19">
         <v>0</v>
       </c>
       <c r="J31">
@@ -4293,7 +4315,7 @@
       <c r="M31">
         <v>0</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="19">
         <v>0</v>
       </c>
       <c r="O31">
@@ -4308,7 +4330,7 @@
       <c r="R31">
         <v>0</v>
       </c>
-      <c r="S31">
+      <c r="S31" s="19">
         <v>0</v>
       </c>
       <c r="T31">
@@ -4326,7 +4348,7 @@
       <c r="X31">
         <v>0</v>
       </c>
-      <c r="Y31">
+      <c r="Y31" s="19">
         <v>0</v>
       </c>
       <c r="Z31" s="1">
@@ -4338,25 +4360,25 @@
       <c r="AB31" s="1">
         <v>1</v>
       </c>
-      <c r="AC31" s="1">
+      <c r="AC31" s="24">
         <v>1</v>
       </c>
       <c r="AD31">
         <v>0</v>
       </c>
-      <c r="AE31">
+      <c r="AE31" s="19">
         <v>0</v>
       </c>
       <c r="AF31">
         <v>0</v>
       </c>
-      <c r="AG31">
+      <c r="AG31" s="19">
         <v>0</v>
       </c>
       <c r="AH31">
         <v>1</v>
       </c>
-      <c r="AI31">
+      <c r="AI31" s="19">
         <v>0</v>
       </c>
       <c r="AJ31">
@@ -4392,7 +4414,7 @@
       <c r="H32">
         <v>0</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="19">
         <v>1</v>
       </c>
       <c r="J32">
@@ -4407,7 +4429,7 @@
       <c r="M32">
         <v>0</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="19">
         <v>1</v>
       </c>
       <c r="O32">
@@ -4422,7 +4444,7 @@
       <c r="R32">
         <v>0</v>
       </c>
-      <c r="S32">
+      <c r="S32" s="19">
         <v>1</v>
       </c>
       <c r="T32">
@@ -4440,7 +4462,7 @@
       <c r="X32">
         <v>1</v>
       </c>
-      <c r="Y32">
+      <c r="Y32" s="19">
         <v>1</v>
       </c>
       <c r="Z32" s="1">
@@ -4452,25 +4474,25 @@
       <c r="AB32" s="1">
         <v>1</v>
       </c>
-      <c r="AC32" s="1">
+      <c r="AC32" s="24">
         <v>1</v>
       </c>
       <c r="AD32">
         <v>1</v>
       </c>
-      <c r="AE32">
+      <c r="AE32" s="19">
         <v>1</v>
       </c>
       <c r="AF32">
         <v>1</v>
       </c>
-      <c r="AG32">
+      <c r="AG32" s="19">
         <v>1</v>
       </c>
       <c r="AH32">
         <v>1</v>
       </c>
-      <c r="AI32">
+      <c r="AI32" s="19">
         <v>1</v>
       </c>
       <c r="AJ32">
@@ -4506,7 +4528,7 @@
       <c r="H33">
         <v>0</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="19">
         <v>0</v>
       </c>
       <c r="J33">
@@ -4521,7 +4543,7 @@
       <c r="M33">
         <v>0</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="19">
         <v>0</v>
       </c>
       <c r="O33">
@@ -4536,7 +4558,7 @@
       <c r="R33">
         <v>0</v>
       </c>
-      <c r="S33">
+      <c r="S33" s="19">
         <v>0</v>
       </c>
       <c r="T33">
@@ -4554,7 +4576,7 @@
       <c r="X33">
         <v>0</v>
       </c>
-      <c r="Y33">
+      <c r="Y33" s="19">
         <v>0</v>
       </c>
       <c r="Z33" s="1">
@@ -4566,25 +4588,25 @@
       <c r="AB33" s="1">
         <v>1</v>
       </c>
-      <c r="AC33" s="1">
+      <c r="AC33" s="24">
         <v>0</v>
       </c>
       <c r="AD33">
         <v>1</v>
       </c>
-      <c r="AE33">
+      <c r="AE33" s="19">
         <v>1</v>
       </c>
       <c r="AF33">
         <v>1</v>
       </c>
-      <c r="AG33">
+      <c r="AG33" s="19">
         <v>1</v>
       </c>
       <c r="AH33">
         <v>1</v>
       </c>
-      <c r="AI33">
+      <c r="AI33" s="19">
         <v>1</v>
       </c>
       <c r="AJ33">
@@ -4620,7 +4642,7 @@
       <c r="H34">
         <v>1</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="19">
         <v>0</v>
       </c>
       <c r="J34">
@@ -4635,7 +4657,7 @@
       <c r="M34">
         <v>1</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="19">
         <v>0</v>
       </c>
       <c r="O34">
@@ -4650,7 +4672,7 @@
       <c r="R34">
         <v>1</v>
       </c>
-      <c r="S34">
+      <c r="S34" s="19">
         <v>0</v>
       </c>
       <c r="T34">
@@ -4668,7 +4690,7 @@
       <c r="X34">
         <v>0</v>
       </c>
-      <c r="Y34">
+      <c r="Y34" s="19">
         <v>0</v>
       </c>
       <c r="Z34" s="1">
@@ -4680,25 +4702,25 @@
       <c r="AB34" s="1">
         <v>1</v>
       </c>
-      <c r="AC34" s="1">
+      <c r="AC34" s="24">
         <v>0</v>
       </c>
       <c r="AD34">
         <v>0</v>
       </c>
-      <c r="AE34">
+      <c r="AE34" s="19">
         <v>1</v>
       </c>
       <c r="AF34">
         <v>0</v>
       </c>
-      <c r="AG34">
+      <c r="AG34" s="19">
         <v>1</v>
       </c>
       <c r="AH34">
         <v>0</v>
       </c>
-      <c r="AI34">
+      <c r="AI34" s="19">
         <v>1</v>
       </c>
       <c r="AJ34">
@@ -4734,7 +4756,7 @@
       <c r="H35">
         <v>1</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="19">
         <v>0</v>
       </c>
       <c r="J35">
@@ -4749,7 +4771,7 @@
       <c r="M35">
         <v>1</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="19">
         <v>0</v>
       </c>
       <c r="O35">
@@ -4764,7 +4786,7 @@
       <c r="R35">
         <v>1</v>
       </c>
-      <c r="S35">
+      <c r="S35" s="19">
         <v>0</v>
       </c>
       <c r="T35">
@@ -4782,7 +4804,7 @@
       <c r="X35">
         <v>0</v>
       </c>
-      <c r="Y35">
+      <c r="Y35" s="19">
         <v>0</v>
       </c>
       <c r="Z35" s="1">
@@ -4794,25 +4816,25 @@
       <c r="AB35" s="1">
         <v>1</v>
       </c>
-      <c r="AC35" s="1">
+      <c r="AC35" s="24">
         <v>0</v>
       </c>
       <c r="AD35">
         <v>0</v>
       </c>
-      <c r="AE35">
+      <c r="AE35" s="19">
         <v>0</v>
       </c>
       <c r="AF35">
         <v>0</v>
       </c>
-      <c r="AG35">
+      <c r="AG35" s="19">
         <v>0</v>
       </c>
       <c r="AH35">
         <v>0</v>
       </c>
-      <c r="AI35">
+      <c r="AI35" s="19">
         <v>0</v>
       </c>
       <c r="AJ35">
@@ -4848,7 +4870,7 @@
       <c r="H36">
         <v>1</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="19">
         <v>1</v>
       </c>
       <c r="J36">
@@ -4863,7 +4885,7 @@
       <c r="M36">
         <v>1</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="19">
         <v>1</v>
       </c>
       <c r="O36">
@@ -4878,7 +4900,7 @@
       <c r="R36">
         <v>1</v>
       </c>
-      <c r="S36">
+      <c r="S36" s="19">
         <v>1</v>
       </c>
       <c r="T36">
@@ -4896,7 +4918,7 @@
       <c r="X36">
         <v>0</v>
       </c>
-      <c r="Y36">
+      <c r="Y36" s="19">
         <v>0</v>
       </c>
       <c r="Z36" s="1">
@@ -4908,25 +4930,25 @@
       <c r="AB36" s="1">
         <v>1</v>
       </c>
-      <c r="AC36" s="1">
+      <c r="AC36" s="24">
         <v>0</v>
       </c>
       <c r="AD36">
         <v>0</v>
       </c>
-      <c r="AE36">
+      <c r="AE36" s="19">
         <v>0</v>
       </c>
       <c r="AF36">
         <v>0</v>
       </c>
-      <c r="AG36">
+      <c r="AG36" s="19">
         <v>1</v>
       </c>
       <c r="AH36">
         <v>0</v>
       </c>
-      <c r="AI36">
+      <c r="AI36" s="19">
         <v>1</v>
       </c>
       <c r="AJ36">
@@ -4962,7 +4984,7 @@
       <c r="H37">
         <v>1</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="19">
         <v>0</v>
       </c>
       <c r="J37">
@@ -4977,7 +4999,7 @@
       <c r="M37">
         <v>1</v>
       </c>
-      <c r="N37">
+      <c r="N37" s="19">
         <v>0</v>
       </c>
       <c r="O37">
@@ -4992,7 +5014,7 @@
       <c r="R37">
         <v>1</v>
       </c>
-      <c r="S37">
+      <c r="S37" s="19">
         <v>0</v>
       </c>
       <c r="T37">
@@ -5010,7 +5032,7 @@
       <c r="X37">
         <v>0</v>
       </c>
-      <c r="Y37">
+      <c r="Y37" s="19">
         <v>0</v>
       </c>
       <c r="Z37" s="1">
@@ -5022,25 +5044,25 @@
       <c r="AB37" s="1">
         <v>1</v>
       </c>
-      <c r="AC37" s="1">
+      <c r="AC37" s="24">
         <v>0</v>
       </c>
       <c r="AD37">
         <v>0</v>
       </c>
-      <c r="AE37">
+      <c r="AE37" s="19">
         <v>0</v>
       </c>
       <c r="AF37">
         <v>0</v>
       </c>
-      <c r="AG37">
+      <c r="AG37" s="19">
         <v>0</v>
       </c>
       <c r="AH37">
         <v>1</v>
       </c>
-      <c r="AI37">
+      <c r="AI37" s="19">
         <v>0</v>
       </c>
       <c r="AJ37">
@@ -5076,7 +5098,7 @@
       <c r="H38">
         <v>0</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="19">
         <v>0</v>
       </c>
       <c r="J38">
@@ -5091,7 +5113,7 @@
       <c r="M38">
         <v>0</v>
       </c>
-      <c r="N38">
+      <c r="N38" s="19">
         <v>0</v>
       </c>
       <c r="O38">
@@ -5106,7 +5128,7 @@
       <c r="R38">
         <v>0</v>
       </c>
-      <c r="S38">
+      <c r="S38" s="19">
         <v>0</v>
       </c>
       <c r="T38">
@@ -5124,7 +5146,7 @@
       <c r="X38">
         <v>0</v>
       </c>
-      <c r="Y38">
+      <c r="Y38" s="19">
         <v>0</v>
       </c>
       <c r="Z38" s="1">
@@ -5136,25 +5158,25 @@
       <c r="AB38" s="1">
         <v>1</v>
       </c>
-      <c r="AC38" s="1">
+      <c r="AC38" s="24">
         <v>1</v>
       </c>
       <c r="AD38">
         <v>0</v>
       </c>
-      <c r="AE38">
+      <c r="AE38" s="19">
         <v>0</v>
       </c>
       <c r="AF38">
         <v>0</v>
       </c>
-      <c r="AG38">
+      <c r="AG38" s="19">
         <v>0</v>
       </c>
       <c r="AH38">
         <v>1</v>
       </c>
-      <c r="AI38">
+      <c r="AI38" s="19">
         <v>0</v>
       </c>
       <c r="AJ38">
@@ -5190,7 +5212,7 @@
       <c r="H39">
         <v>0</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="19">
         <v>0</v>
       </c>
       <c r="J39">
@@ -5205,7 +5227,7 @@
       <c r="M39">
         <v>1</v>
       </c>
-      <c r="N39">
+      <c r="N39" s="19">
         <v>0</v>
       </c>
       <c r="O39">
@@ -5220,7 +5242,7 @@
       <c r="R39">
         <v>1</v>
       </c>
-      <c r="S39">
+      <c r="S39" s="19">
         <v>0</v>
       </c>
       <c r="T39">
@@ -5238,7 +5260,7 @@
       <c r="X39">
         <v>0</v>
       </c>
-      <c r="Y39">
+      <c r="Y39" s="19">
         <v>0</v>
       </c>
       <c r="Z39" s="1">
@@ -5250,25 +5272,25 @@
       <c r="AB39" s="1">
         <v>1</v>
       </c>
-      <c r="AC39" s="1">
+      <c r="AC39" s="24">
         <v>0</v>
       </c>
       <c r="AD39">
         <v>0</v>
       </c>
-      <c r="AE39">
+      <c r="AE39" s="19">
         <v>0</v>
       </c>
       <c r="AF39">
         <v>0</v>
       </c>
-      <c r="AG39">
+      <c r="AG39" s="19">
         <v>0</v>
       </c>
       <c r="AH39">
         <v>0</v>
       </c>
-      <c r="AI39">
+      <c r="AI39" s="19">
         <v>0</v>
       </c>
       <c r="AJ39">
@@ -5304,7 +5326,7 @@
       <c r="H40">
         <v>0</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="19">
         <v>0</v>
       </c>
       <c r="J40">
@@ -5319,7 +5341,7 @@
       <c r="M40">
         <v>0</v>
       </c>
-      <c r="N40">
+      <c r="N40" s="19">
         <v>0</v>
       </c>
       <c r="O40">
@@ -5334,7 +5356,7 @@
       <c r="R40">
         <v>0</v>
       </c>
-      <c r="S40">
+      <c r="S40" s="19">
         <v>0</v>
       </c>
       <c r="T40">
@@ -5352,7 +5374,7 @@
       <c r="X40">
         <v>0</v>
       </c>
-      <c r="Y40">
+      <c r="Y40" s="19">
         <v>0</v>
       </c>
       <c r="Z40" s="1">
@@ -5364,25 +5386,25 @@
       <c r="AB40" s="1">
         <v>1</v>
       </c>
-      <c r="AC40" s="1">
+      <c r="AC40" s="24">
         <v>1</v>
       </c>
       <c r="AD40">
         <v>0</v>
       </c>
-      <c r="AE40">
+      <c r="AE40" s="19">
         <v>0</v>
       </c>
       <c r="AF40">
         <v>0</v>
       </c>
-      <c r="AG40">
+      <c r="AG40" s="19">
         <v>0</v>
       </c>
       <c r="AH40">
         <v>1</v>
       </c>
-      <c r="AI40">
+      <c r="AI40" s="19">
         <v>0</v>
       </c>
       <c r="AJ40">
@@ -5418,7 +5440,7 @@
       <c r="H41">
         <v>0</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="19">
         <v>1</v>
       </c>
       <c r="J41">
@@ -5433,7 +5455,7 @@
       <c r="M41">
         <v>0</v>
       </c>
-      <c r="N41">
+      <c r="N41" s="19">
         <v>1</v>
       </c>
       <c r="O41">
@@ -5448,7 +5470,7 @@
       <c r="R41">
         <v>0</v>
       </c>
-      <c r="S41">
+      <c r="S41" s="19">
         <v>1</v>
       </c>
       <c r="T41">
@@ -5466,7 +5488,7 @@
       <c r="X41">
         <v>1</v>
       </c>
-      <c r="Y41">
+      <c r="Y41" s="19">
         <v>0</v>
       </c>
       <c r="Z41" s="1">
@@ -5478,25 +5500,25 @@
       <c r="AB41" s="1">
         <v>1</v>
       </c>
-      <c r="AC41" s="1">
+      <c r="AC41" s="24">
         <v>1</v>
       </c>
       <c r="AD41">
         <v>0</v>
       </c>
-      <c r="AE41">
+      <c r="AE41" s="19">
         <v>1</v>
       </c>
       <c r="AF41">
         <v>0</v>
       </c>
-      <c r="AG41">
+      <c r="AG41" s="19">
         <v>1</v>
       </c>
       <c r="AH41">
         <v>0</v>
       </c>
-      <c r="AI41">
+      <c r="AI41" s="19">
         <v>1</v>
       </c>
       <c r="AJ41">
@@ -5532,7 +5554,7 @@
       <c r="H42">
         <v>0</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="19">
         <v>1</v>
       </c>
       <c r="J42">
@@ -5547,7 +5569,7 @@
       <c r="M42">
         <v>0</v>
       </c>
-      <c r="N42">
+      <c r="N42" s="19">
         <v>1</v>
       </c>
       <c r="O42">
@@ -5562,7 +5584,7 @@
       <c r="R42">
         <v>0</v>
       </c>
-      <c r="S42">
+      <c r="S42" s="19">
         <v>1</v>
       </c>
       <c r="T42">
@@ -5580,7 +5602,7 @@
       <c r="X42">
         <v>1</v>
       </c>
-      <c r="Y42">
+      <c r="Y42" s="19">
         <v>1</v>
       </c>
       <c r="Z42" s="1">
@@ -5592,25 +5614,25 @@
       <c r="AB42" s="1">
         <v>1</v>
       </c>
-      <c r="AC42" s="1">
+      <c r="AC42" s="24">
         <v>1</v>
       </c>
       <c r="AD42">
         <v>0</v>
       </c>
-      <c r="AE42">
+      <c r="AE42" s="19">
         <v>0</v>
       </c>
       <c r="AF42">
         <v>0</v>
       </c>
-      <c r="AG42">
+      <c r="AG42" s="19">
         <v>0</v>
       </c>
       <c r="AH42">
         <v>0</v>
       </c>
-      <c r="AI42">
+      <c r="AI42" s="19">
         <v>1</v>
       </c>
       <c r="AJ42">
@@ -5646,7 +5668,7 @@
       <c r="H43">
         <v>0</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="19">
         <v>0</v>
       </c>
       <c r="J43">
@@ -5661,7 +5683,7 @@
       <c r="M43">
         <v>1</v>
       </c>
-      <c r="N43">
+      <c r="N43" s="19">
         <v>0</v>
       </c>
       <c r="O43">
@@ -5676,7 +5698,7 @@
       <c r="R43">
         <v>0</v>
       </c>
-      <c r="S43">
+      <c r="S43" s="19">
         <v>0</v>
       </c>
       <c r="T43">
@@ -5694,7 +5716,7 @@
       <c r="X43">
         <v>0</v>
       </c>
-      <c r="Y43">
+      <c r="Y43" s="19">
         <v>0</v>
       </c>
       <c r="Z43" s="1">
@@ -5706,25 +5728,25 @@
       <c r="AB43" s="1">
         <v>0</v>
       </c>
-      <c r="AC43" s="1">
+      <c r="AC43" s="24">
         <v>1</v>
       </c>
       <c r="AD43">
         <v>0</v>
       </c>
-      <c r="AE43">
+      <c r="AE43" s="19">
         <v>0</v>
       </c>
       <c r="AF43">
         <v>0</v>
       </c>
-      <c r="AG43">
+      <c r="AG43" s="19">
         <v>0</v>
       </c>
       <c r="AH43">
         <v>0</v>
       </c>
-      <c r="AI43">
+      <c r="AI43" s="19">
         <v>0</v>
       </c>
       <c r="AJ43">
@@ -5760,7 +5782,7 @@
       <c r="H44">
         <v>0</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="19">
         <v>1</v>
       </c>
       <c r="J44">
@@ -5775,7 +5797,7 @@
       <c r="M44">
         <v>0</v>
       </c>
-      <c r="N44">
+      <c r="N44" s="19">
         <v>1</v>
       </c>
       <c r="O44">
@@ -5790,7 +5812,7 @@
       <c r="R44">
         <v>0</v>
       </c>
-      <c r="S44">
+      <c r="S44" s="19">
         <v>1</v>
       </c>
       <c r="T44">
@@ -5808,7 +5830,7 @@
       <c r="X44">
         <v>1</v>
       </c>
-      <c r="Y44">
+      <c r="Y44" s="19">
         <v>0</v>
       </c>
       <c r="Z44" s="1">
@@ -5820,25 +5842,25 @@
       <c r="AB44" s="1">
         <v>1</v>
       </c>
-      <c r="AC44" s="1">
+      <c r="AC44" s="24">
         <v>1</v>
       </c>
       <c r="AD44">
         <v>0</v>
       </c>
-      <c r="AE44">
+      <c r="AE44" s="19">
         <v>1</v>
       </c>
       <c r="AF44">
         <v>0</v>
       </c>
-      <c r="AG44">
+      <c r="AG44" s="19">
         <v>1</v>
       </c>
       <c r="AH44">
         <v>0</v>
       </c>
-      <c r="AI44">
+      <c r="AI44" s="19">
         <v>1</v>
       </c>
       <c r="AJ44">
@@ -5874,7 +5896,7 @@
       <c r="H45">
         <v>0</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="19">
         <v>0</v>
       </c>
       <c r="J45">
@@ -5889,7 +5911,7 @@
       <c r="M45">
         <v>0</v>
       </c>
-      <c r="N45">
+      <c r="N45" s="19">
         <v>0</v>
       </c>
       <c r="O45">
@@ -5904,7 +5926,7 @@
       <c r="R45">
         <v>0</v>
       </c>
-      <c r="S45">
+      <c r="S45" s="19">
         <v>0</v>
       </c>
       <c r="T45">
@@ -5922,7 +5944,7 @@
       <c r="X45">
         <v>0</v>
       </c>
-      <c r="Y45">
+      <c r="Y45" s="19">
         <v>0</v>
       </c>
       <c r="Z45" s="1">
@@ -5934,25 +5956,25 @@
       <c r="AB45" s="1">
         <v>1</v>
       </c>
-      <c r="AC45" s="1">
+      <c r="AC45" s="24">
         <v>1</v>
       </c>
       <c r="AD45">
         <v>0</v>
       </c>
-      <c r="AE45">
+      <c r="AE45" s="19">
         <v>0</v>
       </c>
       <c r="AF45">
         <v>0</v>
       </c>
-      <c r="AG45">
+      <c r="AG45" s="19">
         <v>0</v>
       </c>
       <c r="AH45">
         <v>1</v>
       </c>
-      <c r="AI45">
+      <c r="AI45" s="19">
         <v>0</v>
       </c>
       <c r="AJ45">
@@ -5988,7 +6010,7 @@
       <c r="H46">
         <v>1</v>
       </c>
-      <c r="I46">
+      <c r="I46" s="19">
         <v>0</v>
       </c>
       <c r="J46">
@@ -6003,7 +6025,7 @@
       <c r="M46">
         <v>1</v>
       </c>
-      <c r="N46">
+      <c r="N46" s="19">
         <v>0</v>
       </c>
       <c r="O46">
@@ -6018,7 +6040,7 @@
       <c r="R46">
         <v>1</v>
       </c>
-      <c r="S46">
+      <c r="S46" s="19">
         <v>0</v>
       </c>
       <c r="T46">
@@ -6036,7 +6058,7 @@
       <c r="X46">
         <v>0</v>
       </c>
-      <c r="Y46">
+      <c r="Y46" s="19">
         <v>0</v>
       </c>
       <c r="Z46" s="1">
@@ -6048,25 +6070,25 @@
       <c r="AB46" s="1">
         <v>1</v>
       </c>
-      <c r="AC46" s="1">
+      <c r="AC46" s="24">
         <v>0</v>
       </c>
       <c r="AD46">
         <v>1</v>
       </c>
-      <c r="AE46">
+      <c r="AE46" s="19">
         <v>1</v>
       </c>
       <c r="AF46">
         <v>1</v>
       </c>
-      <c r="AG46">
+      <c r="AG46" s="19">
         <v>1</v>
       </c>
       <c r="AH46">
         <v>1</v>
       </c>
-      <c r="AI46">
+      <c r="AI46" s="19">
         <v>1</v>
       </c>
       <c r="AJ46">
@@ -6102,7 +6124,7 @@
       <c r="H47">
         <v>0</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="19">
         <v>0</v>
       </c>
       <c r="J47">
@@ -6117,7 +6139,7 @@
       <c r="M47">
         <v>1</v>
       </c>
-      <c r="N47">
+      <c r="N47" s="19">
         <v>0</v>
       </c>
       <c r="O47">
@@ -6132,7 +6154,7 @@
       <c r="R47">
         <v>1</v>
       </c>
-      <c r="S47">
+      <c r="S47" s="19">
         <v>0</v>
       </c>
       <c r="T47">
@@ -6150,7 +6172,7 @@
       <c r="X47">
         <v>0</v>
       </c>
-      <c r="Y47">
+      <c r="Y47" s="19">
         <v>0</v>
       </c>
       <c r="Z47" s="1">
@@ -6162,25 +6184,25 @@
       <c r="AB47" s="1">
         <v>1</v>
       </c>
-      <c r="AC47" s="1">
+      <c r="AC47" s="24">
         <v>0</v>
       </c>
       <c r="AD47">
         <v>0</v>
       </c>
-      <c r="AE47">
+      <c r="AE47" s="19">
         <v>0</v>
       </c>
       <c r="AF47">
         <v>1</v>
       </c>
-      <c r="AG47">
+      <c r="AG47" s="19">
         <v>1</v>
       </c>
       <c r="AH47">
         <v>1</v>
       </c>
-      <c r="AI47">
+      <c r="AI47" s="19">
         <v>1</v>
       </c>
       <c r="AJ47">

</xml_diff>

<commit_message>
updated change.xlsx to contain correct strategies
</commit_message>
<xml_diff>
--- a/Mammal matrix.xlsx
+++ b/Mammal matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA49EDBE-D048-834F-B084-CDA20F58E389}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7EB2C0-BE0B-0545-83B5-918751B2D8B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -946,9 +946,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD13" sqref="AD13"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6236,7 +6236,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
mammals - change implementation of D and A so if both above+below ground vertebrates are eaten/affected, it 'or's them together (hasn't worked)
</commit_message>
<xml_diff>
--- a/Mammal matrix.xlsx
+++ b/Mammal matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7EB2C0-BE0B-0545-83B5-918751B2D8B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18274077-389E-0447-BD58-8D19BF60B834}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-1580" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -572,32 +572,11 @@
       <alignment indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -606,6 +585,27 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,9 +946,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -960,128 +960,128 @@
     <col min="5" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5" style="12" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="26" max="28" width="7.6640625" customWidth="1"/>
-    <col min="29" max="29" width="7.6640625" style="19" customWidth="1"/>
+    <col min="29" max="29" width="7.6640625" style="12" customWidth="1"/>
     <col min="30" max="30" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5" style="12" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.5" style="12" bestFit="1" customWidth="1"/>
     <col min="36" max="37" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="10" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="13" t="s">
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="8" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="6" t="s">
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="8" t="s">
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="11" t="s">
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="AA2" s="12" t="s">
+      <c r="AA2" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="AB2" s="11" t="s">
+      <c r="AB2" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="AC2" s="23" t="s">
+      <c r="AC2" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="AD2" s="14" t="s">
+      <c r="AD2" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="16" t="s">
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="AG2" s="16"/>
-      <c r="AH2" s="14" t="s">
+      <c r="AG2" s="21"/>
+      <c r="AH2" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="16" t="s">
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="AK2" s="16"/>
+      <c r="AK2" s="21"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -1096,103 +1096,103 @@
       <c r="D3" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="S3" s="18" t="s">
+      <c r="S3" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="T3" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="U3" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="V3" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="W3" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="X3" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="Y3" s="20" t="s">
+      <c r="Y3" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="Z3" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="AB3" s="11" t="s">
+      <c r="AB3" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="AC3" s="23" t="s">
+      <c r="AC3" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="AD3" s="15" t="s">
+      <c r="AD3" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="AE3" s="21" t="s">
+      <c r="AE3" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="AF3" s="17" t="s">
+      <c r="AF3" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="AG3" s="22" t="s">
+      <c r="AG3" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="AH3" s="15" t="s">
+      <c r="AH3" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="AI3" s="21" t="s">
+      <c r="AI3" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="AJ3" s="17" t="s">
+      <c r="AJ3" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="AK3" s="17" t="s">
+      <c r="AK3" s="10" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1222,7 +1222,7 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="12">
         <v>1</v>
       </c>
       <c r="J4">
@@ -1237,7 +1237,7 @@
       <c r="M4">
         <v>1</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="12">
         <v>1</v>
       </c>
       <c r="O4">
@@ -1252,7 +1252,7 @@
       <c r="R4">
         <v>1</v>
       </c>
-      <c r="S4" s="19">
+      <c r="S4" s="12">
         <v>1</v>
       </c>
       <c r="T4">
@@ -1270,7 +1270,7 @@
       <c r="X4">
         <v>0</v>
       </c>
-      <c r="Y4" s="19">
+      <c r="Y4" s="12">
         <v>0</v>
       </c>
       <c r="Z4" s="1">
@@ -1282,25 +1282,25 @@
       <c r="AB4" s="1">
         <v>1</v>
       </c>
-      <c r="AC4" s="24">
+      <c r="AC4" s="17">
         <v>0</v>
       </c>
       <c r="AD4">
         <v>0</v>
       </c>
-      <c r="AE4" s="19">
+      <c r="AE4" s="12">
         <v>1</v>
       </c>
       <c r="AF4">
         <v>0</v>
       </c>
-      <c r="AG4" s="19">
+      <c r="AG4" s="12">
         <v>1</v>
       </c>
       <c r="AH4">
         <v>0</v>
       </c>
-      <c r="AI4" s="19">
+      <c r="AI4" s="12">
         <v>1</v>
       </c>
       <c r="AJ4">
@@ -1336,7 +1336,7 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="12">
         <v>0</v>
       </c>
       <c r="J5">
@@ -1351,7 +1351,7 @@
       <c r="M5">
         <v>1</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="12">
         <v>0</v>
       </c>
       <c r="O5">
@@ -1366,7 +1366,7 @@
       <c r="R5">
         <v>1</v>
       </c>
-      <c r="S5" s="19">
+      <c r="S5" s="12">
         <v>0</v>
       </c>
       <c r="T5">
@@ -1384,7 +1384,7 @@
       <c r="X5">
         <v>0</v>
       </c>
-      <c r="Y5" s="19">
+      <c r="Y5" s="12">
         <v>0</v>
       </c>
       <c r="Z5" s="1">
@@ -1396,25 +1396,25 @@
       <c r="AB5" s="1">
         <v>1</v>
       </c>
-      <c r="AC5" s="24">
+      <c r="AC5" s="17">
         <v>0</v>
       </c>
       <c r="AD5">
         <v>0</v>
       </c>
-      <c r="AE5" s="19">
+      <c r="AE5" s="12">
         <v>0</v>
       </c>
       <c r="AF5">
         <v>0</v>
       </c>
-      <c r="AG5" s="19">
+      <c r="AG5" s="12">
         <v>1</v>
       </c>
       <c r="AH5">
         <v>0</v>
       </c>
-      <c r="AI5" s="19">
+      <c r="AI5" s="12">
         <v>1</v>
       </c>
       <c r="AJ5">
@@ -1450,7 +1450,7 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="12">
         <v>0</v>
       </c>
       <c r="J6">
@@ -1465,7 +1465,7 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="12">
         <v>0</v>
       </c>
       <c r="O6">
@@ -1480,7 +1480,7 @@
       <c r="R6">
         <v>0</v>
       </c>
-      <c r="S6" s="19">
+      <c r="S6" s="12">
         <v>0</v>
       </c>
       <c r="T6">
@@ -1498,7 +1498,7 @@
       <c r="X6">
         <v>0</v>
       </c>
-      <c r="Y6" s="19">
+      <c r="Y6" s="12">
         <v>0</v>
       </c>
       <c r="Z6" s="1">
@@ -1510,25 +1510,25 @@
       <c r="AB6" s="1">
         <v>1</v>
       </c>
-      <c r="AC6" s="24">
+      <c r="AC6" s="17">
         <v>1</v>
       </c>
       <c r="AD6">
         <v>0</v>
       </c>
-      <c r="AE6" s="19">
+      <c r="AE6" s="12">
         <v>0</v>
       </c>
       <c r="AF6">
         <v>0</v>
       </c>
-      <c r="AG6" s="19">
+      <c r="AG6" s="12">
         <v>0</v>
       </c>
       <c r="AH6">
         <v>1</v>
       </c>
-      <c r="AI6" s="19">
+      <c r="AI6" s="12">
         <v>0</v>
       </c>
       <c r="AJ6">
@@ -1564,7 +1564,7 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="12">
         <v>0</v>
       </c>
       <c r="J7">
@@ -1579,7 +1579,7 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="12">
         <v>0</v>
       </c>
       <c r="O7">
@@ -1594,7 +1594,7 @@
       <c r="R7">
         <v>0</v>
       </c>
-      <c r="S7" s="19">
+      <c r="S7" s="12">
         <v>0</v>
       </c>
       <c r="T7">
@@ -1612,7 +1612,7 @@
       <c r="X7">
         <v>0</v>
       </c>
-      <c r="Y7" s="19">
+      <c r="Y7" s="12">
         <v>0</v>
       </c>
       <c r="Z7" s="1">
@@ -1624,25 +1624,25 @@
       <c r="AB7" s="1">
         <v>1</v>
       </c>
-      <c r="AC7" s="24">
+      <c r="AC7" s="17">
         <v>1</v>
       </c>
       <c r="AD7">
         <v>0</v>
       </c>
-      <c r="AE7" s="19">
+      <c r="AE7" s="12">
         <v>0</v>
       </c>
       <c r="AF7">
         <v>0</v>
       </c>
-      <c r="AG7" s="19">
+      <c r="AG7" s="12">
         <v>0</v>
       </c>
       <c r="AH7">
         <v>1</v>
       </c>
-      <c r="AI7" s="19">
+      <c r="AI7" s="12">
         <v>0</v>
       </c>
       <c r="AJ7">
@@ -1678,7 +1678,7 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="12">
         <v>0</v>
       </c>
       <c r="J8">
@@ -1693,7 +1693,7 @@
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="12">
         <v>0</v>
       </c>
       <c r="O8">
@@ -1708,7 +1708,7 @@
       <c r="R8">
         <v>0</v>
       </c>
-      <c r="S8" s="19">
+      <c r="S8" s="12">
         <v>0</v>
       </c>
       <c r="T8">
@@ -1726,7 +1726,7 @@
       <c r="X8">
         <v>0</v>
       </c>
-      <c r="Y8" s="19">
+      <c r="Y8" s="12">
         <v>0</v>
       </c>
       <c r="Z8" s="1">
@@ -1738,25 +1738,25 @@
       <c r="AB8" s="1">
         <v>1</v>
       </c>
-      <c r="AC8" s="24">
+      <c r="AC8" s="17">
         <v>1</v>
       </c>
       <c r="AD8">
         <v>0</v>
       </c>
-      <c r="AE8" s="19">
+      <c r="AE8" s="12">
         <v>0</v>
       </c>
       <c r="AF8">
         <v>0</v>
       </c>
-      <c r="AG8" s="19">
+      <c r="AG8" s="12">
         <v>0</v>
       </c>
       <c r="AH8">
         <v>1</v>
       </c>
-      <c r="AI8" s="19">
+      <c r="AI8" s="12">
         <v>0</v>
       </c>
       <c r="AJ8">
@@ -1792,7 +1792,7 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="12">
         <v>0</v>
       </c>
       <c r="J9">
@@ -1807,7 +1807,7 @@
       <c r="M9">
         <v>1</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="12">
         <v>0</v>
       </c>
       <c r="O9">
@@ -1822,7 +1822,7 @@
       <c r="R9">
         <v>1</v>
       </c>
-      <c r="S9" s="19">
+      <c r="S9" s="12">
         <v>0</v>
       </c>
       <c r="T9">
@@ -1840,7 +1840,7 @@
       <c r="X9">
         <v>0</v>
       </c>
-      <c r="Y9" s="19">
+      <c r="Y9" s="12">
         <v>0</v>
       </c>
       <c r="Z9" s="1">
@@ -1852,25 +1852,25 @@
       <c r="AB9" s="1">
         <v>1</v>
       </c>
-      <c r="AC9" s="24">
+      <c r="AC9" s="17">
         <v>0</v>
       </c>
       <c r="AD9">
         <v>1</v>
       </c>
-      <c r="AE9" s="19">
+      <c r="AE9" s="12">
         <v>0</v>
       </c>
       <c r="AF9">
         <v>1</v>
       </c>
-      <c r="AG9" s="19">
+      <c r="AG9" s="12">
         <v>0</v>
       </c>
       <c r="AH9">
         <v>1</v>
       </c>
-      <c r="AI9" s="19">
+      <c r="AI9" s="12">
         <v>0</v>
       </c>
       <c r="AJ9">
@@ -1906,7 +1906,7 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="12">
         <v>0</v>
       </c>
       <c r="J10">
@@ -1921,7 +1921,7 @@
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="12">
         <v>0</v>
       </c>
       <c r="O10">
@@ -1936,7 +1936,7 @@
       <c r="R10">
         <v>0</v>
       </c>
-      <c r="S10" s="19">
+      <c r="S10" s="12">
         <v>0</v>
       </c>
       <c r="T10">
@@ -1954,7 +1954,7 @@
       <c r="X10">
         <v>0</v>
       </c>
-      <c r="Y10" s="19">
+      <c r="Y10" s="12">
         <v>0</v>
       </c>
       <c r="Z10" s="1">
@@ -1966,25 +1966,25 @@
       <c r="AB10" s="1">
         <v>1</v>
       </c>
-      <c r="AC10" s="24">
+      <c r="AC10" s="17">
         <v>1</v>
       </c>
       <c r="AD10">
         <v>0</v>
       </c>
-      <c r="AE10" s="19">
+      <c r="AE10" s="12">
         <v>0</v>
       </c>
       <c r="AF10">
         <v>0</v>
       </c>
-      <c r="AG10" s="19">
+      <c r="AG10" s="12">
         <v>0</v>
       </c>
       <c r="AH10">
         <v>1</v>
       </c>
-      <c r="AI10" s="19">
+      <c r="AI10" s="12">
         <v>0</v>
       </c>
       <c r="AJ10">
@@ -2020,7 +2020,7 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="12">
         <v>1</v>
       </c>
       <c r="J11">
@@ -2035,7 +2035,7 @@
       <c r="M11">
         <v>1</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="12">
         <v>1</v>
       </c>
       <c r="O11">
@@ -2050,7 +2050,7 @@
       <c r="R11">
         <v>1</v>
       </c>
-      <c r="S11" s="19">
+      <c r="S11" s="12">
         <v>1</v>
       </c>
       <c r="T11">
@@ -2068,7 +2068,7 @@
       <c r="X11">
         <v>1</v>
       </c>
-      <c r="Y11" s="19">
+      <c r="Y11" s="12">
         <v>0</v>
       </c>
       <c r="Z11" s="1">
@@ -2080,25 +2080,25 @@
       <c r="AB11" s="1">
         <v>1</v>
       </c>
-      <c r="AC11" s="24">
+      <c r="AC11" s="17">
         <v>1</v>
       </c>
       <c r="AD11">
         <v>1</v>
       </c>
-      <c r="AE11" s="19">
+      <c r="AE11" s="12">
         <v>1</v>
       </c>
       <c r="AF11">
         <v>1</v>
       </c>
-      <c r="AG11" s="19">
+      <c r="AG11" s="12">
         <v>1</v>
       </c>
       <c r="AH11">
         <v>1</v>
       </c>
-      <c r="AI11" s="19">
+      <c r="AI11" s="12">
         <v>1</v>
       </c>
       <c r="AJ11">
@@ -2134,7 +2134,7 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="12">
         <v>0</v>
       </c>
       <c r="J12">
@@ -2149,7 +2149,7 @@
       <c r="M12">
         <v>1</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="12">
         <v>0</v>
       </c>
       <c r="O12">
@@ -2164,7 +2164,7 @@
       <c r="R12">
         <v>1</v>
       </c>
-      <c r="S12" s="19">
+      <c r="S12" s="12">
         <v>0</v>
       </c>
       <c r="T12">
@@ -2182,7 +2182,7 @@
       <c r="X12">
         <v>0</v>
       </c>
-      <c r="Y12" s="19">
+      <c r="Y12" s="12">
         <v>0</v>
       </c>
       <c r="Z12" s="1">
@@ -2194,25 +2194,25 @@
       <c r="AB12" s="1">
         <v>1</v>
       </c>
-      <c r="AC12" s="24">
+      <c r="AC12" s="17">
         <v>1</v>
       </c>
       <c r="AD12">
         <v>0</v>
       </c>
-      <c r="AE12" s="19">
+      <c r="AE12" s="12">
         <v>0</v>
       </c>
       <c r="AF12">
         <v>0</v>
       </c>
-      <c r="AG12" s="19">
+      <c r="AG12" s="12">
         <v>0</v>
       </c>
       <c r="AH12">
         <v>1</v>
       </c>
-      <c r="AI12" s="19">
+      <c r="AI12" s="12">
         <v>0</v>
       </c>
       <c r="AJ12">
@@ -2248,7 +2248,7 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="12">
         <v>0</v>
       </c>
       <c r="J13">
@@ -2263,7 +2263,7 @@
       <c r="M13">
         <v>0</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13" s="12">
         <v>0</v>
       </c>
       <c r="O13">
@@ -2278,7 +2278,7 @@
       <c r="R13">
         <v>1</v>
       </c>
-      <c r="S13" s="19">
+      <c r="S13" s="12">
         <v>0</v>
       </c>
       <c r="T13">
@@ -2296,7 +2296,7 @@
       <c r="X13">
         <v>0</v>
       </c>
-      <c r="Y13" s="19">
+      <c r="Y13" s="12">
         <v>0</v>
       </c>
       <c r="Z13" s="1">
@@ -2308,25 +2308,25 @@
       <c r="AB13" s="1">
         <v>1</v>
       </c>
-      <c r="AC13" s="24">
+      <c r="AC13" s="17">
         <v>0</v>
       </c>
       <c r="AD13">
         <v>0</v>
       </c>
-      <c r="AE13" s="19">
+      <c r="AE13" s="12">
         <v>0</v>
       </c>
       <c r="AF13">
         <v>0</v>
       </c>
-      <c r="AG13" s="19">
+      <c r="AG13" s="12">
         <v>0</v>
       </c>
       <c r="AH13">
         <v>1</v>
       </c>
-      <c r="AI13" s="19">
+      <c r="AI13" s="12">
         <v>1</v>
       </c>
       <c r="AJ13">
@@ -2362,7 +2362,7 @@
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="12">
         <v>0</v>
       </c>
       <c r="J14">
@@ -2377,7 +2377,7 @@
       <c r="M14">
         <v>0</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="12">
         <v>0</v>
       </c>
       <c r="O14">
@@ -2392,7 +2392,7 @@
       <c r="R14">
         <v>0</v>
       </c>
-      <c r="S14" s="19">
+      <c r="S14" s="12">
         <v>0</v>
       </c>
       <c r="T14">
@@ -2410,7 +2410,7 @@
       <c r="X14">
         <v>0</v>
       </c>
-      <c r="Y14" s="19">
+      <c r="Y14" s="12">
         <v>0</v>
       </c>
       <c r="Z14" s="1">
@@ -2422,25 +2422,25 @@
       <c r="AB14" s="1">
         <v>1</v>
       </c>
-      <c r="AC14" s="24">
+      <c r="AC14" s="17">
         <v>0</v>
       </c>
       <c r="AD14">
         <v>0</v>
       </c>
-      <c r="AE14" s="19">
+      <c r="AE14" s="12">
         <v>1</v>
       </c>
       <c r="AF14">
         <v>0</v>
       </c>
-      <c r="AG14" s="19">
+      <c r="AG14" s="12">
         <v>1</v>
       </c>
       <c r="AH14">
         <v>0</v>
       </c>
-      <c r="AI14" s="19">
+      <c r="AI14" s="12">
         <v>1</v>
       </c>
       <c r="AJ14">
@@ -2476,7 +2476,7 @@
       <c r="H15">
         <v>0</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="12">
         <v>0</v>
       </c>
       <c r="J15">
@@ -2491,7 +2491,7 @@
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="N15" s="19">
+      <c r="N15" s="12">
         <v>0</v>
       </c>
       <c r="O15">
@@ -2506,7 +2506,7 @@
       <c r="R15">
         <v>0</v>
       </c>
-      <c r="S15" s="19">
+      <c r="S15" s="12">
         <v>0</v>
       </c>
       <c r="T15">
@@ -2524,7 +2524,7 @@
       <c r="X15">
         <v>0</v>
       </c>
-      <c r="Y15" s="19">
+      <c r="Y15" s="12">
         <v>0</v>
       </c>
       <c r="Z15" s="1">
@@ -2536,25 +2536,25 @@
       <c r="AB15" s="1">
         <v>1</v>
       </c>
-      <c r="AC15" s="24">
+      <c r="AC15" s="17">
         <v>0</v>
       </c>
       <c r="AD15">
         <v>1</v>
       </c>
-      <c r="AE15" s="19">
+      <c r="AE15" s="12">
         <v>1</v>
       </c>
       <c r="AF15">
         <v>1</v>
       </c>
-      <c r="AG15" s="19">
+      <c r="AG15" s="12">
         <v>1</v>
       </c>
       <c r="AH15">
         <v>1</v>
       </c>
-      <c r="AI15" s="19">
+      <c r="AI15" s="12">
         <v>1</v>
       </c>
       <c r="AJ15">
@@ -2590,7 +2590,7 @@
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="12">
         <v>0</v>
       </c>
       <c r="J16">
@@ -2605,7 +2605,7 @@
       <c r="M16">
         <v>0</v>
       </c>
-      <c r="N16" s="19">
+      <c r="N16" s="12">
         <v>0</v>
       </c>
       <c r="O16">
@@ -2620,7 +2620,7 @@
       <c r="R16">
         <v>0</v>
       </c>
-      <c r="S16" s="19">
+      <c r="S16" s="12">
         <v>0</v>
       </c>
       <c r="T16">
@@ -2638,7 +2638,7 @@
       <c r="X16">
         <v>0</v>
       </c>
-      <c r="Y16" s="19">
+      <c r="Y16" s="12">
         <v>0</v>
       </c>
       <c r="Z16" s="1">
@@ -2650,25 +2650,25 @@
       <c r="AB16" s="1">
         <v>1</v>
       </c>
-      <c r="AC16" s="24">
+      <c r="AC16" s="17">
         <v>1</v>
       </c>
       <c r="AD16">
         <v>0</v>
       </c>
-      <c r="AE16" s="19">
+      <c r="AE16" s="12">
         <v>0</v>
       </c>
       <c r="AF16">
         <v>0</v>
       </c>
-      <c r="AG16" s="19">
+      <c r="AG16" s="12">
         <v>0</v>
       </c>
       <c r="AH16">
         <v>1</v>
       </c>
-      <c r="AI16" s="19">
+      <c r="AI16" s="12">
         <v>0</v>
       </c>
       <c r="AJ16">
@@ -2704,7 +2704,7 @@
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="12">
         <v>0</v>
       </c>
       <c r="J17">
@@ -2719,7 +2719,7 @@
       <c r="M17">
         <v>1</v>
       </c>
-      <c r="N17" s="19">
+      <c r="N17" s="12">
         <v>0</v>
       </c>
       <c r="O17">
@@ -2734,7 +2734,7 @@
       <c r="R17">
         <v>1</v>
       </c>
-      <c r="S17" s="19">
+      <c r="S17" s="12">
         <v>0</v>
       </c>
       <c r="T17">
@@ -2752,7 +2752,7 @@
       <c r="X17">
         <v>0</v>
       </c>
-      <c r="Y17" s="19">
+      <c r="Y17" s="12">
         <v>0</v>
       </c>
       <c r="Z17" s="1">
@@ -2764,25 +2764,25 @@
       <c r="AB17" s="1">
         <v>1</v>
       </c>
-      <c r="AC17" s="24">
+      <c r="AC17" s="17">
         <v>0</v>
       </c>
       <c r="AD17">
         <v>0</v>
       </c>
-      <c r="AE17" s="19">
+      <c r="AE17" s="12">
         <v>0</v>
       </c>
       <c r="AF17">
         <v>0</v>
       </c>
-      <c r="AG17" s="19">
+      <c r="AG17" s="12">
         <v>0</v>
       </c>
       <c r="AH17">
         <v>0</v>
       </c>
-      <c r="AI17" s="19">
+      <c r="AI17" s="12">
         <v>0</v>
       </c>
       <c r="AJ17">
@@ -2818,7 +2818,7 @@
       <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="12">
         <v>0</v>
       </c>
       <c r="J18">
@@ -2833,7 +2833,7 @@
       <c r="M18">
         <v>1</v>
       </c>
-      <c r="N18" s="19">
+      <c r="N18" s="12">
         <v>0</v>
       </c>
       <c r="O18">
@@ -2848,7 +2848,7 @@
       <c r="R18">
         <v>1</v>
       </c>
-      <c r="S18" s="19">
+      <c r="S18" s="12">
         <v>0</v>
       </c>
       <c r="T18">
@@ -2866,7 +2866,7 @@
       <c r="X18">
         <v>0</v>
       </c>
-      <c r="Y18" s="19">
+      <c r="Y18" s="12">
         <v>0</v>
       </c>
       <c r="Z18" s="1">
@@ -2878,25 +2878,25 @@
       <c r="AB18" s="1">
         <v>1</v>
       </c>
-      <c r="AC18" s="24">
+      <c r="AC18" s="17">
         <v>0</v>
       </c>
       <c r="AD18">
         <v>1</v>
       </c>
-      <c r="AE18" s="19">
+      <c r="AE18" s="12">
         <v>1</v>
       </c>
       <c r="AF18">
         <v>1</v>
       </c>
-      <c r="AG18" s="19">
+      <c r="AG18" s="12">
         <v>1</v>
       </c>
       <c r="AH18">
         <v>1</v>
       </c>
-      <c r="AI18" s="19">
+      <c r="AI18" s="12">
         <v>1</v>
       </c>
       <c r="AJ18">
@@ -2932,7 +2932,7 @@
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="12">
         <v>0</v>
       </c>
       <c r="J19">
@@ -2947,7 +2947,7 @@
       <c r="M19">
         <v>0</v>
       </c>
-      <c r="N19" s="19">
+      <c r="N19" s="12">
         <v>0</v>
       </c>
       <c r="O19">
@@ -2962,7 +2962,7 @@
       <c r="R19">
         <v>0</v>
       </c>
-      <c r="S19" s="19">
+      <c r="S19" s="12">
         <v>0</v>
       </c>
       <c r="T19">
@@ -2980,7 +2980,7 @@
       <c r="X19">
         <v>0</v>
       </c>
-      <c r="Y19" s="19">
+      <c r="Y19" s="12">
         <v>0</v>
       </c>
       <c r="Z19" s="1">
@@ -2992,25 +2992,25 @@
       <c r="AB19" s="1">
         <v>1</v>
       </c>
-      <c r="AC19" s="24">
+      <c r="AC19" s="17">
         <v>1</v>
       </c>
       <c r="AD19">
         <v>0</v>
       </c>
-      <c r="AE19" s="19">
+      <c r="AE19" s="12">
         <v>0</v>
       </c>
       <c r="AF19">
         <v>0</v>
       </c>
-      <c r="AG19" s="19">
+      <c r="AG19" s="12">
         <v>0</v>
       </c>
       <c r="AH19">
         <v>0</v>
       </c>
-      <c r="AI19" s="19">
+      <c r="AI19" s="12">
         <v>0</v>
       </c>
       <c r="AJ19">
@@ -3046,7 +3046,7 @@
       <c r="H20">
         <v>0</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="12">
         <v>0</v>
       </c>
       <c r="J20">
@@ -3061,7 +3061,7 @@
       <c r="M20">
         <v>0</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="12">
         <v>0</v>
       </c>
       <c r="O20">
@@ -3076,7 +3076,7 @@
       <c r="R20">
         <v>0</v>
       </c>
-      <c r="S20" s="19">
+      <c r="S20" s="12">
         <v>0</v>
       </c>
       <c r="T20">
@@ -3094,7 +3094,7 @@
       <c r="X20">
         <v>0</v>
       </c>
-      <c r="Y20" s="19">
+      <c r="Y20" s="12">
         <v>0</v>
       </c>
       <c r="Z20" s="1">
@@ -3106,25 +3106,25 @@
       <c r="AB20" s="1">
         <v>1</v>
       </c>
-      <c r="AC20" s="24">
+      <c r="AC20" s="17">
         <v>1</v>
       </c>
       <c r="AD20">
         <v>0</v>
       </c>
-      <c r="AE20" s="19">
+      <c r="AE20" s="12">
         <v>0</v>
       </c>
       <c r="AF20">
         <v>0</v>
       </c>
-      <c r="AG20" s="19">
+      <c r="AG20" s="12">
         <v>0</v>
       </c>
       <c r="AH20">
         <v>1</v>
       </c>
-      <c r="AI20" s="19">
+      <c r="AI20" s="12">
         <v>0</v>
       </c>
       <c r="AJ20">
@@ -3160,7 +3160,7 @@
       <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="12">
         <v>0</v>
       </c>
       <c r="J21">
@@ -3175,7 +3175,7 @@
       <c r="M21">
         <v>1</v>
       </c>
-      <c r="N21" s="19">
+      <c r="N21" s="12">
         <v>0</v>
       </c>
       <c r="O21">
@@ -3190,7 +3190,7 @@
       <c r="R21">
         <v>1</v>
       </c>
-      <c r="S21" s="19">
+      <c r="S21" s="12">
         <v>0</v>
       </c>
       <c r="T21">
@@ -3208,7 +3208,7 @@
       <c r="X21">
         <v>0</v>
       </c>
-      <c r="Y21" s="19">
+      <c r="Y21" s="12">
         <v>0</v>
       </c>
       <c r="Z21" s="1">
@@ -3220,25 +3220,25 @@
       <c r="AB21" s="1">
         <v>1</v>
       </c>
-      <c r="AC21" s="24">
+      <c r="AC21" s="17">
         <v>1</v>
       </c>
       <c r="AD21">
         <v>1</v>
       </c>
-      <c r="AE21" s="19">
+      <c r="AE21" s="12">
         <v>1</v>
       </c>
       <c r="AF21">
         <v>1</v>
       </c>
-      <c r="AG21" s="19">
+      <c r="AG21" s="12">
         <v>1</v>
       </c>
       <c r="AH21">
         <v>1</v>
       </c>
-      <c r="AI21" s="19">
+      <c r="AI21" s="12">
         <v>1</v>
       </c>
       <c r="AJ21">
@@ -3274,7 +3274,7 @@
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="12">
         <v>1</v>
       </c>
       <c r="J22">
@@ -3289,7 +3289,7 @@
       <c r="M22">
         <v>1</v>
       </c>
-      <c r="N22" s="19">
+      <c r="N22" s="12">
         <v>1</v>
       </c>
       <c r="O22">
@@ -3304,7 +3304,7 @@
       <c r="R22">
         <v>1</v>
       </c>
-      <c r="S22" s="19">
+      <c r="S22" s="12">
         <v>1</v>
       </c>
       <c r="T22">
@@ -3322,7 +3322,7 @@
       <c r="X22">
         <v>0</v>
       </c>
-      <c r="Y22" s="19">
+      <c r="Y22" s="12">
         <v>0</v>
       </c>
       <c r="Z22" s="1">
@@ -3334,25 +3334,25 @@
       <c r="AB22" s="1">
         <v>1</v>
       </c>
-      <c r="AC22" s="24">
+      <c r="AC22" s="17">
         <v>0</v>
       </c>
       <c r="AD22">
         <v>0</v>
       </c>
-      <c r="AE22" s="19">
+      <c r="AE22" s="12">
         <v>0</v>
       </c>
       <c r="AF22">
         <v>1</v>
       </c>
-      <c r="AG22" s="19">
+      <c r="AG22" s="12">
         <v>0</v>
       </c>
       <c r="AH22">
         <v>1</v>
       </c>
-      <c r="AI22" s="19">
+      <c r="AI22" s="12">
         <v>0</v>
       </c>
       <c r="AJ22">
@@ -3388,7 +3388,7 @@
       <c r="H23">
         <v>1</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="12">
         <v>0</v>
       </c>
       <c r="J23">
@@ -3403,7 +3403,7 @@
       <c r="M23">
         <v>1</v>
       </c>
-      <c r="N23" s="19">
+      <c r="N23" s="12">
         <v>0</v>
       </c>
       <c r="O23">
@@ -3418,7 +3418,7 @@
       <c r="R23">
         <v>1</v>
       </c>
-      <c r="S23" s="19">
+      <c r="S23" s="12">
         <v>0</v>
       </c>
       <c r="T23">
@@ -3436,7 +3436,7 @@
       <c r="X23">
         <v>0</v>
       </c>
-      <c r="Y23" s="19">
+      <c r="Y23" s="12">
         <v>0</v>
       </c>
       <c r="Z23" s="1">
@@ -3448,25 +3448,25 @@
       <c r="AB23" s="1">
         <v>1</v>
       </c>
-      <c r="AC23" s="24">
+      <c r="AC23" s="17">
         <v>0</v>
       </c>
       <c r="AD23">
         <v>1</v>
       </c>
-      <c r="AE23" s="19">
+      <c r="AE23" s="12">
         <v>0</v>
       </c>
       <c r="AF23">
         <v>1</v>
       </c>
-      <c r="AG23" s="19">
+      <c r="AG23" s="12">
         <v>0</v>
       </c>
       <c r="AH23">
         <v>1</v>
       </c>
-      <c r="AI23" s="19">
+      <c r="AI23" s="12">
         <v>0</v>
       </c>
       <c r="AJ23">
@@ -3502,7 +3502,7 @@
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="I24" s="19">
+      <c r="I24" s="12">
         <v>0</v>
       </c>
       <c r="J24">
@@ -3517,7 +3517,7 @@
       <c r="M24">
         <v>0</v>
       </c>
-      <c r="N24" s="19">
+      <c r="N24" s="12">
         <v>0</v>
       </c>
       <c r="O24">
@@ -3532,7 +3532,7 @@
       <c r="R24">
         <v>0</v>
       </c>
-      <c r="S24" s="19">
+      <c r="S24" s="12">
         <v>0</v>
       </c>
       <c r="T24">
@@ -3550,7 +3550,7 @@
       <c r="X24">
         <v>0</v>
       </c>
-      <c r="Y24" s="19">
+      <c r="Y24" s="12">
         <v>0</v>
       </c>
       <c r="Z24" s="1">
@@ -3562,25 +3562,25 @@
       <c r="AB24" s="1">
         <v>1</v>
       </c>
-      <c r="AC24" s="24">
+      <c r="AC24" s="17">
         <v>1</v>
       </c>
       <c r="AD24">
         <v>0</v>
       </c>
-      <c r="AE24" s="19">
+      <c r="AE24" s="12">
         <v>0</v>
       </c>
       <c r="AF24">
         <v>0</v>
       </c>
-      <c r="AG24" s="19">
+      <c r="AG24" s="12">
         <v>0</v>
       </c>
       <c r="AH24">
         <v>1</v>
       </c>
-      <c r="AI24" s="19">
+      <c r="AI24" s="12">
         <v>0</v>
       </c>
       <c r="AJ24">
@@ -3616,7 +3616,7 @@
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="I25" s="19">
+      <c r="I25" s="12">
         <v>0</v>
       </c>
       <c r="J25">
@@ -3631,7 +3631,7 @@
       <c r="M25">
         <v>0</v>
       </c>
-      <c r="N25" s="19">
+      <c r="N25" s="12">
         <v>0</v>
       </c>
       <c r="O25">
@@ -3646,7 +3646,7 @@
       <c r="R25">
         <v>0</v>
       </c>
-      <c r="S25" s="19">
+      <c r="S25" s="12">
         <v>0</v>
       </c>
       <c r="T25">
@@ -3664,7 +3664,7 @@
       <c r="X25">
         <v>0</v>
       </c>
-      <c r="Y25" s="19">
+      <c r="Y25" s="12">
         <v>0</v>
       </c>
       <c r="Z25" s="1">
@@ -3676,25 +3676,25 @@
       <c r="AB25" s="1">
         <v>1</v>
       </c>
-      <c r="AC25" s="24">
+      <c r="AC25" s="17">
         <v>1</v>
       </c>
       <c r="AD25">
         <v>0</v>
       </c>
-      <c r="AE25" s="19">
+      <c r="AE25" s="12">
         <v>0</v>
       </c>
       <c r="AF25">
         <v>0</v>
       </c>
-      <c r="AG25" s="19">
+      <c r="AG25" s="12">
         <v>0</v>
       </c>
       <c r="AH25">
         <v>0</v>
       </c>
-      <c r="AI25" s="19">
+      <c r="AI25" s="12">
         <v>0</v>
       </c>
       <c r="AJ25">
@@ -3730,7 +3730,7 @@
       <c r="H26">
         <v>1</v>
       </c>
-      <c r="I26" s="19">
+      <c r="I26" s="12">
         <v>0</v>
       </c>
       <c r="J26">
@@ -3745,7 +3745,7 @@
       <c r="M26">
         <v>1</v>
       </c>
-      <c r="N26" s="19">
+      <c r="N26" s="12">
         <v>0</v>
       </c>
       <c r="O26">
@@ -3760,7 +3760,7 @@
       <c r="R26">
         <v>1</v>
       </c>
-      <c r="S26" s="19">
+      <c r="S26" s="12">
         <v>0</v>
       </c>
       <c r="T26">
@@ -3778,7 +3778,7 @@
       <c r="X26">
         <v>0</v>
       </c>
-      <c r="Y26" s="19">
+      <c r="Y26" s="12">
         <v>0</v>
       </c>
       <c r="Z26" s="1">
@@ -3790,25 +3790,25 @@
       <c r="AB26" s="1">
         <v>1</v>
       </c>
-      <c r="AC26" s="24">
+      <c r="AC26" s="17">
         <v>0</v>
       </c>
       <c r="AD26">
         <v>0</v>
       </c>
-      <c r="AE26" s="19">
+      <c r="AE26" s="12">
         <v>0</v>
       </c>
       <c r="AF26">
         <v>0</v>
       </c>
-      <c r="AG26" s="19">
+      <c r="AG26" s="12">
         <v>0</v>
       </c>
       <c r="AH26">
         <v>1</v>
       </c>
-      <c r="AI26" s="19">
+      <c r="AI26" s="12">
         <v>0</v>
       </c>
       <c r="AJ26">
@@ -3844,7 +3844,7 @@
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="I27" s="19">
+      <c r="I27" s="12">
         <v>0</v>
       </c>
       <c r="J27">
@@ -3859,7 +3859,7 @@
       <c r="M27">
         <v>0</v>
       </c>
-      <c r="N27" s="19">
+      <c r="N27" s="12">
         <v>0</v>
       </c>
       <c r="O27">
@@ -3874,7 +3874,7 @@
       <c r="R27">
         <v>0</v>
       </c>
-      <c r="S27" s="19">
+      <c r="S27" s="12">
         <v>0</v>
       </c>
       <c r="T27">
@@ -3892,7 +3892,7 @@
       <c r="X27">
         <v>0</v>
       </c>
-      <c r="Y27" s="19">
+      <c r="Y27" s="12">
         <v>0</v>
       </c>
       <c r="Z27" s="1">
@@ -3904,25 +3904,25 @@
       <c r="AB27" s="1">
         <v>1</v>
       </c>
-      <c r="AC27" s="24">
+      <c r="AC27" s="17">
         <v>1</v>
       </c>
       <c r="AD27">
         <v>0</v>
       </c>
-      <c r="AE27" s="19">
+      <c r="AE27" s="12">
         <v>0</v>
       </c>
       <c r="AF27">
         <v>0</v>
       </c>
-      <c r="AG27" s="19">
+      <c r="AG27" s="12">
         <v>0</v>
       </c>
       <c r="AH27">
         <v>1</v>
       </c>
-      <c r="AI27" s="19">
+      <c r="AI27" s="12">
         <v>0</v>
       </c>
       <c r="AJ27">
@@ -3958,7 +3958,7 @@
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="I28" s="19">
+      <c r="I28" s="12">
         <v>0</v>
       </c>
       <c r="J28">
@@ -3973,7 +3973,7 @@
       <c r="M28">
         <v>0</v>
       </c>
-      <c r="N28" s="19">
+      <c r="N28" s="12">
         <v>0</v>
       </c>
       <c r="O28">
@@ -3988,7 +3988,7 @@
       <c r="R28">
         <v>0</v>
       </c>
-      <c r="S28" s="19">
+      <c r="S28" s="12">
         <v>0</v>
       </c>
       <c r="T28">
@@ -4006,7 +4006,7 @@
       <c r="X28">
         <v>0</v>
       </c>
-      <c r="Y28" s="19">
+      <c r="Y28" s="12">
         <v>0</v>
       </c>
       <c r="Z28" s="1">
@@ -4018,25 +4018,25 @@
       <c r="AB28" s="1">
         <v>1</v>
       </c>
-      <c r="AC28" s="24">
+      <c r="AC28" s="17">
         <v>1</v>
       </c>
       <c r="AD28">
         <v>0</v>
       </c>
-      <c r="AE28" s="19">
+      <c r="AE28" s="12">
         <v>0</v>
       </c>
       <c r="AF28">
         <v>0</v>
       </c>
-      <c r="AG28" s="19">
+      <c r="AG28" s="12">
         <v>0</v>
       </c>
       <c r="AH28">
         <v>1</v>
       </c>
-      <c r="AI28" s="19">
+      <c r="AI28" s="12">
         <v>0</v>
       </c>
       <c r="AJ28">
@@ -4072,7 +4072,7 @@
       <c r="H29">
         <v>0</v>
       </c>
-      <c r="I29" s="19">
+      <c r="I29" s="12">
         <v>0</v>
       </c>
       <c r="J29">
@@ -4087,7 +4087,7 @@
       <c r="M29">
         <v>0</v>
       </c>
-      <c r="N29" s="19">
+      <c r="N29" s="12">
         <v>0</v>
       </c>
       <c r="O29">
@@ -4102,7 +4102,7 @@
       <c r="R29">
         <v>0</v>
       </c>
-      <c r="S29" s="19">
+      <c r="S29" s="12">
         <v>0</v>
       </c>
       <c r="T29">
@@ -4120,7 +4120,7 @@
       <c r="X29">
         <v>0</v>
       </c>
-      <c r="Y29" s="19">
+      <c r="Y29" s="12">
         <v>0</v>
       </c>
       <c r="Z29" s="1">
@@ -4132,25 +4132,25 @@
       <c r="AB29" s="1">
         <v>1</v>
       </c>
-      <c r="AC29" s="24">
+      <c r="AC29" s="17">
         <v>1</v>
       </c>
       <c r="AD29">
         <v>0</v>
       </c>
-      <c r="AE29" s="19">
+      <c r="AE29" s="12">
         <v>0</v>
       </c>
       <c r="AF29">
         <v>0</v>
       </c>
-      <c r="AG29" s="19">
+      <c r="AG29" s="12">
         <v>0</v>
       </c>
       <c r="AH29">
         <v>1</v>
       </c>
-      <c r="AI29" s="19">
+      <c r="AI29" s="12">
         <v>0</v>
       </c>
       <c r="AJ29">
@@ -4186,7 +4186,7 @@
       <c r="H30">
         <v>0</v>
       </c>
-      <c r="I30" s="19">
+      <c r="I30" s="12">
         <v>0</v>
       </c>
       <c r="J30">
@@ -4201,7 +4201,7 @@
       <c r="M30">
         <v>0</v>
       </c>
-      <c r="N30" s="19">
+      <c r="N30" s="12">
         <v>0</v>
       </c>
       <c r="O30">
@@ -4216,7 +4216,7 @@
       <c r="R30">
         <v>0</v>
       </c>
-      <c r="S30" s="19">
+      <c r="S30" s="12">
         <v>0</v>
       </c>
       <c r="T30">
@@ -4234,7 +4234,7 @@
       <c r="X30">
         <v>1</v>
       </c>
-      <c r="Y30" s="19">
+      <c r="Y30" s="12">
         <v>1</v>
       </c>
       <c r="Z30" s="1">
@@ -4246,25 +4246,25 @@
       <c r="AB30" s="1">
         <v>0</v>
       </c>
-      <c r="AC30" s="24">
+      <c r="AC30" s="17">
         <v>1</v>
       </c>
       <c r="AD30">
         <v>0</v>
       </c>
-      <c r="AE30" s="19">
+      <c r="AE30" s="12">
         <v>0</v>
       </c>
       <c r="AF30">
         <v>0</v>
       </c>
-      <c r="AG30" s="19">
+      <c r="AG30" s="12">
         <v>0</v>
       </c>
       <c r="AH30">
         <v>0</v>
       </c>
-      <c r="AI30" s="19">
+      <c r="AI30" s="12">
         <v>0</v>
       </c>
       <c r="AJ30">
@@ -4300,7 +4300,7 @@
       <c r="H31">
         <v>0</v>
       </c>
-      <c r="I31" s="19">
+      <c r="I31" s="12">
         <v>0</v>
       </c>
       <c r="J31">
@@ -4315,7 +4315,7 @@
       <c r="M31">
         <v>0</v>
       </c>
-      <c r="N31" s="19">
+      <c r="N31" s="12">
         <v>0</v>
       </c>
       <c r="O31">
@@ -4330,7 +4330,7 @@
       <c r="R31">
         <v>0</v>
       </c>
-      <c r="S31" s="19">
+      <c r="S31" s="12">
         <v>0</v>
       </c>
       <c r="T31">
@@ -4348,7 +4348,7 @@
       <c r="X31">
         <v>0</v>
       </c>
-      <c r="Y31" s="19">
+      <c r="Y31" s="12">
         <v>0</v>
       </c>
       <c r="Z31" s="1">
@@ -4360,25 +4360,25 @@
       <c r="AB31" s="1">
         <v>1</v>
       </c>
-      <c r="AC31" s="24">
+      <c r="AC31" s="17">
         <v>1</v>
       </c>
       <c r="AD31">
         <v>0</v>
       </c>
-      <c r="AE31" s="19">
+      <c r="AE31" s="12">
         <v>0</v>
       </c>
       <c r="AF31">
         <v>0</v>
       </c>
-      <c r="AG31" s="19">
+      <c r="AG31" s="12">
         <v>0</v>
       </c>
       <c r="AH31">
         <v>1</v>
       </c>
-      <c r="AI31" s="19">
+      <c r="AI31" s="12">
         <v>0</v>
       </c>
       <c r="AJ31">
@@ -4414,7 +4414,7 @@
       <c r="H32">
         <v>0</v>
       </c>
-      <c r="I32" s="19">
+      <c r="I32" s="12">
         <v>1</v>
       </c>
       <c r="J32">
@@ -4429,7 +4429,7 @@
       <c r="M32">
         <v>0</v>
       </c>
-      <c r="N32" s="19">
+      <c r="N32" s="12">
         <v>1</v>
       </c>
       <c r="O32">
@@ -4444,7 +4444,7 @@
       <c r="R32">
         <v>0</v>
       </c>
-      <c r="S32" s="19">
+      <c r="S32" s="12">
         <v>1</v>
       </c>
       <c r="T32">
@@ -4462,7 +4462,7 @@
       <c r="X32">
         <v>1</v>
       </c>
-      <c r="Y32" s="19">
+      <c r="Y32" s="12">
         <v>1</v>
       </c>
       <c r="Z32" s="1">
@@ -4474,25 +4474,25 @@
       <c r="AB32" s="1">
         <v>1</v>
       </c>
-      <c r="AC32" s="24">
+      <c r="AC32" s="17">
         <v>1</v>
       </c>
       <c r="AD32">
         <v>1</v>
       </c>
-      <c r="AE32" s="19">
+      <c r="AE32" s="12">
         <v>1</v>
       </c>
       <c r="AF32">
         <v>1</v>
       </c>
-      <c r="AG32" s="19">
+      <c r="AG32" s="12">
         <v>1</v>
       </c>
       <c r="AH32">
         <v>1</v>
       </c>
-      <c r="AI32" s="19">
+      <c r="AI32" s="12">
         <v>1</v>
       </c>
       <c r="AJ32">
@@ -4528,7 +4528,7 @@
       <c r="H33">
         <v>0</v>
       </c>
-      <c r="I33" s="19">
+      <c r="I33" s="12">
         <v>0</v>
       </c>
       <c r="J33">
@@ -4543,7 +4543,7 @@
       <c r="M33">
         <v>0</v>
       </c>
-      <c r="N33" s="19">
+      <c r="N33" s="12">
         <v>0</v>
       </c>
       <c r="O33">
@@ -4558,7 +4558,7 @@
       <c r="R33">
         <v>0</v>
       </c>
-      <c r="S33" s="19">
+      <c r="S33" s="12">
         <v>0</v>
       </c>
       <c r="T33">
@@ -4576,7 +4576,7 @@
       <c r="X33">
         <v>0</v>
       </c>
-      <c r="Y33" s="19">
+      <c r="Y33" s="12">
         <v>0</v>
       </c>
       <c r="Z33" s="1">
@@ -4588,25 +4588,25 @@
       <c r="AB33" s="1">
         <v>1</v>
       </c>
-      <c r="AC33" s="24">
+      <c r="AC33" s="17">
         <v>0</v>
       </c>
       <c r="AD33">
         <v>1</v>
       </c>
-      <c r="AE33" s="19">
+      <c r="AE33" s="12">
         <v>1</v>
       </c>
       <c r="AF33">
         <v>1</v>
       </c>
-      <c r="AG33" s="19">
+      <c r="AG33" s="12">
         <v>1</v>
       </c>
       <c r="AH33">
         <v>1</v>
       </c>
-      <c r="AI33" s="19">
+      <c r="AI33" s="12">
         <v>1</v>
       </c>
       <c r="AJ33">
@@ -4642,7 +4642,7 @@
       <c r="H34">
         <v>1</v>
       </c>
-      <c r="I34" s="19">
+      <c r="I34" s="12">
         <v>0</v>
       </c>
       <c r="J34">
@@ -4657,7 +4657,7 @@
       <c r="M34">
         <v>1</v>
       </c>
-      <c r="N34" s="19">
+      <c r="N34" s="12">
         <v>0</v>
       </c>
       <c r="O34">
@@ -4672,7 +4672,7 @@
       <c r="R34">
         <v>1</v>
       </c>
-      <c r="S34" s="19">
+      <c r="S34" s="12">
         <v>0</v>
       </c>
       <c r="T34">
@@ -4690,7 +4690,7 @@
       <c r="X34">
         <v>0</v>
       </c>
-      <c r="Y34" s="19">
+      <c r="Y34" s="12">
         <v>0</v>
       </c>
       <c r="Z34" s="1">
@@ -4702,25 +4702,25 @@
       <c r="AB34" s="1">
         <v>1</v>
       </c>
-      <c r="AC34" s="24">
+      <c r="AC34" s="17">
         <v>0</v>
       </c>
       <c r="AD34">
         <v>0</v>
       </c>
-      <c r="AE34" s="19">
+      <c r="AE34" s="12">
         <v>1</v>
       </c>
       <c r="AF34">
         <v>0</v>
       </c>
-      <c r="AG34" s="19">
+      <c r="AG34" s="12">
         <v>1</v>
       </c>
       <c r="AH34">
         <v>0</v>
       </c>
-      <c r="AI34" s="19">
+      <c r="AI34" s="12">
         <v>1</v>
       </c>
       <c r="AJ34">
@@ -4756,7 +4756,7 @@
       <c r="H35">
         <v>1</v>
       </c>
-      <c r="I35" s="19">
+      <c r="I35" s="12">
         <v>0</v>
       </c>
       <c r="J35">
@@ -4771,7 +4771,7 @@
       <c r="M35">
         <v>1</v>
       </c>
-      <c r="N35" s="19">
+      <c r="N35" s="12">
         <v>0</v>
       </c>
       <c r="O35">
@@ -4786,7 +4786,7 @@
       <c r="R35">
         <v>1</v>
       </c>
-      <c r="S35" s="19">
+      <c r="S35" s="12">
         <v>0</v>
       </c>
       <c r="T35">
@@ -4804,7 +4804,7 @@
       <c r="X35">
         <v>0</v>
       </c>
-      <c r="Y35" s="19">
+      <c r="Y35" s="12">
         <v>0</v>
       </c>
       <c r="Z35" s="1">
@@ -4816,25 +4816,25 @@
       <c r="AB35" s="1">
         <v>1</v>
       </c>
-      <c r="AC35" s="24">
+      <c r="AC35" s="17">
         <v>0</v>
       </c>
       <c r="AD35">
         <v>0</v>
       </c>
-      <c r="AE35" s="19">
+      <c r="AE35" s="12">
         <v>0</v>
       </c>
       <c r="AF35">
         <v>0</v>
       </c>
-      <c r="AG35" s="19">
+      <c r="AG35" s="12">
         <v>0</v>
       </c>
       <c r="AH35">
         <v>0</v>
       </c>
-      <c r="AI35" s="19">
+      <c r="AI35" s="12">
         <v>0</v>
       </c>
       <c r="AJ35">
@@ -4870,7 +4870,7 @@
       <c r="H36">
         <v>1</v>
       </c>
-      <c r="I36" s="19">
+      <c r="I36" s="12">
         <v>1</v>
       </c>
       <c r="J36">
@@ -4885,7 +4885,7 @@
       <c r="M36">
         <v>1</v>
       </c>
-      <c r="N36" s="19">
+      <c r="N36" s="12">
         <v>1</v>
       </c>
       <c r="O36">
@@ -4900,7 +4900,7 @@
       <c r="R36">
         <v>1</v>
       </c>
-      <c r="S36" s="19">
+      <c r="S36" s="12">
         <v>1</v>
       </c>
       <c r="T36">
@@ -4918,7 +4918,7 @@
       <c r="X36">
         <v>0</v>
       </c>
-      <c r="Y36" s="19">
+      <c r="Y36" s="12">
         <v>0</v>
       </c>
       <c r="Z36" s="1">
@@ -4930,25 +4930,25 @@
       <c r="AB36" s="1">
         <v>1</v>
       </c>
-      <c r="AC36" s="24">
+      <c r="AC36" s="17">
         <v>0</v>
       </c>
       <c r="AD36">
         <v>0</v>
       </c>
-      <c r="AE36" s="19">
+      <c r="AE36" s="12">
         <v>0</v>
       </c>
       <c r="AF36">
         <v>0</v>
       </c>
-      <c r="AG36" s="19">
+      <c r="AG36" s="12">
         <v>1</v>
       </c>
       <c r="AH36">
         <v>0</v>
       </c>
-      <c r="AI36" s="19">
+      <c r="AI36" s="12">
         <v>1</v>
       </c>
       <c r="AJ36">
@@ -4984,7 +4984,7 @@
       <c r="H37">
         <v>1</v>
       </c>
-      <c r="I37" s="19">
+      <c r="I37" s="12">
         <v>0</v>
       </c>
       <c r="J37">
@@ -4999,7 +4999,7 @@
       <c r="M37">
         <v>1</v>
       </c>
-      <c r="N37" s="19">
+      <c r="N37" s="12">
         <v>0</v>
       </c>
       <c r="O37">
@@ -5014,7 +5014,7 @@
       <c r="R37">
         <v>1</v>
       </c>
-      <c r="S37" s="19">
+      <c r="S37" s="12">
         <v>0</v>
       </c>
       <c r="T37">
@@ -5032,7 +5032,7 @@
       <c r="X37">
         <v>0</v>
       </c>
-      <c r="Y37" s="19">
+      <c r="Y37" s="12">
         <v>0</v>
       </c>
       <c r="Z37" s="1">
@@ -5044,25 +5044,25 @@
       <c r="AB37" s="1">
         <v>1</v>
       </c>
-      <c r="AC37" s="24">
+      <c r="AC37" s="17">
         <v>0</v>
       </c>
       <c r="AD37">
         <v>0</v>
       </c>
-      <c r="AE37" s="19">
+      <c r="AE37" s="12">
         <v>0</v>
       </c>
       <c r="AF37">
         <v>0</v>
       </c>
-      <c r="AG37" s="19">
+      <c r="AG37" s="12">
         <v>0</v>
       </c>
       <c r="AH37">
         <v>1</v>
       </c>
-      <c r="AI37" s="19">
+      <c r="AI37" s="12">
         <v>0</v>
       </c>
       <c r="AJ37">
@@ -5098,7 +5098,7 @@
       <c r="H38">
         <v>0</v>
       </c>
-      <c r="I38" s="19">
+      <c r="I38" s="12">
         <v>0</v>
       </c>
       <c r="J38">
@@ -5113,7 +5113,7 @@
       <c r="M38">
         <v>0</v>
       </c>
-      <c r="N38" s="19">
+      <c r="N38" s="12">
         <v>0</v>
       </c>
       <c r="O38">
@@ -5128,7 +5128,7 @@
       <c r="R38">
         <v>0</v>
       </c>
-      <c r="S38" s="19">
+      <c r="S38" s="12">
         <v>0</v>
       </c>
       <c r="T38">
@@ -5146,7 +5146,7 @@
       <c r="X38">
         <v>0</v>
       </c>
-      <c r="Y38" s="19">
+      <c r="Y38" s="12">
         <v>0</v>
       </c>
       <c r="Z38" s="1">
@@ -5158,25 +5158,25 @@
       <c r="AB38" s="1">
         <v>1</v>
       </c>
-      <c r="AC38" s="24">
+      <c r="AC38" s="17">
         <v>1</v>
       </c>
       <c r="AD38">
         <v>0</v>
       </c>
-      <c r="AE38" s="19">
+      <c r="AE38" s="12">
         <v>0</v>
       </c>
       <c r="AF38">
         <v>0</v>
       </c>
-      <c r="AG38" s="19">
+      <c r="AG38" s="12">
         <v>0</v>
       </c>
       <c r="AH38">
         <v>1</v>
       </c>
-      <c r="AI38" s="19">
+      <c r="AI38" s="12">
         <v>0</v>
       </c>
       <c r="AJ38">
@@ -5212,7 +5212,7 @@
       <c r="H39">
         <v>0</v>
       </c>
-      <c r="I39" s="19">
+      <c r="I39" s="12">
         <v>0</v>
       </c>
       <c r="J39">
@@ -5227,7 +5227,7 @@
       <c r="M39">
         <v>1</v>
       </c>
-      <c r="N39" s="19">
+      <c r="N39" s="12">
         <v>0</v>
       </c>
       <c r="O39">
@@ -5242,7 +5242,7 @@
       <c r="R39">
         <v>1</v>
       </c>
-      <c r="S39" s="19">
+      <c r="S39" s="12">
         <v>0</v>
       </c>
       <c r="T39">
@@ -5260,7 +5260,7 @@
       <c r="X39">
         <v>0</v>
       </c>
-      <c r="Y39" s="19">
+      <c r="Y39" s="12">
         <v>0</v>
       </c>
       <c r="Z39" s="1">
@@ -5272,25 +5272,25 @@
       <c r="AB39" s="1">
         <v>1</v>
       </c>
-      <c r="AC39" s="24">
+      <c r="AC39" s="17">
         <v>0</v>
       </c>
       <c r="AD39">
         <v>0</v>
       </c>
-      <c r="AE39" s="19">
+      <c r="AE39" s="12">
         <v>0</v>
       </c>
       <c r="AF39">
         <v>0</v>
       </c>
-      <c r="AG39" s="19">
+      <c r="AG39" s="12">
         <v>0</v>
       </c>
       <c r="AH39">
         <v>0</v>
       </c>
-      <c r="AI39" s="19">
+      <c r="AI39" s="12">
         <v>0</v>
       </c>
       <c r="AJ39">
@@ -5326,7 +5326,7 @@
       <c r="H40">
         <v>0</v>
       </c>
-      <c r="I40" s="19">
+      <c r="I40" s="12">
         <v>0</v>
       </c>
       <c r="J40">
@@ -5341,7 +5341,7 @@
       <c r="M40">
         <v>0</v>
       </c>
-      <c r="N40" s="19">
+      <c r="N40" s="12">
         <v>0</v>
       </c>
       <c r="O40">
@@ -5356,7 +5356,7 @@
       <c r="R40">
         <v>0</v>
       </c>
-      <c r="S40" s="19">
+      <c r="S40" s="12">
         <v>0</v>
       </c>
       <c r="T40">
@@ -5374,7 +5374,7 @@
       <c r="X40">
         <v>0</v>
       </c>
-      <c r="Y40" s="19">
+      <c r="Y40" s="12">
         <v>0</v>
       </c>
       <c r="Z40" s="1">
@@ -5386,25 +5386,25 @@
       <c r="AB40" s="1">
         <v>1</v>
       </c>
-      <c r="AC40" s="24">
+      <c r="AC40" s="17">
         <v>1</v>
       </c>
       <c r="AD40">
         <v>0</v>
       </c>
-      <c r="AE40" s="19">
+      <c r="AE40" s="12">
         <v>0</v>
       </c>
       <c r="AF40">
         <v>0</v>
       </c>
-      <c r="AG40" s="19">
+      <c r="AG40" s="12">
         <v>0</v>
       </c>
       <c r="AH40">
         <v>1</v>
       </c>
-      <c r="AI40" s="19">
+      <c r="AI40" s="12">
         <v>0</v>
       </c>
       <c r="AJ40">
@@ -5440,7 +5440,7 @@
       <c r="H41">
         <v>0</v>
       </c>
-      <c r="I41" s="19">
+      <c r="I41" s="12">
         <v>1</v>
       </c>
       <c r="J41">
@@ -5455,7 +5455,7 @@
       <c r="M41">
         <v>0</v>
       </c>
-      <c r="N41" s="19">
+      <c r="N41" s="12">
         <v>1</v>
       </c>
       <c r="O41">
@@ -5470,7 +5470,7 @@
       <c r="R41">
         <v>0</v>
       </c>
-      <c r="S41" s="19">
+      <c r="S41" s="12">
         <v>1</v>
       </c>
       <c r="T41">
@@ -5488,7 +5488,7 @@
       <c r="X41">
         <v>1</v>
       </c>
-      <c r="Y41" s="19">
+      <c r="Y41" s="12">
         <v>0</v>
       </c>
       <c r="Z41" s="1">
@@ -5500,25 +5500,25 @@
       <c r="AB41" s="1">
         <v>1</v>
       </c>
-      <c r="AC41" s="24">
+      <c r="AC41" s="17">
         <v>1</v>
       </c>
       <c r="AD41">
         <v>0</v>
       </c>
-      <c r="AE41" s="19">
+      <c r="AE41" s="12">
         <v>1</v>
       </c>
       <c r="AF41">
         <v>0</v>
       </c>
-      <c r="AG41" s="19">
+      <c r="AG41" s="12">
         <v>1</v>
       </c>
       <c r="AH41">
         <v>0</v>
       </c>
-      <c r="AI41" s="19">
+      <c r="AI41" s="12">
         <v>1</v>
       </c>
       <c r="AJ41">
@@ -5554,7 +5554,7 @@
       <c r="H42">
         <v>0</v>
       </c>
-      <c r="I42" s="19">
+      <c r="I42" s="12">
         <v>1</v>
       </c>
       <c r="J42">
@@ -5569,7 +5569,7 @@
       <c r="M42">
         <v>0</v>
       </c>
-      <c r="N42" s="19">
+      <c r="N42" s="12">
         <v>1</v>
       </c>
       <c r="O42">
@@ -5584,7 +5584,7 @@
       <c r="R42">
         <v>0</v>
       </c>
-      <c r="S42" s="19">
+      <c r="S42" s="12">
         <v>1</v>
       </c>
       <c r="T42">
@@ -5602,7 +5602,7 @@
       <c r="X42">
         <v>1</v>
       </c>
-      <c r="Y42" s="19">
+      <c r="Y42" s="12">
         <v>1</v>
       </c>
       <c r="Z42" s="1">
@@ -5614,25 +5614,25 @@
       <c r="AB42" s="1">
         <v>1</v>
       </c>
-      <c r="AC42" s="24">
+      <c r="AC42" s="17">
         <v>1</v>
       </c>
       <c r="AD42">
         <v>0</v>
       </c>
-      <c r="AE42" s="19">
+      <c r="AE42" s="12">
         <v>0</v>
       </c>
       <c r="AF42">
         <v>0</v>
       </c>
-      <c r="AG42" s="19">
+      <c r="AG42" s="12">
         <v>0</v>
       </c>
       <c r="AH42">
         <v>0</v>
       </c>
-      <c r="AI42" s="19">
+      <c r="AI42" s="12">
         <v>1</v>
       </c>
       <c r="AJ42">
@@ -5668,7 +5668,7 @@
       <c r="H43">
         <v>0</v>
       </c>
-      <c r="I43" s="19">
+      <c r="I43" s="12">
         <v>0</v>
       </c>
       <c r="J43">
@@ -5683,7 +5683,7 @@
       <c r="M43">
         <v>1</v>
       </c>
-      <c r="N43" s="19">
+      <c r="N43" s="12">
         <v>0</v>
       </c>
       <c r="O43">
@@ -5698,7 +5698,7 @@
       <c r="R43">
         <v>0</v>
       </c>
-      <c r="S43" s="19">
+      <c r="S43" s="12">
         <v>0</v>
       </c>
       <c r="T43">
@@ -5716,7 +5716,7 @@
       <c r="X43">
         <v>0</v>
       </c>
-      <c r="Y43" s="19">
+      <c r="Y43" s="12">
         <v>0</v>
       </c>
       <c r="Z43" s="1">
@@ -5728,25 +5728,25 @@
       <c r="AB43" s="1">
         <v>0</v>
       </c>
-      <c r="AC43" s="24">
+      <c r="AC43" s="17">
         <v>1</v>
       </c>
       <c r="AD43">
         <v>0</v>
       </c>
-      <c r="AE43" s="19">
+      <c r="AE43" s="12">
         <v>0</v>
       </c>
       <c r="AF43">
         <v>0</v>
       </c>
-      <c r="AG43" s="19">
+      <c r="AG43" s="12">
         <v>0</v>
       </c>
       <c r="AH43">
         <v>0</v>
       </c>
-      <c r="AI43" s="19">
+      <c r="AI43" s="12">
         <v>0</v>
       </c>
       <c r="AJ43">
@@ -5782,7 +5782,7 @@
       <c r="H44">
         <v>0</v>
       </c>
-      <c r="I44" s="19">
+      <c r="I44" s="12">
         <v>1</v>
       </c>
       <c r="J44">
@@ -5797,7 +5797,7 @@
       <c r="M44">
         <v>0</v>
       </c>
-      <c r="N44" s="19">
+      <c r="N44" s="12">
         <v>1</v>
       </c>
       <c r="O44">
@@ -5812,7 +5812,7 @@
       <c r="R44">
         <v>0</v>
       </c>
-      <c r="S44" s="19">
+      <c r="S44" s="12">
         <v>1</v>
       </c>
       <c r="T44">
@@ -5830,7 +5830,7 @@
       <c r="X44">
         <v>1</v>
       </c>
-      <c r="Y44" s="19">
+      <c r="Y44" s="12">
         <v>0</v>
       </c>
       <c r="Z44" s="1">
@@ -5842,25 +5842,25 @@
       <c r="AB44" s="1">
         <v>1</v>
       </c>
-      <c r="AC44" s="24">
+      <c r="AC44" s="17">
         <v>1</v>
       </c>
       <c r="AD44">
         <v>0</v>
       </c>
-      <c r="AE44" s="19">
+      <c r="AE44" s="12">
         <v>1</v>
       </c>
       <c r="AF44">
         <v>0</v>
       </c>
-      <c r="AG44" s="19">
+      <c r="AG44" s="12">
         <v>1</v>
       </c>
       <c r="AH44">
         <v>0</v>
       </c>
-      <c r="AI44" s="19">
+      <c r="AI44" s="12">
         <v>1</v>
       </c>
       <c r="AJ44">
@@ -5896,7 +5896,7 @@
       <c r="H45">
         <v>0</v>
       </c>
-      <c r="I45" s="19">
+      <c r="I45" s="12">
         <v>0</v>
       </c>
       <c r="J45">
@@ -5911,7 +5911,7 @@
       <c r="M45">
         <v>0</v>
       </c>
-      <c r="N45" s="19">
+      <c r="N45" s="12">
         <v>0</v>
       </c>
       <c r="O45">
@@ -5926,7 +5926,7 @@
       <c r="R45">
         <v>0</v>
       </c>
-      <c r="S45" s="19">
+      <c r="S45" s="12">
         <v>0</v>
       </c>
       <c r="T45">
@@ -5944,7 +5944,7 @@
       <c r="X45">
         <v>0</v>
       </c>
-      <c r="Y45" s="19">
+      <c r="Y45" s="12">
         <v>0</v>
       </c>
       <c r="Z45" s="1">
@@ -5956,25 +5956,25 @@
       <c r="AB45" s="1">
         <v>1</v>
       </c>
-      <c r="AC45" s="24">
+      <c r="AC45" s="17">
         <v>1</v>
       </c>
       <c r="AD45">
         <v>0</v>
       </c>
-      <c r="AE45" s="19">
+      <c r="AE45" s="12">
         <v>0</v>
       </c>
       <c r="AF45">
         <v>0</v>
       </c>
-      <c r="AG45" s="19">
+      <c r="AG45" s="12">
         <v>0</v>
       </c>
       <c r="AH45">
         <v>1</v>
       </c>
-      <c r="AI45" s="19">
+      <c r="AI45" s="12">
         <v>0</v>
       </c>
       <c r="AJ45">
@@ -6010,7 +6010,7 @@
       <c r="H46">
         <v>1</v>
       </c>
-      <c r="I46" s="19">
+      <c r="I46" s="12">
         <v>0</v>
       </c>
       <c r="J46">
@@ -6025,7 +6025,7 @@
       <c r="M46">
         <v>1</v>
       </c>
-      <c r="N46" s="19">
+      <c r="N46" s="12">
         <v>0</v>
       </c>
       <c r="O46">
@@ -6040,7 +6040,7 @@
       <c r="R46">
         <v>1</v>
       </c>
-      <c r="S46" s="19">
+      <c r="S46" s="12">
         <v>0</v>
       </c>
       <c r="T46">
@@ -6058,7 +6058,7 @@
       <c r="X46">
         <v>0</v>
       </c>
-      <c r="Y46" s="19">
+      <c r="Y46" s="12">
         <v>0</v>
       </c>
       <c r="Z46" s="1">
@@ -6070,25 +6070,25 @@
       <c r="AB46" s="1">
         <v>1</v>
       </c>
-      <c r="AC46" s="24">
+      <c r="AC46" s="17">
         <v>0</v>
       </c>
       <c r="AD46">
         <v>1</v>
       </c>
-      <c r="AE46" s="19">
+      <c r="AE46" s="12">
         <v>1</v>
       </c>
       <c r="AF46">
         <v>1</v>
       </c>
-      <c r="AG46" s="19">
+      <c r="AG46" s="12">
         <v>1</v>
       </c>
       <c r="AH46">
         <v>1</v>
       </c>
-      <c r="AI46" s="19">
+      <c r="AI46" s="12">
         <v>1</v>
       </c>
       <c r="AJ46">
@@ -6124,7 +6124,7 @@
       <c r="H47">
         <v>0</v>
       </c>
-      <c r="I47" s="19">
+      <c r="I47" s="12">
         <v>0</v>
       </c>
       <c r="J47">
@@ -6139,7 +6139,7 @@
       <c r="M47">
         <v>1</v>
       </c>
-      <c r="N47" s="19">
+      <c r="N47" s="12">
         <v>0</v>
       </c>
       <c r="O47">
@@ -6154,7 +6154,7 @@
       <c r="R47">
         <v>1</v>
       </c>
-      <c r="S47" s="19">
+      <c r="S47" s="12">
         <v>0</v>
       </c>
       <c r="T47">
@@ -6172,7 +6172,7 @@
       <c r="X47">
         <v>0</v>
       </c>
-      <c r="Y47" s="19">
+      <c r="Y47" s="12">
         <v>0</v>
       </c>
       <c r="Z47" s="1">
@@ -6184,25 +6184,25 @@
       <c r="AB47" s="1">
         <v>1</v>
       </c>
-      <c r="AC47" s="24">
+      <c r="AC47" s="17">
         <v>0</v>
       </c>
       <c r="AD47">
         <v>0</v>
       </c>
-      <c r="AE47" s="19">
+      <c r="AE47" s="12">
         <v>0</v>
       </c>
       <c r="AF47">
         <v>1</v>
       </c>
-      <c r="AG47" s="19">
+      <c r="AG47" s="12">
         <v>1</v>
       </c>
       <c r="AH47">
         <v>1</v>
       </c>
-      <c r="AI47" s="19">
+      <c r="AI47" s="12">
         <v>1</v>
       </c>
       <c r="AJ47">
@@ -6214,17 +6214,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E1:Y1"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="T2:Y2"/>
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="AD1:AK1"/>
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="E1:Y1"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:N2"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="T2:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
minor change to mammal matrix
</commit_message>
<xml_diff>
--- a/Mammal matrix.xlsx
+++ b/Mammal matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7EB2C0-BE0B-0545-83B5-918751B2D8B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37F7DCF-A0FE-4E4B-8F5D-71784ABDA625}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="KEY" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$3:$AK$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$A$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -481,7 +481,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -542,6 +542,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -564,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -572,32 +578,11 @@
       <alignment indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -606,6 +591,28 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,9 +953,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -960,128 +967,128 @@
     <col min="5" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5" style="12" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="26" max="28" width="7.6640625" customWidth="1"/>
-    <col min="29" max="29" width="7.6640625" style="19" customWidth="1"/>
+    <col min="29" max="29" width="7.6640625" style="12" customWidth="1"/>
     <col min="30" max="30" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5" style="12" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.5" style="12" bestFit="1" customWidth="1"/>
     <col min="36" max="37" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="10" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="13" t="s">
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="8" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="6" t="s">
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="8" t="s">
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="11" t="s">
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="AA2" s="12" t="s">
+      <c r="AA2" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="AB2" s="11" t="s">
+      <c r="AB2" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="AC2" s="23" t="s">
+      <c r="AC2" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="AD2" s="14" t="s">
+      <c r="AD2" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="16" t="s">
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="AG2" s="16"/>
-      <c r="AH2" s="14" t="s">
+      <c r="AG2" s="21"/>
+      <c r="AH2" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="16" t="s">
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="AK2" s="16"/>
+      <c r="AK2" s="21"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -1096,103 +1103,103 @@
       <c r="D3" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="S3" s="18" t="s">
+      <c r="S3" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="T3" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="U3" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="V3" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="W3" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="X3" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="Y3" s="20" t="s">
+      <c r="Y3" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="Z3" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="AB3" s="11" t="s">
+      <c r="AB3" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="AC3" s="23" t="s">
+      <c r="AC3" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="AD3" s="15" t="s">
+      <c r="AD3" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="AE3" s="21" t="s">
+      <c r="AE3" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="AF3" s="17" t="s">
+      <c r="AF3" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="AG3" s="22" t="s">
+      <c r="AG3" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="AH3" s="15" t="s">
+      <c r="AH3" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="AI3" s="21" t="s">
+      <c r="AI3" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="AJ3" s="17" t="s">
+      <c r="AJ3" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="AK3" s="17" t="s">
+      <c r="AK3" s="10" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1222,7 +1229,7 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="12">
         <v>1</v>
       </c>
       <c r="J4">
@@ -1237,7 +1244,7 @@
       <c r="M4">
         <v>1</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="12">
         <v>1</v>
       </c>
       <c r="O4">
@@ -1252,7 +1259,7 @@
       <c r="R4">
         <v>1</v>
       </c>
-      <c r="S4" s="19">
+      <c r="S4" s="12">
         <v>1</v>
       </c>
       <c r="T4">
@@ -1270,7 +1277,7 @@
       <c r="X4">
         <v>0</v>
       </c>
-      <c r="Y4" s="19">
+      <c r="Y4" s="12">
         <v>0</v>
       </c>
       <c r="Z4" s="1">
@@ -1282,25 +1289,25 @@
       <c r="AB4" s="1">
         <v>1</v>
       </c>
-      <c r="AC4" s="24">
+      <c r="AC4" s="17">
         <v>0</v>
       </c>
       <c r="AD4">
         <v>0</v>
       </c>
-      <c r="AE4" s="19">
+      <c r="AE4" s="12">
         <v>1</v>
       </c>
       <c r="AF4">
         <v>0</v>
       </c>
-      <c r="AG4" s="19">
+      <c r="AG4" s="12">
         <v>1</v>
       </c>
       <c r="AH4">
         <v>0</v>
       </c>
-      <c r="AI4" s="19">
+      <c r="AI4" s="12">
         <v>1</v>
       </c>
       <c r="AJ4">
@@ -1336,7 +1343,7 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="12">
         <v>0</v>
       </c>
       <c r="J5">
@@ -1351,7 +1358,7 @@
       <c r="M5">
         <v>1</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="12">
         <v>0</v>
       </c>
       <c r="O5">
@@ -1366,7 +1373,7 @@
       <c r="R5">
         <v>1</v>
       </c>
-      <c r="S5" s="19">
+      <c r="S5" s="12">
         <v>0</v>
       </c>
       <c r="T5">
@@ -1384,7 +1391,7 @@
       <c r="X5">
         <v>0</v>
       </c>
-      <c r="Y5" s="19">
+      <c r="Y5" s="12">
         <v>0</v>
       </c>
       <c r="Z5" s="1">
@@ -1396,25 +1403,25 @@
       <c r="AB5" s="1">
         <v>1</v>
       </c>
-      <c r="AC5" s="24">
+      <c r="AC5" s="17">
         <v>0</v>
       </c>
       <c r="AD5">
         <v>0</v>
       </c>
-      <c r="AE5" s="19">
+      <c r="AE5" s="12">
         <v>0</v>
       </c>
       <c r="AF5">
         <v>0</v>
       </c>
-      <c r="AG5" s="19">
+      <c r="AG5" s="12">
         <v>1</v>
       </c>
       <c r="AH5">
         <v>0</v>
       </c>
-      <c r="AI5" s="19">
+      <c r="AI5" s="12">
         <v>1</v>
       </c>
       <c r="AJ5">
@@ -1450,7 +1457,7 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="12">
         <v>0</v>
       </c>
       <c r="J6">
@@ -1465,7 +1472,7 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="12">
         <v>0</v>
       </c>
       <c r="O6">
@@ -1480,7 +1487,7 @@
       <c r="R6">
         <v>0</v>
       </c>
-      <c r="S6" s="19">
+      <c r="S6" s="12">
         <v>0</v>
       </c>
       <c r="T6">
@@ -1498,7 +1505,7 @@
       <c r="X6">
         <v>0</v>
       </c>
-      <c r="Y6" s="19">
+      <c r="Y6" s="12">
         <v>0</v>
       </c>
       <c r="Z6" s="1">
@@ -1510,25 +1517,25 @@
       <c r="AB6" s="1">
         <v>1</v>
       </c>
-      <c r="AC6" s="24">
+      <c r="AC6" s="17">
         <v>1</v>
       </c>
       <c r="AD6">
         <v>0</v>
       </c>
-      <c r="AE6" s="19">
+      <c r="AE6" s="12">
         <v>0</v>
       </c>
       <c r="AF6">
         <v>0</v>
       </c>
-      <c r="AG6" s="19">
+      <c r="AG6" s="12">
         <v>0</v>
       </c>
       <c r="AH6">
         <v>1</v>
       </c>
-      <c r="AI6" s="19">
+      <c r="AI6" s="12">
         <v>0</v>
       </c>
       <c r="AJ6">
@@ -1564,7 +1571,7 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="12">
         <v>0</v>
       </c>
       <c r="J7">
@@ -1579,7 +1586,7 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="12">
         <v>0</v>
       </c>
       <c r="O7">
@@ -1594,7 +1601,7 @@
       <c r="R7">
         <v>0</v>
       </c>
-      <c r="S7" s="19">
+      <c r="S7" s="12">
         <v>0</v>
       </c>
       <c r="T7">
@@ -1612,7 +1619,7 @@
       <c r="X7">
         <v>0</v>
       </c>
-      <c r="Y7" s="19">
+      <c r="Y7" s="12">
         <v>0</v>
       </c>
       <c r="Z7" s="1">
@@ -1624,25 +1631,25 @@
       <c r="AB7" s="1">
         <v>1</v>
       </c>
-      <c r="AC7" s="24">
+      <c r="AC7" s="17">
         <v>1</v>
       </c>
       <c r="AD7">
         <v>0</v>
       </c>
-      <c r="AE7" s="19">
+      <c r="AE7" s="12">
         <v>0</v>
       </c>
       <c r="AF7">
         <v>0</v>
       </c>
-      <c r="AG7" s="19">
+      <c r="AG7" s="12">
         <v>0</v>
       </c>
       <c r="AH7">
         <v>1</v>
       </c>
-      <c r="AI7" s="19">
+      <c r="AI7" s="12">
         <v>0</v>
       </c>
       <c r="AJ7">
@@ -1678,7 +1685,7 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="12">
         <v>0</v>
       </c>
       <c r="J8">
@@ -1693,7 +1700,7 @@
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="12">
         <v>0</v>
       </c>
       <c r="O8">
@@ -1708,7 +1715,7 @@
       <c r="R8">
         <v>0</v>
       </c>
-      <c r="S8" s="19">
+      <c r="S8" s="12">
         <v>0</v>
       </c>
       <c r="T8">
@@ -1726,7 +1733,7 @@
       <c r="X8">
         <v>0</v>
       </c>
-      <c r="Y8" s="19">
+      <c r="Y8" s="12">
         <v>0</v>
       </c>
       <c r="Z8" s="1">
@@ -1738,25 +1745,25 @@
       <c r="AB8" s="1">
         <v>1</v>
       </c>
-      <c r="AC8" s="24">
+      <c r="AC8" s="17">
         <v>1</v>
       </c>
       <c r="AD8">
         <v>0</v>
       </c>
-      <c r="AE8" s="19">
+      <c r="AE8" s="12">
         <v>0</v>
       </c>
       <c r="AF8">
         <v>0</v>
       </c>
-      <c r="AG8" s="19">
+      <c r="AG8" s="12">
         <v>0</v>
       </c>
       <c r="AH8">
         <v>1</v>
       </c>
-      <c r="AI8" s="19">
+      <c r="AI8" s="12">
         <v>0</v>
       </c>
       <c r="AJ8">
@@ -1792,7 +1799,7 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="12">
         <v>0</v>
       </c>
       <c r="J9">
@@ -1807,7 +1814,7 @@
       <c r="M9">
         <v>1</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="12">
         <v>0</v>
       </c>
       <c r="O9">
@@ -1822,7 +1829,7 @@
       <c r="R9">
         <v>1</v>
       </c>
-      <c r="S9" s="19">
+      <c r="S9" s="12">
         <v>0</v>
       </c>
       <c r="T9">
@@ -1840,7 +1847,7 @@
       <c r="X9">
         <v>0</v>
       </c>
-      <c r="Y9" s="19">
+      <c r="Y9" s="12">
         <v>0</v>
       </c>
       <c r="Z9" s="1">
@@ -1852,25 +1859,25 @@
       <c r="AB9" s="1">
         <v>1</v>
       </c>
-      <c r="AC9" s="24">
+      <c r="AC9" s="17">
         <v>0</v>
       </c>
       <c r="AD9">
         <v>1</v>
       </c>
-      <c r="AE9" s="19">
+      <c r="AE9" s="12">
         <v>0</v>
       </c>
       <c r="AF9">
         <v>1</v>
       </c>
-      <c r="AG9" s="19">
+      <c r="AG9" s="12">
         <v>0</v>
       </c>
       <c r="AH9">
         <v>1</v>
       </c>
-      <c r="AI9" s="19">
+      <c r="AI9" s="12">
         <v>0</v>
       </c>
       <c r="AJ9">
@@ -1906,7 +1913,7 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="12">
         <v>0</v>
       </c>
       <c r="J10">
@@ -1921,7 +1928,7 @@
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="12">
         <v>0</v>
       </c>
       <c r="O10">
@@ -1936,7 +1943,7 @@
       <c r="R10">
         <v>0</v>
       </c>
-      <c r="S10" s="19">
+      <c r="S10" s="12">
         <v>0</v>
       </c>
       <c r="T10">
@@ -1954,7 +1961,7 @@
       <c r="X10">
         <v>0</v>
       </c>
-      <c r="Y10" s="19">
+      <c r="Y10" s="12">
         <v>0</v>
       </c>
       <c r="Z10" s="1">
@@ -1966,25 +1973,25 @@
       <c r="AB10" s="1">
         <v>1</v>
       </c>
-      <c r="AC10" s="24">
+      <c r="AC10" s="17">
         <v>1</v>
       </c>
       <c r="AD10">
         <v>0</v>
       </c>
-      <c r="AE10" s="19">
+      <c r="AE10" s="12">
         <v>0</v>
       </c>
       <c r="AF10">
         <v>0</v>
       </c>
-      <c r="AG10" s="19">
+      <c r="AG10" s="12">
         <v>0</v>
       </c>
       <c r="AH10">
         <v>1</v>
       </c>
-      <c r="AI10" s="19">
+      <c r="AI10" s="12">
         <v>0</v>
       </c>
       <c r="AJ10">
@@ -1995,7 +2002,7 @@
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2020,7 +2027,7 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="12">
         <v>1</v>
       </c>
       <c r="J11">
@@ -2035,7 +2042,7 @@
       <c r="M11">
         <v>1</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="12">
         <v>1</v>
       </c>
       <c r="O11">
@@ -2050,7 +2057,7 @@
       <c r="R11">
         <v>1</v>
       </c>
-      <c r="S11" s="19">
+      <c r="S11" s="12">
         <v>1</v>
       </c>
       <c r="T11">
@@ -2068,7 +2075,7 @@
       <c r="X11">
         <v>1</v>
       </c>
-      <c r="Y11" s="19">
+      <c r="Y11" s="12">
         <v>0</v>
       </c>
       <c r="Z11" s="1">
@@ -2080,25 +2087,25 @@
       <c r="AB11" s="1">
         <v>1</v>
       </c>
-      <c r="AC11" s="24">
+      <c r="AC11" s="17">
         <v>1</v>
       </c>
       <c r="AD11">
         <v>1</v>
       </c>
-      <c r="AE11" s="19">
+      <c r="AE11" s="12">
         <v>1</v>
       </c>
       <c r="AF11">
         <v>1</v>
       </c>
-      <c r="AG11" s="19">
+      <c r="AG11" s="12">
         <v>1</v>
       </c>
       <c r="AH11">
         <v>1</v>
       </c>
-      <c r="AI11" s="19">
+      <c r="AI11" s="12">
         <v>1</v>
       </c>
       <c r="AJ11">
@@ -2134,7 +2141,7 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="12">
         <v>0</v>
       </c>
       <c r="J12">
@@ -2149,7 +2156,7 @@
       <c r="M12">
         <v>1</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="12">
         <v>0</v>
       </c>
       <c r="O12">
@@ -2164,7 +2171,7 @@
       <c r="R12">
         <v>1</v>
       </c>
-      <c r="S12" s="19">
+      <c r="S12" s="12">
         <v>0</v>
       </c>
       <c r="T12">
@@ -2182,7 +2189,7 @@
       <c r="X12">
         <v>0</v>
       </c>
-      <c r="Y12" s="19">
+      <c r="Y12" s="12">
         <v>0</v>
       </c>
       <c r="Z12" s="1">
@@ -2194,25 +2201,25 @@
       <c r="AB12" s="1">
         <v>1</v>
       </c>
-      <c r="AC12" s="24">
+      <c r="AC12" s="17">
         <v>1</v>
       </c>
       <c r="AD12">
         <v>0</v>
       </c>
-      <c r="AE12" s="19">
+      <c r="AE12" s="12">
         <v>0</v>
       </c>
       <c r="AF12">
         <v>0</v>
       </c>
-      <c r="AG12" s="19">
+      <c r="AG12" s="12">
         <v>0</v>
       </c>
       <c r="AH12">
         <v>1</v>
       </c>
-      <c r="AI12" s="19">
+      <c r="AI12" s="12">
         <v>0</v>
       </c>
       <c r="AJ12">
@@ -2248,7 +2255,7 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="12">
         <v>0</v>
       </c>
       <c r="J13">
@@ -2263,7 +2270,7 @@
       <c r="M13">
         <v>0</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13" s="12">
         <v>0</v>
       </c>
       <c r="O13">
@@ -2278,7 +2285,7 @@
       <c r="R13">
         <v>1</v>
       </c>
-      <c r="S13" s="19">
+      <c r="S13" s="12">
         <v>0</v>
       </c>
       <c r="T13">
@@ -2296,7 +2303,7 @@
       <c r="X13">
         <v>0</v>
       </c>
-      <c r="Y13" s="19">
+      <c r="Y13" s="12">
         <v>0</v>
       </c>
       <c r="Z13" s="1">
@@ -2308,25 +2315,25 @@
       <c r="AB13" s="1">
         <v>1</v>
       </c>
-      <c r="AC13" s="24">
+      <c r="AC13" s="17">
         <v>0</v>
       </c>
       <c r="AD13">
         <v>0</v>
       </c>
-      <c r="AE13" s="19">
+      <c r="AE13" s="12">
         <v>0</v>
       </c>
       <c r="AF13">
         <v>0</v>
       </c>
-      <c r="AG13" s="19">
+      <c r="AG13" s="12">
         <v>0</v>
       </c>
       <c r="AH13">
         <v>1</v>
       </c>
-      <c r="AI13" s="19">
+      <c r="AI13" s="12">
         <v>1</v>
       </c>
       <c r="AJ13">
@@ -2362,7 +2369,7 @@
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="12">
         <v>0</v>
       </c>
       <c r="J14">
@@ -2377,7 +2384,7 @@
       <c r="M14">
         <v>0</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="12">
         <v>0</v>
       </c>
       <c r="O14">
@@ -2392,7 +2399,7 @@
       <c r="R14">
         <v>0</v>
       </c>
-      <c r="S14" s="19">
+      <c r="S14" s="12">
         <v>0</v>
       </c>
       <c r="T14">
@@ -2410,7 +2417,7 @@
       <c r="X14">
         <v>0</v>
       </c>
-      <c r="Y14" s="19">
+      <c r="Y14" s="12">
         <v>0</v>
       </c>
       <c r="Z14" s="1">
@@ -2422,25 +2429,25 @@
       <c r="AB14" s="1">
         <v>1</v>
       </c>
-      <c r="AC14" s="24">
+      <c r="AC14" s="17">
         <v>0</v>
       </c>
       <c r="AD14">
         <v>0</v>
       </c>
-      <c r="AE14" s="19">
+      <c r="AE14" s="12">
         <v>1</v>
       </c>
       <c r="AF14">
         <v>0</v>
       </c>
-      <c r="AG14" s="19">
+      <c r="AG14" s="12">
         <v>1</v>
       </c>
       <c r="AH14">
         <v>0</v>
       </c>
-      <c r="AI14" s="19">
+      <c r="AI14" s="12">
         <v>1</v>
       </c>
       <c r="AJ14">
@@ -2476,7 +2483,7 @@
       <c r="H15">
         <v>0</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="12">
         <v>0</v>
       </c>
       <c r="J15">
@@ -2491,7 +2498,7 @@
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="N15" s="19">
+      <c r="N15" s="12">
         <v>0</v>
       </c>
       <c r="O15">
@@ -2506,7 +2513,7 @@
       <c r="R15">
         <v>0</v>
       </c>
-      <c r="S15" s="19">
+      <c r="S15" s="12">
         <v>0</v>
       </c>
       <c r="T15">
@@ -2524,7 +2531,7 @@
       <c r="X15">
         <v>0</v>
       </c>
-      <c r="Y15" s="19">
+      <c r="Y15" s="12">
         <v>0</v>
       </c>
       <c r="Z15" s="1">
@@ -2536,25 +2543,25 @@
       <c r="AB15" s="1">
         <v>1</v>
       </c>
-      <c r="AC15" s="24">
+      <c r="AC15" s="17">
         <v>0</v>
       </c>
       <c r="AD15">
         <v>1</v>
       </c>
-      <c r="AE15" s="19">
+      <c r="AE15" s="12">
         <v>1</v>
       </c>
       <c r="AF15">
         <v>1</v>
       </c>
-      <c r="AG15" s="19">
+      <c r="AG15" s="12">
         <v>1</v>
       </c>
       <c r="AH15">
         <v>1</v>
       </c>
-      <c r="AI15" s="19">
+      <c r="AI15" s="12">
         <v>1</v>
       </c>
       <c r="AJ15">
@@ -2590,7 +2597,7 @@
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="12">
         <v>0</v>
       </c>
       <c r="J16">
@@ -2605,7 +2612,7 @@
       <c r="M16">
         <v>0</v>
       </c>
-      <c r="N16" s="19">
+      <c r="N16" s="12">
         <v>0</v>
       </c>
       <c r="O16">
@@ -2620,7 +2627,7 @@
       <c r="R16">
         <v>0</v>
       </c>
-      <c r="S16" s="19">
+      <c r="S16" s="12">
         <v>0</v>
       </c>
       <c r="T16">
@@ -2638,7 +2645,7 @@
       <c r="X16">
         <v>0</v>
       </c>
-      <c r="Y16" s="19">
+      <c r="Y16" s="12">
         <v>0</v>
       </c>
       <c r="Z16" s="1">
@@ -2650,25 +2657,25 @@
       <c r="AB16" s="1">
         <v>1</v>
       </c>
-      <c r="AC16" s="24">
+      <c r="AC16" s="17">
         <v>1</v>
       </c>
       <c r="AD16">
         <v>0</v>
       </c>
-      <c r="AE16" s="19">
+      <c r="AE16" s="12">
         <v>0</v>
       </c>
       <c r="AF16">
         <v>0</v>
       </c>
-      <c r="AG16" s="19">
+      <c r="AG16" s="12">
         <v>0</v>
       </c>
       <c r="AH16">
         <v>1</v>
       </c>
-      <c r="AI16" s="19">
+      <c r="AI16" s="12">
         <v>0</v>
       </c>
       <c r="AJ16">
@@ -2704,7 +2711,7 @@
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="12">
         <v>0</v>
       </c>
       <c r="J17">
@@ -2719,7 +2726,7 @@
       <c r="M17">
         <v>1</v>
       </c>
-      <c r="N17" s="19">
+      <c r="N17" s="12">
         <v>0</v>
       </c>
       <c r="O17">
@@ -2734,7 +2741,7 @@
       <c r="R17">
         <v>1</v>
       </c>
-      <c r="S17" s="19">
+      <c r="S17" s="12">
         <v>0</v>
       </c>
       <c r="T17">
@@ -2752,7 +2759,7 @@
       <c r="X17">
         <v>0</v>
       </c>
-      <c r="Y17" s="19">
+      <c r="Y17" s="12">
         <v>0</v>
       </c>
       <c r="Z17" s="1">
@@ -2764,25 +2771,25 @@
       <c r="AB17" s="1">
         <v>1</v>
       </c>
-      <c r="AC17" s="24">
+      <c r="AC17" s="17">
         <v>0</v>
       </c>
       <c r="AD17">
         <v>0</v>
       </c>
-      <c r="AE17" s="19">
+      <c r="AE17" s="12">
         <v>0</v>
       </c>
       <c r="AF17">
         <v>0</v>
       </c>
-      <c r="AG17" s="19">
+      <c r="AG17" s="12">
         <v>0</v>
       </c>
       <c r="AH17">
         <v>0</v>
       </c>
-      <c r="AI17" s="19">
+      <c r="AI17" s="12">
         <v>0</v>
       </c>
       <c r="AJ17">
@@ -2818,7 +2825,7 @@
       <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="12">
         <v>0</v>
       </c>
       <c r="J18">
@@ -2833,7 +2840,7 @@
       <c r="M18">
         <v>1</v>
       </c>
-      <c r="N18" s="19">
+      <c r="N18" s="12">
         <v>0</v>
       </c>
       <c r="O18">
@@ -2848,7 +2855,7 @@
       <c r="R18">
         <v>1</v>
       </c>
-      <c r="S18" s="19">
+      <c r="S18" s="12">
         <v>0</v>
       </c>
       <c r="T18">
@@ -2866,7 +2873,7 @@
       <c r="X18">
         <v>0</v>
       </c>
-      <c r="Y18" s="19">
+      <c r="Y18" s="12">
         <v>0</v>
       </c>
       <c r="Z18" s="1">
@@ -2878,25 +2885,25 @@
       <c r="AB18" s="1">
         <v>1</v>
       </c>
-      <c r="AC18" s="24">
+      <c r="AC18" s="17">
         <v>0</v>
       </c>
       <c r="AD18">
         <v>1</v>
       </c>
-      <c r="AE18" s="19">
+      <c r="AE18" s="12">
         <v>1</v>
       </c>
       <c r="AF18">
         <v>1</v>
       </c>
-      <c r="AG18" s="19">
+      <c r="AG18" s="12">
         <v>1</v>
       </c>
       <c r="AH18">
         <v>1</v>
       </c>
-      <c r="AI18" s="19">
+      <c r="AI18" s="12">
         <v>1</v>
       </c>
       <c r="AJ18">
@@ -2932,7 +2939,7 @@
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="12">
         <v>0</v>
       </c>
       <c r="J19">
@@ -2947,7 +2954,7 @@
       <c r="M19">
         <v>0</v>
       </c>
-      <c r="N19" s="19">
+      <c r="N19" s="12">
         <v>0</v>
       </c>
       <c r="O19">
@@ -2962,7 +2969,7 @@
       <c r="R19">
         <v>0</v>
       </c>
-      <c r="S19" s="19">
+      <c r="S19" s="12">
         <v>0</v>
       </c>
       <c r="T19">
@@ -2980,7 +2987,7 @@
       <c r="X19">
         <v>0</v>
       </c>
-      <c r="Y19" s="19">
+      <c r="Y19" s="12">
         <v>0</v>
       </c>
       <c r="Z19" s="1">
@@ -2992,25 +2999,25 @@
       <c r="AB19" s="1">
         <v>1</v>
       </c>
-      <c r="AC19" s="24">
+      <c r="AC19" s="17">
         <v>1</v>
       </c>
       <c r="AD19">
         <v>0</v>
       </c>
-      <c r="AE19" s="19">
+      <c r="AE19" s="12">
         <v>0</v>
       </c>
       <c r="AF19">
         <v>0</v>
       </c>
-      <c r="AG19" s="19">
+      <c r="AG19" s="12">
         <v>0</v>
       </c>
       <c r="AH19">
         <v>0</v>
       </c>
-      <c r="AI19" s="19">
+      <c r="AI19" s="12">
         <v>0</v>
       </c>
       <c r="AJ19">
@@ -3046,7 +3053,7 @@
       <c r="H20">
         <v>0</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="12">
         <v>0</v>
       </c>
       <c r="J20">
@@ -3061,7 +3068,7 @@
       <c r="M20">
         <v>0</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="12">
         <v>0</v>
       </c>
       <c r="O20">
@@ -3076,7 +3083,7 @@
       <c r="R20">
         <v>0</v>
       </c>
-      <c r="S20" s="19">
+      <c r="S20" s="12">
         <v>0</v>
       </c>
       <c r="T20">
@@ -3094,7 +3101,7 @@
       <c r="X20">
         <v>0</v>
       </c>
-      <c r="Y20" s="19">
+      <c r="Y20" s="12">
         <v>0</v>
       </c>
       <c r="Z20" s="1">
@@ -3106,25 +3113,25 @@
       <c r="AB20" s="1">
         <v>1</v>
       </c>
-      <c r="AC20" s="24">
+      <c r="AC20" s="17">
         <v>1</v>
       </c>
       <c r="AD20">
         <v>0</v>
       </c>
-      <c r="AE20" s="19">
+      <c r="AE20" s="12">
         <v>0</v>
       </c>
       <c r="AF20">
         <v>0</v>
       </c>
-      <c r="AG20" s="19">
+      <c r="AG20" s="12">
         <v>0</v>
       </c>
       <c r="AH20">
         <v>1</v>
       </c>
-      <c r="AI20" s="19">
+      <c r="AI20" s="12">
         <v>0</v>
       </c>
       <c r="AJ20">
@@ -3160,7 +3167,7 @@
       <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="12">
         <v>0</v>
       </c>
       <c r="J21">
@@ -3175,7 +3182,7 @@
       <c r="M21">
         <v>1</v>
       </c>
-      <c r="N21" s="19">
+      <c r="N21" s="12">
         <v>0</v>
       </c>
       <c r="O21">
@@ -3190,7 +3197,7 @@
       <c r="R21">
         <v>1</v>
       </c>
-      <c r="S21" s="19">
+      <c r="S21" s="12">
         <v>0</v>
       </c>
       <c r="T21">
@@ -3208,7 +3215,7 @@
       <c r="X21">
         <v>0</v>
       </c>
-      <c r="Y21" s="19">
+      <c r="Y21" s="12">
         <v>0</v>
       </c>
       <c r="Z21" s="1">
@@ -3220,25 +3227,25 @@
       <c r="AB21" s="1">
         <v>1</v>
       </c>
-      <c r="AC21" s="24">
+      <c r="AC21" s="17">
         <v>1</v>
       </c>
       <c r="AD21">
         <v>1</v>
       </c>
-      <c r="AE21" s="19">
+      <c r="AE21" s="12">
         <v>1</v>
       </c>
       <c r="AF21">
         <v>1</v>
       </c>
-      <c r="AG21" s="19">
+      <c r="AG21" s="12">
         <v>1</v>
       </c>
       <c r="AH21">
         <v>1</v>
       </c>
-      <c r="AI21" s="19">
+      <c r="AI21" s="12">
         <v>1</v>
       </c>
       <c r="AJ21">
@@ -3274,7 +3281,7 @@
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="12">
         <v>1</v>
       </c>
       <c r="J22">
@@ -3289,7 +3296,7 @@
       <c r="M22">
         <v>1</v>
       </c>
-      <c r="N22" s="19">
+      <c r="N22" s="12">
         <v>1</v>
       </c>
       <c r="O22">
@@ -3304,7 +3311,7 @@
       <c r="R22">
         <v>1</v>
       </c>
-      <c r="S22" s="19">
+      <c r="S22" s="12">
         <v>1</v>
       </c>
       <c r="T22">
@@ -3322,7 +3329,7 @@
       <c r="X22">
         <v>0</v>
       </c>
-      <c r="Y22" s="19">
+      <c r="Y22" s="12">
         <v>0</v>
       </c>
       <c r="Z22" s="1">
@@ -3334,25 +3341,25 @@
       <c r="AB22" s="1">
         <v>1</v>
       </c>
-      <c r="AC22" s="24">
+      <c r="AC22" s="17">
         <v>0</v>
       </c>
       <c r="AD22">
         <v>0</v>
       </c>
-      <c r="AE22" s="19">
+      <c r="AE22" s="12">
         <v>0</v>
       </c>
       <c r="AF22">
         <v>1</v>
       </c>
-      <c r="AG22" s="19">
+      <c r="AG22" s="12">
         <v>0</v>
       </c>
       <c r="AH22">
         <v>1</v>
       </c>
-      <c r="AI22" s="19">
+      <c r="AI22" s="12">
         <v>0</v>
       </c>
       <c r="AJ22">
@@ -3388,7 +3395,7 @@
       <c r="H23">
         <v>1</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="12">
         <v>0</v>
       </c>
       <c r="J23">
@@ -3403,7 +3410,7 @@
       <c r="M23">
         <v>1</v>
       </c>
-      <c r="N23" s="19">
+      <c r="N23" s="12">
         <v>0</v>
       </c>
       <c r="O23">
@@ -3418,7 +3425,7 @@
       <c r="R23">
         <v>1</v>
       </c>
-      <c r="S23" s="19">
+      <c r="S23" s="12">
         <v>0</v>
       </c>
       <c r="T23">
@@ -3436,7 +3443,7 @@
       <c r="X23">
         <v>0</v>
       </c>
-      <c r="Y23" s="19">
+      <c r="Y23" s="12">
         <v>0</v>
       </c>
       <c r="Z23" s="1">
@@ -3448,25 +3455,25 @@
       <c r="AB23" s="1">
         <v>1</v>
       </c>
-      <c r="AC23" s="24">
+      <c r="AC23" s="17">
         <v>0</v>
       </c>
       <c r="AD23">
         <v>1</v>
       </c>
-      <c r="AE23" s="19">
+      <c r="AE23" s="12">
         <v>0</v>
       </c>
       <c r="AF23">
         <v>1</v>
       </c>
-      <c r="AG23" s="19">
+      <c r="AG23" s="12">
         <v>0</v>
       </c>
       <c r="AH23">
         <v>1</v>
       </c>
-      <c r="AI23" s="19">
+      <c r="AI23" s="12">
         <v>0</v>
       </c>
       <c r="AJ23">
@@ -3502,7 +3509,7 @@
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="I24" s="19">
+      <c r="I24" s="12">
         <v>0</v>
       </c>
       <c r="J24">
@@ -3517,7 +3524,7 @@
       <c r="M24">
         <v>0</v>
       </c>
-      <c r="N24" s="19">
+      <c r="N24" s="12">
         <v>0</v>
       </c>
       <c r="O24">
@@ -3532,7 +3539,7 @@
       <c r="R24">
         <v>0</v>
       </c>
-      <c r="S24" s="19">
+      <c r="S24" s="12">
         <v>0</v>
       </c>
       <c r="T24">
@@ -3550,7 +3557,7 @@
       <c r="X24">
         <v>0</v>
       </c>
-      <c r="Y24" s="19">
+      <c r="Y24" s="12">
         <v>0</v>
       </c>
       <c r="Z24" s="1">
@@ -3562,25 +3569,25 @@
       <c r="AB24" s="1">
         <v>1</v>
       </c>
-      <c r="AC24" s="24">
+      <c r="AC24" s="17">
         <v>1</v>
       </c>
       <c r="AD24">
         <v>0</v>
       </c>
-      <c r="AE24" s="19">
+      <c r="AE24" s="12">
         <v>0</v>
       </c>
       <c r="AF24">
         <v>0</v>
       </c>
-      <c r="AG24" s="19">
+      <c r="AG24" s="12">
         <v>0</v>
       </c>
       <c r="AH24">
         <v>1</v>
       </c>
-      <c r="AI24" s="19">
+      <c r="AI24" s="12">
         <v>0</v>
       </c>
       <c r="AJ24">
@@ -3616,7 +3623,7 @@
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="I25" s="19">
+      <c r="I25" s="12">
         <v>0</v>
       </c>
       <c r="J25">
@@ -3631,7 +3638,7 @@
       <c r="M25">
         <v>0</v>
       </c>
-      <c r="N25" s="19">
+      <c r="N25" s="12">
         <v>0</v>
       </c>
       <c r="O25">
@@ -3646,7 +3653,7 @@
       <c r="R25">
         <v>0</v>
       </c>
-      <c r="S25" s="19">
+      <c r="S25" s="12">
         <v>0</v>
       </c>
       <c r="T25">
@@ -3664,7 +3671,7 @@
       <c r="X25">
         <v>0</v>
       </c>
-      <c r="Y25" s="19">
+      <c r="Y25" s="12">
         <v>0</v>
       </c>
       <c r="Z25" s="1">
@@ -3676,25 +3683,25 @@
       <c r="AB25" s="1">
         <v>1</v>
       </c>
-      <c r="AC25" s="24">
+      <c r="AC25" s="17">
         <v>1</v>
       </c>
       <c r="AD25">
         <v>0</v>
       </c>
-      <c r="AE25" s="19">
+      <c r="AE25" s="12">
         <v>0</v>
       </c>
       <c r="AF25">
         <v>0</v>
       </c>
-      <c r="AG25" s="19">
+      <c r="AG25" s="12">
         <v>0</v>
       </c>
       <c r="AH25">
         <v>0</v>
       </c>
-      <c r="AI25" s="19">
+      <c r="AI25" s="12">
         <v>0</v>
       </c>
       <c r="AJ25">
@@ -3730,7 +3737,7 @@
       <c r="H26">
         <v>1</v>
       </c>
-      <c r="I26" s="19">
+      <c r="I26" s="12">
         <v>0</v>
       </c>
       <c r="J26">
@@ -3745,7 +3752,7 @@
       <c r="M26">
         <v>1</v>
       </c>
-      <c r="N26" s="19">
+      <c r="N26" s="12">
         <v>0</v>
       </c>
       <c r="O26">
@@ -3760,7 +3767,7 @@
       <c r="R26">
         <v>1</v>
       </c>
-      <c r="S26" s="19">
+      <c r="S26" s="12">
         <v>0</v>
       </c>
       <c r="T26">
@@ -3778,7 +3785,7 @@
       <c r="X26">
         <v>0</v>
       </c>
-      <c r="Y26" s="19">
+      <c r="Y26" s="12">
         <v>0</v>
       </c>
       <c r="Z26" s="1">
@@ -3790,25 +3797,25 @@
       <c r="AB26" s="1">
         <v>1</v>
       </c>
-      <c r="AC26" s="24">
+      <c r="AC26" s="17">
         <v>0</v>
       </c>
       <c r="AD26">
         <v>0</v>
       </c>
-      <c r="AE26" s="19">
+      <c r="AE26" s="12">
         <v>0</v>
       </c>
       <c r="AF26">
         <v>0</v>
       </c>
-      <c r="AG26" s="19">
+      <c r="AG26" s="12">
         <v>0</v>
       </c>
       <c r="AH26">
         <v>1</v>
       </c>
-      <c r="AI26" s="19">
+      <c r="AI26" s="12">
         <v>0</v>
       </c>
       <c r="AJ26">
@@ -3844,7 +3851,7 @@
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="I27" s="19">
+      <c r="I27" s="12">
         <v>0</v>
       </c>
       <c r="J27">
@@ -3859,7 +3866,7 @@
       <c r="M27">
         <v>0</v>
       </c>
-      <c r="N27" s="19">
+      <c r="N27" s="12">
         <v>0</v>
       </c>
       <c r="O27">
@@ -3874,7 +3881,7 @@
       <c r="R27">
         <v>0</v>
       </c>
-      <c r="S27" s="19">
+      <c r="S27" s="12">
         <v>0</v>
       </c>
       <c r="T27">
@@ -3892,7 +3899,7 @@
       <c r="X27">
         <v>0</v>
       </c>
-      <c r="Y27" s="19">
+      <c r="Y27" s="12">
         <v>0</v>
       </c>
       <c r="Z27" s="1">
@@ -3904,25 +3911,25 @@
       <c r="AB27" s="1">
         <v>1</v>
       </c>
-      <c r="AC27" s="24">
+      <c r="AC27" s="17">
         <v>1</v>
       </c>
       <c r="AD27">
         <v>0</v>
       </c>
-      <c r="AE27" s="19">
+      <c r="AE27" s="12">
         <v>0</v>
       </c>
       <c r="AF27">
         <v>0</v>
       </c>
-      <c r="AG27" s="19">
+      <c r="AG27" s="12">
         <v>0</v>
       </c>
       <c r="AH27">
         <v>1</v>
       </c>
-      <c r="AI27" s="19">
+      <c r="AI27" s="12">
         <v>0</v>
       </c>
       <c r="AJ27">
@@ -3958,7 +3965,7 @@
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="I28" s="19">
+      <c r="I28" s="12">
         <v>0</v>
       </c>
       <c r="J28">
@@ -3973,7 +3980,7 @@
       <c r="M28">
         <v>0</v>
       </c>
-      <c r="N28" s="19">
+      <c r="N28" s="12">
         <v>0</v>
       </c>
       <c r="O28">
@@ -3988,7 +3995,7 @@
       <c r="R28">
         <v>0</v>
       </c>
-      <c r="S28" s="19">
+      <c r="S28" s="12">
         <v>0</v>
       </c>
       <c r="T28">
@@ -4006,7 +4013,7 @@
       <c r="X28">
         <v>0</v>
       </c>
-      <c r="Y28" s="19">
+      <c r="Y28" s="12">
         <v>0</v>
       </c>
       <c r="Z28" s="1">
@@ -4018,25 +4025,25 @@
       <c r="AB28" s="1">
         <v>1</v>
       </c>
-      <c r="AC28" s="24">
+      <c r="AC28" s="17">
         <v>1</v>
       </c>
       <c r="AD28">
         <v>0</v>
       </c>
-      <c r="AE28" s="19">
+      <c r="AE28" s="12">
         <v>0</v>
       </c>
       <c r="AF28">
         <v>0</v>
       </c>
-      <c r="AG28" s="19">
+      <c r="AG28" s="12">
         <v>0</v>
       </c>
       <c r="AH28">
         <v>1</v>
       </c>
-      <c r="AI28" s="19">
+      <c r="AI28" s="12">
         <v>0</v>
       </c>
       <c r="AJ28">
@@ -4072,7 +4079,7 @@
       <c r="H29">
         <v>0</v>
       </c>
-      <c r="I29" s="19">
+      <c r="I29" s="12">
         <v>0</v>
       </c>
       <c r="J29">
@@ -4087,7 +4094,7 @@
       <c r="M29">
         <v>0</v>
       </c>
-      <c r="N29" s="19">
+      <c r="N29" s="12">
         <v>0</v>
       </c>
       <c r="O29">
@@ -4102,7 +4109,7 @@
       <c r="R29">
         <v>0</v>
       </c>
-      <c r="S29" s="19">
+      <c r="S29" s="12">
         <v>0</v>
       </c>
       <c r="T29">
@@ -4120,7 +4127,7 @@
       <c r="X29">
         <v>0</v>
       </c>
-      <c r="Y29" s="19">
+      <c r="Y29" s="12">
         <v>0</v>
       </c>
       <c r="Z29" s="1">
@@ -4132,25 +4139,25 @@
       <c r="AB29" s="1">
         <v>1</v>
       </c>
-      <c r="AC29" s="24">
+      <c r="AC29" s="17">
         <v>1</v>
       </c>
       <c r="AD29">
         <v>0</v>
       </c>
-      <c r="AE29" s="19">
+      <c r="AE29" s="12">
         <v>0</v>
       </c>
       <c r="AF29">
         <v>0</v>
       </c>
-      <c r="AG29" s="19">
+      <c r="AG29" s="12">
         <v>0</v>
       </c>
       <c r="AH29">
         <v>1</v>
       </c>
-      <c r="AI29" s="19">
+      <c r="AI29" s="12">
         <v>0</v>
       </c>
       <c r="AJ29">
@@ -4186,7 +4193,7 @@
       <c r="H30">
         <v>0</v>
       </c>
-      <c r="I30" s="19">
+      <c r="I30" s="12">
         <v>0</v>
       </c>
       <c r="J30">
@@ -4201,7 +4208,7 @@
       <c r="M30">
         <v>0</v>
       </c>
-      <c r="N30" s="19">
+      <c r="N30" s="12">
         <v>0</v>
       </c>
       <c r="O30">
@@ -4216,7 +4223,7 @@
       <c r="R30">
         <v>0</v>
       </c>
-      <c r="S30" s="19">
+      <c r="S30" s="12">
         <v>0</v>
       </c>
       <c r="T30">
@@ -4234,7 +4241,7 @@
       <c r="X30">
         <v>1</v>
       </c>
-      <c r="Y30" s="19">
+      <c r="Y30" s="12">
         <v>1</v>
       </c>
       <c r="Z30" s="1">
@@ -4246,25 +4253,25 @@
       <c r="AB30" s="1">
         <v>0</v>
       </c>
-      <c r="AC30" s="24">
+      <c r="AC30" s="17">
         <v>1</v>
       </c>
       <c r="AD30">
         <v>0</v>
       </c>
-      <c r="AE30" s="19">
+      <c r="AE30" s="12">
         <v>0</v>
       </c>
       <c r="AF30">
         <v>0</v>
       </c>
-      <c r="AG30" s="19">
+      <c r="AG30" s="12">
         <v>0</v>
       </c>
       <c r="AH30">
         <v>0</v>
       </c>
-      <c r="AI30" s="19">
+      <c r="AI30" s="12">
         <v>0</v>
       </c>
       <c r="AJ30">
@@ -4300,7 +4307,7 @@
       <c r="H31">
         <v>0</v>
       </c>
-      <c r="I31" s="19">
+      <c r="I31" s="12">
         <v>0</v>
       </c>
       <c r="J31">
@@ -4315,7 +4322,7 @@
       <c r="M31">
         <v>0</v>
       </c>
-      <c r="N31" s="19">
+      <c r="N31" s="12">
         <v>0</v>
       </c>
       <c r="O31">
@@ -4330,7 +4337,7 @@
       <c r="R31">
         <v>0</v>
       </c>
-      <c r="S31" s="19">
+      <c r="S31" s="12">
         <v>0</v>
       </c>
       <c r="T31">
@@ -4348,7 +4355,7 @@
       <c r="X31">
         <v>0</v>
       </c>
-      <c r="Y31" s="19">
+      <c r="Y31" s="12">
         <v>0</v>
       </c>
       <c r="Z31" s="1">
@@ -4360,25 +4367,25 @@
       <c r="AB31" s="1">
         <v>1</v>
       </c>
-      <c r="AC31" s="24">
+      <c r="AC31" s="17">
         <v>1</v>
       </c>
       <c r="AD31">
         <v>0</v>
       </c>
-      <c r="AE31" s="19">
+      <c r="AE31" s="12">
         <v>0</v>
       </c>
       <c r="AF31">
         <v>0</v>
       </c>
-      <c r="AG31" s="19">
+      <c r="AG31" s="12">
         <v>0</v>
       </c>
       <c r="AH31">
         <v>1</v>
       </c>
-      <c r="AI31" s="19">
+      <c r="AI31" s="12">
         <v>0</v>
       </c>
       <c r="AJ31">
@@ -4389,7 +4396,7 @@
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="25" t="s">
         <v>57</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -4414,7 +4421,7 @@
       <c r="H32">
         <v>0</v>
       </c>
-      <c r="I32" s="19">
+      <c r="I32" s="12">
         <v>1</v>
       </c>
       <c r="J32">
@@ -4429,7 +4436,7 @@
       <c r="M32">
         <v>0</v>
       </c>
-      <c r="N32" s="19">
+      <c r="N32" s="12">
         <v>1</v>
       </c>
       <c r="O32">
@@ -4444,7 +4451,7 @@
       <c r="R32">
         <v>0</v>
       </c>
-      <c r="S32" s="19">
+      <c r="S32" s="12">
         <v>1</v>
       </c>
       <c r="T32">
@@ -4462,7 +4469,7 @@
       <c r="X32">
         <v>1</v>
       </c>
-      <c r="Y32" s="19">
+      <c r="Y32" s="12">
         <v>1</v>
       </c>
       <c r="Z32" s="1">
@@ -4474,25 +4481,25 @@
       <c r="AB32" s="1">
         <v>1</v>
       </c>
-      <c r="AC32" s="24">
+      <c r="AC32" s="17">
         <v>1</v>
       </c>
       <c r="AD32">
         <v>1</v>
       </c>
-      <c r="AE32" s="19">
+      <c r="AE32" s="12">
         <v>1</v>
       </c>
       <c r="AF32">
         <v>1</v>
       </c>
-      <c r="AG32" s="19">
+      <c r="AG32" s="12">
         <v>1</v>
       </c>
       <c r="AH32">
         <v>1</v>
       </c>
-      <c r="AI32" s="19">
+      <c r="AI32" s="12">
         <v>1</v>
       </c>
       <c r="AJ32">
@@ -4503,7 +4510,7 @@
       </c>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="25" t="s">
         <v>59</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -4528,7 +4535,7 @@
       <c r="H33">
         <v>0</v>
       </c>
-      <c r="I33" s="19">
+      <c r="I33" s="12">
         <v>0</v>
       </c>
       <c r="J33">
@@ -4543,7 +4550,7 @@
       <c r="M33">
         <v>0</v>
       </c>
-      <c r="N33" s="19">
+      <c r="N33" s="12">
         <v>0</v>
       </c>
       <c r="O33">
@@ -4558,7 +4565,7 @@
       <c r="R33">
         <v>0</v>
       </c>
-      <c r="S33" s="19">
+      <c r="S33" s="12">
         <v>0</v>
       </c>
       <c r="T33">
@@ -4576,7 +4583,7 @@
       <c r="X33">
         <v>0</v>
       </c>
-      <c r="Y33" s="19">
+      <c r="Y33" s="12">
         <v>0</v>
       </c>
       <c r="Z33" s="1">
@@ -4588,25 +4595,25 @@
       <c r="AB33" s="1">
         <v>1</v>
       </c>
-      <c r="AC33" s="24">
+      <c r="AC33" s="17">
         <v>0</v>
       </c>
       <c r="AD33">
         <v>1</v>
       </c>
-      <c r="AE33" s="19">
+      <c r="AE33" s="12">
         <v>1</v>
       </c>
       <c r="AF33">
         <v>1</v>
       </c>
-      <c r="AG33" s="19">
+      <c r="AG33" s="12">
         <v>1</v>
       </c>
       <c r="AH33">
         <v>1</v>
       </c>
-      <c r="AI33" s="19">
+      <c r="AI33" s="12">
         <v>1</v>
       </c>
       <c r="AJ33">
@@ -4642,7 +4649,7 @@
       <c r="H34">
         <v>1</v>
       </c>
-      <c r="I34" s="19">
+      <c r="I34" s="12">
         <v>0</v>
       </c>
       <c r="J34">
@@ -4657,7 +4664,7 @@
       <c r="M34">
         <v>1</v>
       </c>
-      <c r="N34" s="19">
+      <c r="N34" s="12">
         <v>0</v>
       </c>
       <c r="O34">
@@ -4672,7 +4679,7 @@
       <c r="R34">
         <v>1</v>
       </c>
-      <c r="S34" s="19">
+      <c r="S34" s="12">
         <v>0</v>
       </c>
       <c r="T34">
@@ -4690,7 +4697,7 @@
       <c r="X34">
         <v>0</v>
       </c>
-      <c r="Y34" s="19">
+      <c r="Y34" s="12">
         <v>0</v>
       </c>
       <c r="Z34" s="1">
@@ -4702,25 +4709,25 @@
       <c r="AB34" s="1">
         <v>1</v>
       </c>
-      <c r="AC34" s="24">
+      <c r="AC34" s="17">
         <v>0</v>
       </c>
       <c r="AD34">
         <v>0</v>
       </c>
-      <c r="AE34" s="19">
+      <c r="AE34" s="12">
         <v>1</v>
       </c>
       <c r="AF34">
         <v>0</v>
       </c>
-      <c r="AG34" s="19">
+      <c r="AG34" s="12">
         <v>1</v>
       </c>
       <c r="AH34">
         <v>0</v>
       </c>
-      <c r="AI34" s="19">
+      <c r="AI34" s="12">
         <v>1</v>
       </c>
       <c r="AJ34">
@@ -4756,7 +4763,7 @@
       <c r="H35">
         <v>1</v>
       </c>
-      <c r="I35" s="19">
+      <c r="I35" s="12">
         <v>0</v>
       </c>
       <c r="J35">
@@ -4771,7 +4778,7 @@
       <c r="M35">
         <v>1</v>
       </c>
-      <c r="N35" s="19">
+      <c r="N35" s="12">
         <v>0</v>
       </c>
       <c r="O35">
@@ -4786,7 +4793,7 @@
       <c r="R35">
         <v>1</v>
       </c>
-      <c r="S35" s="19">
+      <c r="S35" s="12">
         <v>0</v>
       </c>
       <c r="T35">
@@ -4804,7 +4811,7 @@
       <c r="X35">
         <v>0</v>
       </c>
-      <c r="Y35" s="19">
+      <c r="Y35" s="12">
         <v>0</v>
       </c>
       <c r="Z35" s="1">
@@ -4816,25 +4823,25 @@
       <c r="AB35" s="1">
         <v>1</v>
       </c>
-      <c r="AC35" s="24">
+      <c r="AC35" s="17">
         <v>0</v>
       </c>
       <c r="AD35">
         <v>0</v>
       </c>
-      <c r="AE35" s="19">
+      <c r="AE35" s="12">
         <v>0</v>
       </c>
       <c r="AF35">
         <v>0</v>
       </c>
-      <c r="AG35" s="19">
+      <c r="AG35" s="12">
         <v>0</v>
       </c>
       <c r="AH35">
         <v>0</v>
       </c>
-      <c r="AI35" s="19">
+      <c r="AI35" s="12">
         <v>0</v>
       </c>
       <c r="AJ35">
@@ -4870,7 +4877,7 @@
       <c r="H36">
         <v>1</v>
       </c>
-      <c r="I36" s="19">
+      <c r="I36" s="12">
         <v>1</v>
       </c>
       <c r="J36">
@@ -4885,7 +4892,7 @@
       <c r="M36">
         <v>1</v>
       </c>
-      <c r="N36" s="19">
+      <c r="N36" s="12">
         <v>1</v>
       </c>
       <c r="O36">
@@ -4900,7 +4907,7 @@
       <c r="R36">
         <v>1</v>
       </c>
-      <c r="S36" s="19">
+      <c r="S36" s="12">
         <v>1</v>
       </c>
       <c r="T36">
@@ -4918,7 +4925,7 @@
       <c r="X36">
         <v>0</v>
       </c>
-      <c r="Y36" s="19">
+      <c r="Y36" s="12">
         <v>0</v>
       </c>
       <c r="Z36" s="1">
@@ -4930,25 +4937,25 @@
       <c r="AB36" s="1">
         <v>1</v>
       </c>
-      <c r="AC36" s="24">
+      <c r="AC36" s="17">
         <v>0</v>
       </c>
       <c r="AD36">
         <v>0</v>
       </c>
-      <c r="AE36" s="19">
+      <c r="AE36" s="12">
         <v>0</v>
       </c>
       <c r="AF36">
         <v>0</v>
       </c>
-      <c r="AG36" s="19">
+      <c r="AG36" s="12">
         <v>1</v>
       </c>
       <c r="AH36">
         <v>0</v>
       </c>
-      <c r="AI36" s="19">
+      <c r="AI36" s="12">
         <v>1</v>
       </c>
       <c r="AJ36">
@@ -4984,7 +4991,7 @@
       <c r="H37">
         <v>1</v>
       </c>
-      <c r="I37" s="19">
+      <c r="I37" s="12">
         <v>0</v>
       </c>
       <c r="J37">
@@ -4999,7 +5006,7 @@
       <c r="M37">
         <v>1</v>
       </c>
-      <c r="N37" s="19">
+      <c r="N37" s="12">
         <v>0</v>
       </c>
       <c r="O37">
@@ -5014,7 +5021,7 @@
       <c r="R37">
         <v>1</v>
       </c>
-      <c r="S37" s="19">
+      <c r="S37" s="12">
         <v>0</v>
       </c>
       <c r="T37">
@@ -5032,7 +5039,7 @@
       <c r="X37">
         <v>0</v>
       </c>
-      <c r="Y37" s="19">
+      <c r="Y37" s="12">
         <v>0</v>
       </c>
       <c r="Z37" s="1">
@@ -5044,25 +5051,25 @@
       <c r="AB37" s="1">
         <v>1</v>
       </c>
-      <c r="AC37" s="24">
+      <c r="AC37" s="17">
         <v>0</v>
       </c>
       <c r="AD37">
         <v>0</v>
       </c>
-      <c r="AE37" s="19">
+      <c r="AE37" s="12">
         <v>0</v>
       </c>
       <c r="AF37">
         <v>0</v>
       </c>
-      <c r="AG37" s="19">
+      <c r="AG37" s="12">
         <v>0</v>
       </c>
       <c r="AH37">
         <v>1</v>
       </c>
-      <c r="AI37" s="19">
+      <c r="AI37" s="12">
         <v>0</v>
       </c>
       <c r="AJ37">
@@ -5098,7 +5105,7 @@
       <c r="H38">
         <v>0</v>
       </c>
-      <c r="I38" s="19">
+      <c r="I38" s="12">
         <v>0</v>
       </c>
       <c r="J38">
@@ -5113,7 +5120,7 @@
       <c r="M38">
         <v>0</v>
       </c>
-      <c r="N38" s="19">
+      <c r="N38" s="12">
         <v>0</v>
       </c>
       <c r="O38">
@@ -5128,7 +5135,7 @@
       <c r="R38">
         <v>0</v>
       </c>
-      <c r="S38" s="19">
+      <c r="S38" s="12">
         <v>0</v>
       </c>
       <c r="T38">
@@ -5146,7 +5153,7 @@
       <c r="X38">
         <v>0</v>
       </c>
-      <c r="Y38" s="19">
+      <c r="Y38" s="12">
         <v>0</v>
       </c>
       <c r="Z38" s="1">
@@ -5158,25 +5165,25 @@
       <c r="AB38" s="1">
         <v>1</v>
       </c>
-      <c r="AC38" s="24">
+      <c r="AC38" s="17">
         <v>1</v>
       </c>
       <c r="AD38">
         <v>0</v>
       </c>
-      <c r="AE38" s="19">
+      <c r="AE38" s="12">
         <v>0</v>
       </c>
       <c r="AF38">
         <v>0</v>
       </c>
-      <c r="AG38" s="19">
+      <c r="AG38" s="12">
         <v>0</v>
       </c>
       <c r="AH38">
         <v>1</v>
       </c>
-      <c r="AI38" s="19">
+      <c r="AI38" s="12">
         <v>0</v>
       </c>
       <c r="AJ38">
@@ -5212,7 +5219,7 @@
       <c r="H39">
         <v>0</v>
       </c>
-      <c r="I39" s="19">
+      <c r="I39" s="12">
         <v>0</v>
       </c>
       <c r="J39">
@@ -5227,7 +5234,7 @@
       <c r="M39">
         <v>1</v>
       </c>
-      <c r="N39" s="19">
+      <c r="N39" s="12">
         <v>0</v>
       </c>
       <c r="O39">
@@ -5242,7 +5249,7 @@
       <c r="R39">
         <v>1</v>
       </c>
-      <c r="S39" s="19">
+      <c r="S39" s="12">
         <v>0</v>
       </c>
       <c r="T39">
@@ -5260,7 +5267,7 @@
       <c r="X39">
         <v>0</v>
       </c>
-      <c r="Y39" s="19">
+      <c r="Y39" s="12">
         <v>0</v>
       </c>
       <c r="Z39" s="1">
@@ -5272,25 +5279,25 @@
       <c r="AB39" s="1">
         <v>1</v>
       </c>
-      <c r="AC39" s="24">
+      <c r="AC39" s="17">
         <v>0</v>
       </c>
       <c r="AD39">
         <v>0</v>
       </c>
-      <c r="AE39" s="19">
+      <c r="AE39" s="12">
         <v>0</v>
       </c>
       <c r="AF39">
         <v>0</v>
       </c>
-      <c r="AG39" s="19">
+      <c r="AG39" s="12">
         <v>0</v>
       </c>
       <c r="AH39">
         <v>0</v>
       </c>
-      <c r="AI39" s="19">
+      <c r="AI39" s="12">
         <v>0</v>
       </c>
       <c r="AJ39">
@@ -5326,7 +5333,7 @@
       <c r="H40">
         <v>0</v>
       </c>
-      <c r="I40" s="19">
+      <c r="I40" s="12">
         <v>0</v>
       </c>
       <c r="J40">
@@ -5341,7 +5348,7 @@
       <c r="M40">
         <v>0</v>
       </c>
-      <c r="N40" s="19">
+      <c r="N40" s="12">
         <v>0</v>
       </c>
       <c r="O40">
@@ -5356,7 +5363,7 @@
       <c r="R40">
         <v>0</v>
       </c>
-      <c r="S40" s="19">
+      <c r="S40" s="12">
         <v>0</v>
       </c>
       <c r="T40">
@@ -5374,7 +5381,7 @@
       <c r="X40">
         <v>0</v>
       </c>
-      <c r="Y40" s="19">
+      <c r="Y40" s="12">
         <v>0</v>
       </c>
       <c r="Z40" s="1">
@@ -5386,25 +5393,25 @@
       <c r="AB40" s="1">
         <v>1</v>
       </c>
-      <c r="AC40" s="24">
+      <c r="AC40" s="17">
         <v>1</v>
       </c>
       <c r="AD40">
         <v>0</v>
       </c>
-      <c r="AE40" s="19">
+      <c r="AE40" s="12">
         <v>0</v>
       </c>
       <c r="AF40">
         <v>0</v>
       </c>
-      <c r="AG40" s="19">
+      <c r="AG40" s="12">
         <v>0</v>
       </c>
       <c r="AH40">
         <v>1</v>
       </c>
-      <c r="AI40" s="19">
+      <c r="AI40" s="12">
         <v>0</v>
       </c>
       <c r="AJ40">
@@ -5440,7 +5447,7 @@
       <c r="H41">
         <v>0</v>
       </c>
-      <c r="I41" s="19">
+      <c r="I41" s="12">
         <v>1</v>
       </c>
       <c r="J41">
@@ -5455,7 +5462,7 @@
       <c r="M41">
         <v>0</v>
       </c>
-      <c r="N41" s="19">
+      <c r="N41" s="12">
         <v>1</v>
       </c>
       <c r="O41">
@@ -5470,7 +5477,7 @@
       <c r="R41">
         <v>0</v>
       </c>
-      <c r="S41" s="19">
+      <c r="S41" s="12">
         <v>1</v>
       </c>
       <c r="T41">
@@ -5488,7 +5495,7 @@
       <c r="X41">
         <v>1</v>
       </c>
-      <c r="Y41" s="19">
+      <c r="Y41" s="12">
         <v>0</v>
       </c>
       <c r="Z41" s="1">
@@ -5500,25 +5507,25 @@
       <c r="AB41" s="1">
         <v>1</v>
       </c>
-      <c r="AC41" s="24">
+      <c r="AC41" s="17">
         <v>1</v>
       </c>
       <c r="AD41">
         <v>0</v>
       </c>
-      <c r="AE41" s="19">
+      <c r="AE41" s="12">
         <v>1</v>
       </c>
       <c r="AF41">
         <v>0</v>
       </c>
-      <c r="AG41" s="19">
+      <c r="AG41" s="12">
         <v>1</v>
       </c>
       <c r="AH41">
         <v>0</v>
       </c>
-      <c r="AI41" s="19">
+      <c r="AI41" s="12">
         <v>1</v>
       </c>
       <c r="AJ41">
@@ -5529,7 +5536,7 @@
       </c>
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="25" t="s">
         <v>77</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -5554,7 +5561,7 @@
       <c r="H42">
         <v>0</v>
       </c>
-      <c r="I42" s="19">
+      <c r="I42" s="12">
         <v>1</v>
       </c>
       <c r="J42">
@@ -5569,7 +5576,7 @@
       <c r="M42">
         <v>0</v>
       </c>
-      <c r="N42" s="19">
+      <c r="N42" s="12">
         <v>1</v>
       </c>
       <c r="O42">
@@ -5584,7 +5591,7 @@
       <c r="R42">
         <v>0</v>
       </c>
-      <c r="S42" s="19">
+      <c r="S42" s="12">
         <v>1</v>
       </c>
       <c r="T42">
@@ -5602,7 +5609,7 @@
       <c r="X42">
         <v>1</v>
       </c>
-      <c r="Y42" s="19">
+      <c r="Y42" s="12">
         <v>1</v>
       </c>
       <c r="Z42" s="1">
@@ -5614,25 +5621,25 @@
       <c r="AB42" s="1">
         <v>1</v>
       </c>
-      <c r="AC42" s="24">
+      <c r="AC42" s="17">
         <v>1</v>
       </c>
       <c r="AD42">
         <v>0</v>
       </c>
-      <c r="AE42" s="19">
+      <c r="AE42" s="12">
         <v>0</v>
       </c>
       <c r="AF42">
         <v>0</v>
       </c>
-      <c r="AG42" s="19">
+      <c r="AG42" s="12">
         <v>0</v>
       </c>
       <c r="AH42">
         <v>0</v>
       </c>
-      <c r="AI42" s="19">
+      <c r="AI42" s="12">
         <v>1</v>
       </c>
       <c r="AJ42">
@@ -5668,7 +5675,7 @@
       <c r="H43">
         <v>0</v>
       </c>
-      <c r="I43" s="19">
+      <c r="I43" s="12">
         <v>0</v>
       </c>
       <c r="J43">
@@ -5683,7 +5690,7 @@
       <c r="M43">
         <v>1</v>
       </c>
-      <c r="N43" s="19">
+      <c r="N43" s="12">
         <v>0</v>
       </c>
       <c r="O43">
@@ -5698,7 +5705,7 @@
       <c r="R43">
         <v>0</v>
       </c>
-      <c r="S43" s="19">
+      <c r="S43" s="12">
         <v>0</v>
       </c>
       <c r="T43">
@@ -5716,7 +5723,7 @@
       <c r="X43">
         <v>0</v>
       </c>
-      <c r="Y43" s="19">
+      <c r="Y43" s="12">
         <v>0</v>
       </c>
       <c r="Z43" s="1">
@@ -5728,25 +5735,25 @@
       <c r="AB43" s="1">
         <v>0</v>
       </c>
-      <c r="AC43" s="24">
+      <c r="AC43" s="17">
         <v>1</v>
       </c>
       <c r="AD43">
         <v>0</v>
       </c>
-      <c r="AE43" s="19">
+      <c r="AE43" s="12">
         <v>0</v>
       </c>
       <c r="AF43">
         <v>0</v>
       </c>
-      <c r="AG43" s="19">
+      <c r="AG43" s="12">
         <v>0</v>
       </c>
       <c r="AH43">
         <v>0</v>
       </c>
-      <c r="AI43" s="19">
+      <c r="AI43" s="12">
         <v>0</v>
       </c>
       <c r="AJ43">
@@ -5782,7 +5789,7 @@
       <c r="H44">
         <v>0</v>
       </c>
-      <c r="I44" s="19">
+      <c r="I44" s="12">
         <v>1</v>
       </c>
       <c r="J44">
@@ -5797,7 +5804,7 @@
       <c r="M44">
         <v>0</v>
       </c>
-      <c r="N44" s="19">
+      <c r="N44" s="12">
         <v>1</v>
       </c>
       <c r="O44">
@@ -5812,7 +5819,7 @@
       <c r="R44">
         <v>0</v>
       </c>
-      <c r="S44" s="19">
+      <c r="S44" s="12">
         <v>1</v>
       </c>
       <c r="T44">
@@ -5830,7 +5837,7 @@
       <c r="X44">
         <v>1</v>
       </c>
-      <c r="Y44" s="19">
+      <c r="Y44" s="12">
         <v>0</v>
       </c>
       <c r="Z44" s="1">
@@ -5842,25 +5849,25 @@
       <c r="AB44" s="1">
         <v>1</v>
       </c>
-      <c r="AC44" s="24">
+      <c r="AC44" s="17">
         <v>1</v>
       </c>
       <c r="AD44">
         <v>0</v>
       </c>
-      <c r="AE44" s="19">
+      <c r="AE44" s="12">
         <v>1</v>
       </c>
       <c r="AF44">
         <v>0</v>
       </c>
-      <c r="AG44" s="19">
+      <c r="AG44" s="12">
         <v>1</v>
       </c>
       <c r="AH44">
         <v>0</v>
       </c>
-      <c r="AI44" s="19">
+      <c r="AI44" s="12">
         <v>1</v>
       </c>
       <c r="AJ44">
@@ -5896,7 +5903,7 @@
       <c r="H45">
         <v>0</v>
       </c>
-      <c r="I45" s="19">
+      <c r="I45" s="12">
         <v>0</v>
       </c>
       <c r="J45">
@@ -5911,7 +5918,7 @@
       <c r="M45">
         <v>0</v>
       </c>
-      <c r="N45" s="19">
+      <c r="N45" s="12">
         <v>0</v>
       </c>
       <c r="O45">
@@ -5926,7 +5933,7 @@
       <c r="R45">
         <v>0</v>
       </c>
-      <c r="S45" s="19">
+      <c r="S45" s="12">
         <v>0</v>
       </c>
       <c r="T45">
@@ -5944,7 +5951,7 @@
       <c r="X45">
         <v>0</v>
       </c>
-      <c r="Y45" s="19">
+      <c r="Y45" s="12">
         <v>0</v>
       </c>
       <c r="Z45" s="1">
@@ -5956,25 +5963,25 @@
       <c r="AB45" s="1">
         <v>1</v>
       </c>
-      <c r="AC45" s="24">
+      <c r="AC45" s="17">
         <v>1</v>
       </c>
       <c r="AD45">
         <v>0</v>
       </c>
-      <c r="AE45" s="19">
+      <c r="AE45" s="12">
         <v>0</v>
       </c>
       <c r="AF45">
         <v>0</v>
       </c>
-      <c r="AG45" s="19">
+      <c r="AG45" s="12">
         <v>0</v>
       </c>
       <c r="AH45">
         <v>1</v>
       </c>
-      <c r="AI45" s="19">
+      <c r="AI45" s="12">
         <v>0</v>
       </c>
       <c r="AJ45">
@@ -5985,7 +5992,7 @@
       </c>
     </row>
     <row r="46" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="25" t="s">
         <v>85</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -6010,7 +6017,7 @@
       <c r="H46">
         <v>1</v>
       </c>
-      <c r="I46" s="19">
+      <c r="I46" s="12">
         <v>0</v>
       </c>
       <c r="J46">
@@ -6025,7 +6032,7 @@
       <c r="M46">
         <v>1</v>
       </c>
-      <c r="N46" s="19">
+      <c r="N46" s="12">
         <v>0</v>
       </c>
       <c r="O46">
@@ -6040,7 +6047,7 @@
       <c r="R46">
         <v>1</v>
       </c>
-      <c r="S46" s="19">
+      <c r="S46" s="12">
         <v>0</v>
       </c>
       <c r="T46">
@@ -6058,7 +6065,7 @@
       <c r="X46">
         <v>0</v>
       </c>
-      <c r="Y46" s="19">
+      <c r="Y46" s="12">
         <v>0</v>
       </c>
       <c r="Z46" s="1">
@@ -6070,25 +6077,25 @@
       <c r="AB46" s="1">
         <v>1</v>
       </c>
-      <c r="AC46" s="24">
+      <c r="AC46" s="17">
         <v>0</v>
       </c>
       <c r="AD46">
         <v>1</v>
       </c>
-      <c r="AE46" s="19">
+      <c r="AE46" s="12">
         <v>1</v>
       </c>
       <c r="AF46">
         <v>1</v>
       </c>
-      <c r="AG46" s="19">
+      <c r="AG46" s="12">
         <v>1</v>
       </c>
       <c r="AH46">
         <v>1</v>
       </c>
-      <c r="AI46" s="19">
+      <c r="AI46" s="12">
         <v>1</v>
       </c>
       <c r="AJ46">
@@ -6124,7 +6131,7 @@
       <c r="H47">
         <v>0</v>
       </c>
-      <c r="I47" s="19">
+      <c r="I47" s="12">
         <v>0</v>
       </c>
       <c r="J47">
@@ -6139,7 +6146,7 @@
       <c r="M47">
         <v>1</v>
       </c>
-      <c r="N47" s="19">
+      <c r="N47" s="12">
         <v>0</v>
       </c>
       <c r="O47">
@@ -6154,7 +6161,7 @@
       <c r="R47">
         <v>1</v>
       </c>
-      <c r="S47" s="19">
+      <c r="S47" s="12">
         <v>0</v>
       </c>
       <c r="T47">
@@ -6172,7 +6179,7 @@
       <c r="X47">
         <v>0</v>
       </c>
-      <c r="Y47" s="19">
+      <c r="Y47" s="12">
         <v>0</v>
       </c>
       <c r="Z47" s="1">
@@ -6184,25 +6191,25 @@
       <c r="AB47" s="1">
         <v>1</v>
       </c>
-      <c r="AC47" s="24">
+      <c r="AC47" s="17">
         <v>0</v>
       </c>
       <c r="AD47">
         <v>0</v>
       </c>
-      <c r="AE47" s="19">
+      <c r="AE47" s="12">
         <v>0</v>
       </c>
       <c r="AF47">
         <v>1</v>
       </c>
-      <c r="AG47" s="19">
+      <c r="AG47" s="12">
         <v>1</v>
       </c>
       <c r="AH47">
         <v>1</v>
       </c>
-      <c r="AI47" s="19">
+      <c r="AI47" s="12">
         <v>1</v>
       </c>
       <c r="AJ47">
@@ -6213,18 +6220,19 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A47" xr:uid="{C5F9261E-F944-A348-B7AA-D5D3D3EB9722}"/>
   <mergeCells count="11">
+    <mergeCell ref="E1:Y1"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="T2:Y2"/>
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="AD1:AK1"/>
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="E1:Y1"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:N2"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="T2:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>